<commit_message>
Finance File Updated 17/4/96
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
@@ -30,12 +30,12 @@
     <sheet name="اردیبهشت 96" sheetId="21" r:id="rId21"/>
     <sheet name="خرداد 96" sheetId="22" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="631">
   <si>
     <t>18/1/95</t>
   </si>
@@ -1925,6 +1925,9 @@
   </si>
   <si>
     <t>منابع نقدی</t>
+  </si>
+  <si>
+    <t>16/4/1396</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2278,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -26046,8 +26079,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26097,7 +26130,7 @@
       </c>
       <c r="D2" s="11">
         <f>D3+C2</f>
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="E2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -26105,7 +26138,7 @@
       </c>
       <c r="F2" s="11">
         <f>B2*(D2-E2)</f>
-        <v>34521900</v>
+        <v>35779000</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>1</v>
@@ -26123,7 +26156,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D66" si="0">D4+C3</f>
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E66" si="1">IF(B3&gt;0,1,0)</f>
@@ -26131,7 +26164,7 @@
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F66" si="2">B3*(D3-E3)</f>
-        <v>1065000000</v>
+        <v>1104000000</v>
       </c>
       <c r="G3" s="11"/>
     </row>
@@ -26147,7 +26180,7 @@
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" si="1"/>
@@ -26155,7 +26188,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" si="2"/>
-        <v>-70600000</v>
+        <v>-73200000</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -26171,7 +26204,7 @@
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="1"/>
@@ -26179,7 +26212,7 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="2"/>
-        <v>-35100000</v>
+        <v>-36400000</v>
       </c>
       <c r="G5" s="11"/>
     </row>
@@ -26195,7 +26228,7 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
@@ -26203,7 +26236,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="2"/>
-        <v>-19250000</v>
+        <v>-19965000</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -26219,7 +26252,7 @@
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
@@ -26227,7 +26260,7 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="2"/>
-        <v>-69800000</v>
+        <v>-72400000</v>
       </c>
       <c r="G7" s="11"/>
     </row>
@@ -26243,7 +26276,7 @@
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
@@ -26251,7 +26284,7 @@
       </c>
       <c r="F8" s="11">
         <f t="shared" si="2"/>
-        <v>-69000000</v>
+        <v>-71600000</v>
       </c>
       <c r="G8" s="11"/>
     </row>
@@ -26267,7 +26300,7 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
@@ -26275,7 +26308,7 @@
       </c>
       <c r="F9" s="11">
         <f t="shared" si="2"/>
-        <v>-319368000</v>
+        <v>-331724500</v>
       </c>
       <c r="G9" s="11"/>
     </row>
@@ -26291,7 +26324,7 @@
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
@@ -26299,7 +26332,7 @@
       </c>
       <c r="F10" s="11">
         <f t="shared" si="2"/>
-        <v>668000000</v>
+        <v>694000000</v>
       </c>
       <c r="G10" s="11"/>
     </row>
@@ -26315,7 +26348,7 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
@@ -26323,7 +26356,7 @@
       </c>
       <c r="F11" s="11">
         <f t="shared" si="2"/>
-        <v>-354645000</v>
+        <v>-368490000</v>
       </c>
       <c r="G11" s="11"/>
     </row>
@@ -26339,7 +26372,7 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
@@ -26347,7 +26380,7 @@
       </c>
       <c r="F12" s="11">
         <f t="shared" si="2"/>
-        <v>-14850000</v>
+        <v>-15435000</v>
       </c>
       <c r="G12" s="11"/>
     </row>
@@ -26363,7 +26396,7 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
@@ -26371,7 +26404,7 @@
       </c>
       <c r="F13" s="11">
         <f t="shared" si="2"/>
-        <v>-658230300</v>
+        <v>-684239400</v>
       </c>
       <c r="G13" s="11"/>
     </row>
@@ -26387,7 +26420,7 @@
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
@@ -26395,7 +26428,7 @@
       </c>
       <c r="F14" s="11">
         <f t="shared" si="2"/>
-        <v>-65000000</v>
+        <v>-67600000</v>
       </c>
       <c r="G14" s="11"/>
     </row>
@@ -26411,7 +26444,7 @@
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="1"/>
@@ -26419,7 +26452,7 @@
       </c>
       <c r="F15" s="11">
         <f t="shared" si="2"/>
-        <v>644000000</v>
+        <v>670000000</v>
       </c>
       <c r="G15" s="11"/>
     </row>
@@ -26435,7 +26468,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
@@ -26443,7 +26476,7 @@
       </c>
       <c r="F16" s="11">
         <f t="shared" si="2"/>
-        <v>644000000</v>
+        <v>670000000</v>
       </c>
       <c r="G16" s="11"/>
     </row>
@@ -26459,7 +26492,7 @@
       </c>
       <c r="D17" s="11">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="1"/>
@@ -26467,7 +26500,7 @@
       </c>
       <c r="F17" s="11">
         <f t="shared" si="2"/>
-        <v>386400000</v>
+        <v>402000000</v>
       </c>
       <c r="G17" s="11"/>
     </row>
@@ -26483,7 +26516,7 @@
       </c>
       <c r="D18" s="11">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
@@ -26491,7 +26524,7 @@
       </c>
       <c r="F18" s="11">
         <f t="shared" si="2"/>
-        <v>322000000</v>
+        <v>335000000</v>
       </c>
       <c r="G18" s="11"/>
     </row>
@@ -26507,7 +26540,7 @@
       </c>
       <c r="D19" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="1"/>
@@ -26515,7 +26548,7 @@
       </c>
       <c r="F19" s="11">
         <f t="shared" si="2"/>
-        <v>963000000</v>
+        <v>1002000000</v>
       </c>
       <c r="G19" s="11"/>
       <c r="L19" t="s">
@@ -26534,7 +26567,7 @@
       </c>
       <c r="D20" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="1"/>
@@ -26542,7 +26575,7 @@
       </c>
       <c r="F20" s="11">
         <f t="shared" si="2"/>
-        <v>-139329400</v>
+        <v>-144954500</v>
       </c>
       <c r="G20" s="11"/>
     </row>
@@ -26558,7 +26591,7 @@
       </c>
       <c r="D21" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="1"/>
@@ -26566,7 +26599,7 @@
       </c>
       <c r="F21" s="11">
         <f t="shared" si="2"/>
-        <v>-139329400</v>
+        <v>-144954500</v>
       </c>
       <c r="G21" s="11"/>
     </row>
@@ -26582,7 +26615,7 @@
       </c>
       <c r="D22" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="1"/>
@@ -26590,7 +26623,7 @@
       </c>
       <c r="F22" s="11">
         <f t="shared" si="2"/>
-        <v>-139329400</v>
+        <v>-144954500</v>
       </c>
       <c r="G22" s="11"/>
     </row>
@@ -26606,7 +26639,7 @@
       </c>
       <c r="D23" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="1"/>
@@ -26614,7 +26647,7 @@
       </c>
       <c r="F23" s="11">
         <f t="shared" si="2"/>
-        <v>-139329400</v>
+        <v>-144954500</v>
       </c>
       <c r="G23" s="11"/>
     </row>
@@ -26630,7 +26663,7 @@
       </c>
       <c r="D24" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="1"/>
@@ -26638,7 +26671,7 @@
       </c>
       <c r="F24" s="11">
         <f t="shared" si="2"/>
-        <v>-139329400</v>
+        <v>-144954500</v>
       </c>
       <c r="G24" s="11"/>
     </row>
@@ -26654,7 +26687,7 @@
       </c>
       <c r="D25" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="1"/>
@@ -26662,7 +26695,7 @@
       </c>
       <c r="F25" s="11">
         <f t="shared" si="2"/>
-        <v>-64400000</v>
+        <v>-67000000</v>
       </c>
       <c r="G25" s="11"/>
     </row>
@@ -26678,7 +26711,7 @@
       </c>
       <c r="D26" s="11">
         <f t="shared" si="0"/>
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="1"/>
@@ -26686,7 +26719,7 @@
       </c>
       <c r="F26" s="11">
         <f t="shared" si="2"/>
-        <v>960000000</v>
+        <v>999000000</v>
       </c>
       <c r="G26" s="11"/>
     </row>
@@ -26702,7 +26735,7 @@
       </c>
       <c r="D27" s="11">
         <f t="shared" si="0"/>
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="1"/>
@@ -26710,7 +26743,7 @@
       </c>
       <c r="F27" s="11">
         <f t="shared" si="2"/>
-        <v>-63800000</v>
+        <v>-66400000</v>
       </c>
       <c r="G27" s="11"/>
     </row>
@@ -26726,7 +26759,7 @@
       </c>
       <c r="D28" s="11">
         <f t="shared" si="0"/>
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="E28" s="11">
         <f t="shared" si="1"/>
@@ -26734,7 +26767,7 @@
       </c>
       <c r="F28" s="11">
         <f t="shared" si="2"/>
-        <v>634000000</v>
+        <v>660000000</v>
       </c>
       <c r="G28" s="11"/>
     </row>
@@ -26750,7 +26783,7 @@
       </c>
       <c r="D29" s="11">
         <f t="shared" si="0"/>
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="E29" s="11">
         <f t="shared" si="1"/>
@@ -26758,7 +26791,7 @@
       </c>
       <c r="F29" s="11">
         <f t="shared" si="2"/>
-        <v>-2219253600</v>
+        <v>-2310264000</v>
       </c>
       <c r="G29" s="11"/>
     </row>
@@ -26774,7 +26807,7 @@
       </c>
       <c r="D30" s="11">
         <f t="shared" si="0"/>
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" si="1"/>
@@ -26782,7 +26815,7 @@
       </c>
       <c r="F30" s="11">
         <f t="shared" si="2"/>
-        <v>-948284400</v>
+        <v>-987296100</v>
       </c>
       <c r="G30" s="11"/>
     </row>
@@ -26798,7 +26831,7 @@
       </c>
       <c r="D31" s="11">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="1"/>
@@ -26806,7 +26839,7 @@
       </c>
       <c r="F31" s="11">
         <f t="shared" si="2"/>
-        <v>-534208500</v>
+        <v>-556255200</v>
       </c>
       <c r="G31" s="11"/>
     </row>
@@ -26822,7 +26855,7 @@
       </c>
       <c r="D32" s="11">
         <f t="shared" si="0"/>
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="1"/>
@@ -26830,7 +26863,7 @@
       </c>
       <c r="F32" s="11">
         <f t="shared" si="2"/>
-        <v>309227300</v>
+        <v>322153200</v>
       </c>
       <c r="G32" s="11"/>
     </row>
@@ -26846,7 +26879,7 @@
       </c>
       <c r="D33" s="11">
         <f t="shared" si="0"/>
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="1"/>
@@ -26854,7 +26887,7 @@
       </c>
       <c r="F33" s="11">
         <f t="shared" si="2"/>
-        <v>10737846</v>
+        <v>11194029</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>383</v>
@@ -26872,7 +26905,7 @@
       </c>
       <c r="D34" s="11">
         <f t="shared" si="0"/>
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="E34" s="11">
         <f t="shared" si="1"/>
@@ -26880,7 +26913,7 @@
       </c>
       <c r="F34" s="11">
         <f t="shared" si="2"/>
-        <v>-260100000</v>
+        <v>-271150000</v>
       </c>
       <c r="G34" s="11"/>
     </row>
@@ -26896,7 +26929,7 @@
       </c>
       <c r="D35" s="11">
         <f t="shared" si="0"/>
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="1"/>
@@ -26904,7 +26937,7 @@
       </c>
       <c r="F35" s="11">
         <f t="shared" si="2"/>
-        <v>-56769000</v>
+        <v>-59245500</v>
       </c>
       <c r="G35" s="11"/>
     </row>
@@ -26920,7 +26953,7 @@
       </c>
       <c r="D36" s="11">
         <f t="shared" si="0"/>
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E36" s="11">
         <f t="shared" si="1"/>
@@ -26928,7 +26961,7 @@
       </c>
       <c r="F36" s="11">
         <f t="shared" si="2"/>
-        <v>59200000</v>
+        <v>61800000</v>
       </c>
       <c r="G36" s="11"/>
     </row>
@@ -26944,7 +26977,7 @@
       </c>
       <c r="D37" s="11">
         <f t="shared" si="0"/>
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E37" s="11">
         <f t="shared" si="1"/>
@@ -26952,7 +26985,7 @@
       </c>
       <c r="F37" s="11">
         <f t="shared" si="2"/>
-        <v>-59400000</v>
+        <v>-62000000</v>
       </c>
       <c r="G37" s="11"/>
     </row>
@@ -26968,7 +27001,7 @@
       </c>
       <c r="D38" s="11">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="E38" s="11">
         <f t="shared" si="1"/>
@@ -26976,7 +27009,7 @@
       </c>
       <c r="F38" s="11">
         <f t="shared" si="2"/>
-        <v>82420844</v>
+        <v>86331322</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>403</v>
@@ -26994,7 +27027,7 @@
       </c>
       <c r="D39" s="11">
         <f t="shared" si="0"/>
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="E39" s="11">
         <f t="shared" si="1"/>
@@ -27002,7 +27035,7 @@
       </c>
       <c r="F39" s="11">
         <f t="shared" si="2"/>
-        <v>-26030000</v>
+        <v>-27265000</v>
       </c>
       <c r="G39" s="11"/>
     </row>
@@ -27018,7 +27051,7 @@
       </c>
       <c r="D40" s="11">
         <f t="shared" si="0"/>
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="1"/>
@@ -27026,7 +27059,7 @@
       </c>
       <c r="F40" s="11">
         <f t="shared" si="2"/>
-        <v>-24140222</v>
+        <v>-25285561</v>
       </c>
       <c r="G40" s="11"/>
     </row>
@@ -27042,7 +27075,7 @@
       </c>
       <c r="D41" s="11">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" si="1"/>
@@ -27050,7 +27083,7 @@
       </c>
       <c r="F41" s="11">
         <f t="shared" si="2"/>
-        <v>-32280000</v>
+        <v>-33840000</v>
       </c>
       <c r="G41" s="11"/>
     </row>
@@ -27066,7 +27099,7 @@
       </c>
       <c r="D42" s="11">
         <f t="shared" si="0"/>
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="E42" s="11">
         <f t="shared" si="1"/>
@@ -27074,7 +27107,7 @@
       </c>
       <c r="F42" s="11">
         <f t="shared" si="2"/>
-        <v>246050184</v>
+        <v>259052836</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>404</v>
@@ -27092,7 +27125,7 @@
       </c>
       <c r="D43" s="11">
         <f t="shared" si="0"/>
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="1"/>
@@ -27100,7 +27133,7 @@
       </c>
       <c r="F43" s="11">
         <f t="shared" si="2"/>
-        <v>-19440000</v>
+        <v>-20480000</v>
       </c>
       <c r="G43" s="11"/>
     </row>
@@ -27116,7 +27149,7 @@
       </c>
       <c r="D44" s="11">
         <f t="shared" si="0"/>
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="1"/>
@@ -27124,7 +27157,7 @@
       </c>
       <c r="F44" s="11">
         <f t="shared" si="2"/>
-        <v>-50435931</v>
+        <v>-53179308</v>
       </c>
       <c r="G44" s="11"/>
     </row>
@@ -27140,7 +27173,7 @@
       </c>
       <c r="D45" s="11">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="1"/>
@@ -27148,7 +27181,7 @@
       </c>
       <c r="F45" s="11">
         <f t="shared" si="2"/>
-        <v>-47600000</v>
+        <v>-50200000</v>
       </c>
       <c r="G45" s="11"/>
     </row>
@@ -27164,7 +27197,7 @@
       </c>
       <c r="D46" s="11">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="1"/>
@@ -27172,7 +27205,7 @@
       </c>
       <c r="F46" s="11">
         <f t="shared" si="2"/>
-        <v>-22515000</v>
+        <v>-23750000</v>
       </c>
       <c r="G46" s="11"/>
     </row>
@@ -27188,7 +27221,7 @@
       </c>
       <c r="D47" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="1"/>
@@ -27196,7 +27229,7 @@
       </c>
       <c r="F47" s="11">
         <f t="shared" si="2"/>
-        <v>-10575000</v>
+        <v>-11160000</v>
       </c>
       <c r="G47" s="11"/>
     </row>
@@ -27212,7 +27245,7 @@
       </c>
       <c r="D48" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="1"/>
@@ -27220,7 +27253,7 @@
       </c>
       <c r="F48" s="11">
         <f t="shared" si="2"/>
-        <v>-15082300</v>
+        <v>-15916640</v>
       </c>
       <c r="G48" s="11"/>
     </row>
@@ -27236,7 +27269,7 @@
       </c>
       <c r="D49" s="11">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="E49" s="11">
         <f t="shared" si="1"/>
@@ -27244,7 +27277,7 @@
       </c>
       <c r="F49" s="11">
         <f t="shared" si="2"/>
-        <v>-6376288</v>
+        <v>-6733580</v>
       </c>
       <c r="G49" s="11"/>
     </row>
@@ -27260,7 +27293,7 @@
       </c>
       <c r="D50" s="11">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="E50" s="11">
         <f t="shared" si="1"/>
@@ -27268,7 +27301,7 @@
       </c>
       <c r="F50" s="11">
         <f t="shared" si="2"/>
-        <v>-32571000</v>
+        <v>-34404000</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -27284,7 +27317,7 @@
       </c>
       <c r="D51" s="11">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="E51" s="11">
         <f t="shared" si="1"/>
@@ -27292,7 +27325,7 @@
       </c>
       <c r="F51" s="11">
         <f t="shared" si="2"/>
-        <v>-6178326</v>
+        <v>-6526024</v>
       </c>
       <c r="G51" s="11"/>
     </row>
@@ -27308,7 +27341,7 @@
       </c>
       <c r="D52" s="11">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="E52" s="11">
         <f t="shared" si="1"/>
@@ -27316,7 +27349,7 @@
       </c>
       <c r="F52" s="11">
         <f t="shared" si="2"/>
-        <v>-12259000</v>
+        <v>-12951900</v>
       </c>
       <c r="G52" s="11"/>
     </row>
@@ -27332,7 +27365,7 @@
       </c>
       <c r="D53" s="11">
         <f t="shared" si="0"/>
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="E53" s="11">
         <f t="shared" si="1"/>
@@ -27340,7 +27373,7 @@
       </c>
       <c r="F53" s="11">
         <f t="shared" si="2"/>
-        <v>228000000</v>
+        <v>241000000</v>
       </c>
       <c r="G53" s="11"/>
     </row>
@@ -27356,7 +27389,7 @@
       </c>
       <c r="D54" s="11">
         <f t="shared" si="0"/>
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="E54" s="11">
         <f t="shared" si="1"/>
@@ -27364,7 +27397,7 @@
       </c>
       <c r="F54" s="11">
         <f t="shared" si="2"/>
-        <v>-4683000</v>
+        <v>-4956000</v>
       </c>
       <c r="G54" s="11"/>
     </row>
@@ -27380,7 +27413,7 @@
       </c>
       <c r="D55" s="11">
         <f t="shared" si="0"/>
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E55" s="11">
         <f t="shared" si="1"/>
@@ -27388,7 +27421,7 @@
       </c>
       <c r="F55" s="11">
         <f t="shared" si="2"/>
-        <v>-217671000</v>
+        <v>-230417500</v>
       </c>
       <c r="G55" s="11"/>
     </row>
@@ -27404,7 +27437,7 @@
       </c>
       <c r="D56" s="11">
         <f t="shared" si="0"/>
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="1"/>
@@ -27412,7 +27445,7 @@
       </c>
       <c r="F56" s="11">
         <f t="shared" si="2"/>
-        <v>-9990000</v>
+        <v>-10575000</v>
       </c>
       <c r="G56" s="11"/>
     </row>
@@ -27428,7 +27461,7 @@
       </c>
       <c r="D57" s="11">
         <f t="shared" si="0"/>
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="E57" s="11">
         <f t="shared" si="1"/>
@@ -27436,7 +27469,7 @@
       </c>
       <c r="F57" s="11">
         <f t="shared" si="2"/>
-        <v>625079312</v>
+        <v>664146769</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>405</v>
@@ -27454,7 +27487,7 @@
       </c>
       <c r="D58" s="11">
         <f t="shared" si="0"/>
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="E58" s="11">
         <f t="shared" si="1"/>
@@ -27462,7 +27495,7 @@
       </c>
       <c r="F58" s="11">
         <f t="shared" si="2"/>
-        <v>416000000</v>
+        <v>442000000</v>
       </c>
       <c r="G58" s="11"/>
     </row>
@@ -27478,7 +27511,7 @@
       </c>
       <c r="D59" s="11">
         <f t="shared" si="0"/>
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="E59" s="11">
         <f t="shared" si="1"/>
@@ -27486,7 +27519,7 @@
       </c>
       <c r="F59" s="11">
         <f t="shared" si="2"/>
-        <v>414000000</v>
+        <v>440000000</v>
       </c>
       <c r="G59" s="11"/>
     </row>
@@ -27502,7 +27535,7 @@
       </c>
       <c r="D60" s="11">
         <f t="shared" si="0"/>
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="E60" s="11">
         <f t="shared" si="1"/>
@@ -27510,7 +27543,7 @@
       </c>
       <c r="F60" s="11">
         <f t="shared" si="2"/>
-        <v>-1456312000</v>
+        <v>-1547331500</v>
       </c>
       <c r="G60" s="11"/>
     </row>
@@ -27526,7 +27559,7 @@
       </c>
       <c r="D61" s="11">
         <f t="shared" si="0"/>
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="E61" s="11">
         <f t="shared" si="1"/>
@@ -27534,7 +27567,7 @@
       </c>
       <c r="F61" s="11">
         <f t="shared" si="2"/>
-        <v>549000000</v>
+        <v>588000000</v>
       </c>
       <c r="G61" s="11"/>
     </row>
@@ -27550,7 +27583,7 @@
       </c>
       <c r="D62" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E62" s="11">
         <f t="shared" si="1"/>
@@ -27558,7 +27591,7 @@
       </c>
       <c r="F62" s="11">
         <f t="shared" si="2"/>
-        <v>-4960947</v>
+        <v>-5313364</v>
       </c>
       <c r="G62" s="11"/>
     </row>
@@ -27574,7 +27607,7 @@
       </c>
       <c r="D63" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E63" s="11">
         <f t="shared" si="1"/>
@@ -27582,7 +27615,7 @@
       </c>
       <c r="F63" s="11">
         <f t="shared" si="2"/>
-        <v>-6036987</v>
+        <v>-6465844</v>
       </c>
       <c r="G63" s="11"/>
     </row>
@@ -27598,7 +27631,7 @@
       </c>
       <c r="D64" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E64" s="11">
         <f t="shared" si="1"/>
@@ -27606,7 +27639,7 @@
       </c>
       <c r="F64" s="11">
         <f t="shared" si="2"/>
-        <v>546000000</v>
+        <v>585000000</v>
       </c>
       <c r="G64" s="11"/>
     </row>
@@ -27622,7 +27655,7 @@
       </c>
       <c r="D65" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E65" s="11">
         <f t="shared" si="1"/>
@@ -27630,7 +27663,7 @@
       </c>
       <c r="F65" s="11">
         <f t="shared" si="2"/>
-        <v>540540000</v>
+        <v>579150000</v>
       </c>
       <c r="G65" s="11"/>
     </row>
@@ -27646,7 +27679,7 @@
       </c>
       <c r="D66" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E66" s="11">
         <f t="shared" si="1"/>
@@ -27654,7 +27687,7 @@
       </c>
       <c r="F66" s="11">
         <f t="shared" si="2"/>
-        <v>182000000</v>
+        <v>195000000</v>
       </c>
       <c r="G66" s="11"/>
     </row>
@@ -27670,7 +27703,7 @@
       </c>
       <c r="D67" s="11">
         <f t="shared" ref="D67:D130" si="3">D68+C67</f>
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E67" s="11">
         <f t="shared" ref="E67:E130" si="4">IF(B67&gt;0,1,0)</f>
@@ -27678,7 +27711,7 @@
       </c>
       <c r="F67" s="11">
         <f t="shared" ref="F67:F137" si="5">B67*(D67-E67)</f>
-        <v>5460000</v>
+        <v>5850000</v>
       </c>
       <c r="G67" s="11"/>
     </row>
@@ -27694,7 +27727,7 @@
       </c>
       <c r="D68" s="11">
         <f t="shared" si="3"/>
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="E68" s="11">
         <f t="shared" si="4"/>
@@ -27702,7 +27735,7 @@
       </c>
       <c r="F68" s="11">
         <f t="shared" si="5"/>
-        <v>5430000000</v>
+        <v>5820000000</v>
       </c>
       <c r="G68" s="11"/>
     </row>
@@ -27718,7 +27751,7 @@
       </c>
       <c r="D69" s="11">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E69" s="11">
         <f t="shared" si="4"/>
@@ -27726,7 +27759,7 @@
       </c>
       <c r="F69" s="11">
         <f t="shared" si="5"/>
-        <v>-36200000</v>
+        <v>-38800000</v>
       </c>
       <c r="G69" s="11"/>
     </row>
@@ -27742,7 +27775,7 @@
       </c>
       <c r="D70" s="11">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E70" s="11">
         <f t="shared" si="4"/>
@@ -27750,7 +27783,7 @@
       </c>
       <c r="F70" s="11">
         <f t="shared" si="5"/>
-        <v>252000000</v>
+        <v>270200000</v>
       </c>
       <c r="G70" s="11"/>
     </row>
@@ -27766,7 +27799,7 @@
       </c>
       <c r="D71" s="11">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E71" s="11">
         <f t="shared" si="4"/>
@@ -27774,7 +27807,7 @@
       </c>
       <c r="F71" s="11">
         <f t="shared" si="5"/>
-        <v>468000000</v>
+        <v>501800000</v>
       </c>
       <c r="G71" s="11"/>
     </row>
@@ -27790,7 +27823,7 @@
       </c>
       <c r="D72" s="11">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E72" s="11">
         <f t="shared" si="4"/>
@@ -27798,7 +27831,7 @@
       </c>
       <c r="F72" s="11">
         <f t="shared" si="5"/>
-        <v>-181000000</v>
+        <v>-194000000</v>
       </c>
       <c r="G72" s="11"/>
     </row>
@@ -27814,7 +27847,7 @@
       </c>
       <c r="D73" s="11">
         <f t="shared" si="3"/>
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="E73" s="11">
         <f t="shared" si="4"/>
@@ -27822,7 +27855,7 @@
       </c>
       <c r="F73" s="11">
         <f t="shared" si="5"/>
-        <v>2670000000</v>
+        <v>2865000000</v>
       </c>
       <c r="G73" s="11"/>
     </row>
@@ -27838,7 +27871,7 @@
       </c>
       <c r="D74" s="11">
         <f t="shared" si="3"/>
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="E74" s="11">
         <f t="shared" si="4"/>
@@ -27846,7 +27879,7 @@
       </c>
       <c r="F74" s="11">
         <f t="shared" si="5"/>
-        <v>-2610730800</v>
+        <v>-2805785400</v>
       </c>
       <c r="G74" s="11"/>
     </row>
@@ -27862,7 +27895,7 @@
       </c>
       <c r="D75" s="11">
         <f t="shared" si="3"/>
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="E75" s="11">
         <f t="shared" si="4"/>
@@ -27870,7 +27903,7 @@
       </c>
       <c r="F75" s="11">
         <f t="shared" si="5"/>
-        <v>-516000000</v>
+        <v>-555000000</v>
       </c>
       <c r="G75" s="11"/>
     </row>
@@ -27886,7 +27919,7 @@
       </c>
       <c r="D76" s="11">
         <f t="shared" si="3"/>
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="E76" s="11">
         <f t="shared" si="4"/>
@@ -27894,7 +27927,7 @@
       </c>
       <c r="F76" s="11">
         <f t="shared" si="5"/>
-        <v>-34400000</v>
+        <v>-37000000</v>
       </c>
       <c r="G76" s="11"/>
     </row>
@@ -27910,7 +27943,7 @@
       </c>
       <c r="D77" s="11">
         <f t="shared" si="3"/>
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="E77" s="11">
         <f t="shared" si="4"/>
@@ -27918,7 +27951,7 @@
       </c>
       <c r="F77" s="11">
         <f t="shared" si="5"/>
-        <v>-2064516000</v>
+        <v>-2220555000</v>
       </c>
       <c r="G77" s="11"/>
     </row>
@@ -27934,7 +27967,7 @@
       </c>
       <c r="D78" s="11">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E78" s="11">
         <f t="shared" si="4"/>
@@ -27942,7 +27975,7 @@
       </c>
       <c r="F78" s="11">
         <f t="shared" si="5"/>
-        <v>-504151200</v>
+        <v>-543162900</v>
       </c>
       <c r="G78" s="11"/>
     </row>
@@ -27958,7 +27991,7 @@
       </c>
       <c r="D79" s="11">
         <f t="shared" si="3"/>
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="E79" s="11">
         <f t="shared" si="4"/>
@@ -27966,7 +27999,7 @@
       </c>
       <c r="F79" s="11">
         <f t="shared" si="5"/>
-        <v>3726000000</v>
+        <v>4025000000</v>
       </c>
       <c r="G79" s="11"/>
     </row>
@@ -27982,7 +28015,7 @@
       </c>
       <c r="D80" s="11">
         <f t="shared" si="3"/>
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="E80" s="11">
         <f t="shared" si="4"/>
@@ -27990,7 +28023,7 @@
       </c>
       <c r="F80" s="11">
         <f t="shared" si="5"/>
-        <v>-94879000</v>
+        <v>-102685500</v>
       </c>
       <c r="G80" s="11"/>
     </row>
@@ -28006,7 +28039,7 @@
       </c>
       <c r="D81" s="11">
         <f t="shared" si="3"/>
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="E81" s="11">
         <f t="shared" si="4"/>
@@ -28014,7 +28047,7 @@
       </c>
       <c r="F81" s="11">
         <f t="shared" si="5"/>
-        <v>-31600000</v>
+        <v>-34200000</v>
       </c>
       <c r="G81" s="11"/>
     </row>
@@ -28030,7 +28063,7 @@
       </c>
       <c r="D82" s="11">
         <f t="shared" si="3"/>
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="E82" s="11">
         <f t="shared" si="4"/>
@@ -28038,7 +28071,7 @@
       </c>
       <c r="F82" s="11">
         <f t="shared" si="5"/>
-        <v>44182476</v>
+        <v>47864349</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>242</v>
@@ -28056,7 +28089,7 @@
       </c>
       <c r="D83" s="11">
         <f t="shared" si="3"/>
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="E83" s="11">
         <f t="shared" si="4"/>
@@ -28064,7 +28097,7 @@
       </c>
       <c r="F83" s="11">
         <f t="shared" si="5"/>
-        <v>-31400000</v>
+        <v>-34000000</v>
       </c>
       <c r="G83" s="11"/>
     </row>
@@ -28080,7 +28113,7 @@
       </c>
       <c r="D84" s="11">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="E84" s="11">
         <f t="shared" si="4"/>
@@ -28088,7 +28121,7 @@
       </c>
       <c r="F84" s="11">
         <f t="shared" si="5"/>
-        <v>308000000</v>
+        <v>334000000</v>
       </c>
       <c r="G84" s="11"/>
     </row>
@@ -28104,7 +28137,7 @@
       </c>
       <c r="D85" s="11">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="E85" s="11">
         <f t="shared" si="4"/>
@@ -28112,7 +28145,7 @@
       </c>
       <c r="F85" s="11">
         <f t="shared" si="5"/>
-        <v>-30400000</v>
+        <v>-33000000</v>
       </c>
       <c r="G85" s="11"/>
     </row>
@@ -28128,7 +28161,7 @@
       </c>
       <c r="D86" s="11">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E86" s="11">
         <f t="shared" si="4"/>
@@ -28136,7 +28169,7 @@
       </c>
       <c r="F86" s="11">
         <f t="shared" si="5"/>
-        <v>-29200000</v>
+        <v>-31800000</v>
       </c>
       <c r="G86" s="11"/>
     </row>
@@ -28152,7 +28185,7 @@
       </c>
       <c r="D87" s="11">
         <f t="shared" si="3"/>
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E87" s="11">
         <f t="shared" si="4"/>
@@ -28160,7 +28193,7 @@
       </c>
       <c r="F87" s="11">
         <f t="shared" si="5"/>
-        <v>-190800000</v>
+        <v>-208025000</v>
       </c>
       <c r="G87" s="11"/>
     </row>
@@ -28176,7 +28209,7 @@
       </c>
       <c r="D88" s="11">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E88" s="11">
         <f t="shared" si="4"/>
@@ -28184,7 +28217,7 @@
       </c>
       <c r="F88" s="11">
         <f t="shared" si="5"/>
-        <v>-64500000</v>
+        <v>-71000000</v>
       </c>
       <c r="G88" s="11"/>
     </row>
@@ -28200,7 +28233,7 @@
       </c>
       <c r="D89" s="11">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E89" s="11">
         <f t="shared" si="4"/>
@@ -28208,7 +28241,7 @@
       </c>
       <c r="F89" s="11">
         <f t="shared" si="5"/>
-        <v>-15480000</v>
+        <v>-17040000</v>
       </c>
       <c r="G89" s="11"/>
     </row>
@@ -28224,7 +28257,7 @@
       </c>
       <c r="D90" s="11">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="E90" s="11">
         <f t="shared" si="4"/>
@@ -28232,7 +28265,7 @@
       </c>
       <c r="F90" s="11">
         <f t="shared" si="5"/>
-        <v>53953830</v>
+        <v>59520495</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>264</v>
@@ -28250,7 +28283,7 @@
       </c>
       <c r="D91" s="11">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E91" s="11">
         <f t="shared" si="4"/>
@@ -28258,7 +28291,7 @@
       </c>
       <c r="F91" s="11">
         <f t="shared" si="5"/>
-        <v>-372248000</v>
+        <v>-411274000</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>345</v>
@@ -28276,7 +28309,7 @@
       </c>
       <c r="D92" s="11">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E92" s="11">
         <f t="shared" si="4"/>
@@ -28284,7 +28317,7 @@
       </c>
       <c r="F92" s="11">
         <f t="shared" si="5"/>
-        <v>-25010000</v>
+        <v>-27675000</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>346</v>
@@ -28302,7 +28335,7 @@
       </c>
       <c r="D93" s="11">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E93" s="11">
         <f t="shared" si="4"/>
@@ -28310,7 +28343,7 @@
       </c>
       <c r="F93" s="11">
         <f t="shared" si="5"/>
-        <v>-42761000</v>
+        <v>-47317500</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>343</v>
@@ -28328,7 +28361,7 @@
       </c>
       <c r="D94" s="11">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="E94" s="11">
         <f t="shared" si="4"/>
@@ -28336,7 +28369,7 @@
       </c>
       <c r="F94" s="11">
         <f t="shared" si="5"/>
-        <v>110000000</v>
+        <v>123000000</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>341</v>
@@ -28354,7 +28387,7 @@
       </c>
       <c r="D95" s="11">
         <f t="shared" si="3"/>
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="E95" s="11">
         <f t="shared" si="4"/>
@@ -28362,7 +28395,7 @@
       </c>
       <c r="F95" s="11">
         <f t="shared" si="5"/>
-        <v>945000000</v>
+        <v>1062000000</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>353</v>
@@ -28381,7 +28414,7 @@
       </c>
       <c r="D96" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E96" s="11">
         <f t="shared" si="4"/>
@@ -28389,7 +28422,7 @@
       </c>
       <c r="F96" s="11">
         <f t="shared" si="5"/>
-        <v>-2704000000</v>
+        <v>-3042000000</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>355</v>
@@ -28407,7 +28440,7 @@
       </c>
       <c r="D97" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E97" s="11">
         <f t="shared" si="4"/>
@@ -28415,7 +28448,7 @@
       </c>
       <c r="F97" s="11">
         <f t="shared" si="5"/>
-        <v>-2704000000</v>
+        <v>-3042000000</v>
       </c>
       <c r="G97" s="11"/>
     </row>
@@ -28431,7 +28464,7 @@
       </c>
       <c r="D98" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E98" s="11">
         <f t="shared" si="4"/>
@@ -28439,7 +28472,7 @@
       </c>
       <c r="F98" s="11">
         <f t="shared" si="5"/>
-        <v>2678000000</v>
+        <v>3016000000</v>
       </c>
       <c r="G98" s="11"/>
     </row>
@@ -28455,7 +28488,7 @@
       </c>
       <c r="D99" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E99" s="11">
         <f t="shared" si="4"/>
@@ -28463,7 +28496,7 @@
       </c>
       <c r="F99" s="11">
         <f t="shared" si="5"/>
-        <v>-20800000</v>
+        <v>-23400000</v>
       </c>
       <c r="G99" s="11"/>
       <c r="I99" t="s">
@@ -28482,7 +28515,7 @@
       </c>
       <c r="D100" s="11">
         <f t="shared" si="3"/>
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E100" s="11">
         <f t="shared" si="4"/>
@@ -28490,7 +28523,7 @@
       </c>
       <c r="F100" s="11">
         <f t="shared" si="5"/>
-        <v>2949200000</v>
+        <v>3328800000</v>
       </c>
       <c r="G100" s="11"/>
     </row>
@@ -28506,7 +28539,7 @@
       </c>
       <c r="D101" s="11">
         <f t="shared" si="3"/>
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E101" s="11">
         <f t="shared" si="4"/>
@@ -28514,7 +28547,7 @@
       </c>
       <c r="F101" s="11">
         <f t="shared" si="5"/>
-        <v>38394720</v>
+        <v>43594005</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>408</v>
@@ -28532,7 +28565,7 @@
       </c>
       <c r="D102" s="11">
         <f t="shared" si="3"/>
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E102" s="11">
         <f t="shared" si="4"/>
@@ -28540,7 +28573,7 @@
       </c>
       <c r="F102" s="11">
         <f t="shared" si="5"/>
-        <v>190000000</v>
+        <v>216000000</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>410</v>
@@ -28558,7 +28591,7 @@
       </c>
       <c r="D103" s="11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="E103" s="11">
         <f t="shared" si="4"/>
@@ -28566,7 +28599,7 @@
       </c>
       <c r="F103" s="11">
         <f t="shared" si="5"/>
-        <v>705000000</v>
+        <v>802500000</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>418</v>
@@ -28584,7 +28617,7 @@
       </c>
       <c r="D104" s="11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="E104" s="11">
         <f t="shared" si="4"/>
@@ -28592,7 +28625,7 @@
       </c>
       <c r="F104" s="11">
         <f t="shared" si="5"/>
-        <v>-6270000000</v>
+        <v>-7128000000</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>432</v>
@@ -28610,7 +28643,7 @@
       </c>
       <c r="D105" s="11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="E105" s="11">
         <f t="shared" si="4"/>
@@ -28618,7 +28651,7 @@
       </c>
       <c r="F105" s="11">
         <f t="shared" si="5"/>
-        <v>-13775000</v>
+        <v>-15660000</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>433</v>
@@ -28636,7 +28669,7 @@
       </c>
       <c r="D106" s="11">
         <f t="shared" si="3"/>
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E106" s="11">
         <f t="shared" si="4"/>
@@ -28644,7 +28677,7 @@
       </c>
       <c r="F106" s="11">
         <f t="shared" si="5"/>
-        <v>552000000</v>
+        <v>630000000</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>434</v>
@@ -28662,7 +28695,7 @@
       </c>
       <c r="D107" s="11">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E107" s="11">
         <f t="shared" si="4"/>
@@ -28670,7 +28703,7 @@
       </c>
       <c r="F107" s="11">
         <f t="shared" si="5"/>
-        <v>-546536900</v>
+        <v>-624613600</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>444</v>
@@ -28688,7 +28721,7 @@
       </c>
       <c r="D108" s="11">
         <f t="shared" si="3"/>
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E108" s="11">
         <f t="shared" si="4"/>
@@ -28696,7 +28729,7 @@
       </c>
       <c r="F108" s="11">
         <f t="shared" si="5"/>
-        <v>522000000</v>
+        <v>600000000</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>452</v>
@@ -28714,7 +28747,7 @@
       </c>
       <c r="D109" s="11">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E109" s="11">
         <f t="shared" si="4"/>
@@ -28722,7 +28755,7 @@
       </c>
       <c r="F109" s="11">
         <f t="shared" si="5"/>
-        <v>-9120000</v>
+        <v>-10680000</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>473</v>
@@ -28740,7 +28773,7 @@
       </c>
       <c r="D110" s="11">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E110" s="11">
         <f t="shared" si="4"/>
@@ -28748,7 +28781,7 @@
       </c>
       <c r="F110" s="11">
         <f t="shared" si="5"/>
-        <v>296000000</v>
+        <v>348000000</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>475</v>
@@ -28766,7 +28799,7 @@
       </c>
       <c r="D111" s="11">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E111" s="11">
         <f t="shared" si="4"/>
@@ -28774,7 +28807,7 @@
       </c>
       <c r="F111" s="11">
         <f t="shared" si="5"/>
-        <v>204400000</v>
+        <v>240800000</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>480</v>
@@ -28792,7 +28825,7 @@
       </c>
       <c r="D112" s="11">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E112" s="11">
         <f t="shared" si="4"/>
@@ -28800,7 +28833,7 @@
       </c>
       <c r="F112" s="11">
         <f t="shared" si="5"/>
-        <v>-14000000</v>
+        <v>-16600000</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>486</v>
@@ -28818,7 +28851,7 @@
       </c>
       <c r="D113" s="11">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E113" s="11">
         <f t="shared" si="4"/>
@@ -28826,7 +28859,7 @@
       </c>
       <c r="F113" s="11">
         <f t="shared" si="5"/>
-        <v>4917080</v>
+        <v>5857110</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>519</v>
@@ -28844,7 +28877,7 @@
       </c>
       <c r="D114" s="11">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E114" s="11">
         <f t="shared" si="4"/>
@@ -28852,7 +28885,7 @@
       </c>
       <c r="F114" s="11">
         <f t="shared" si="5"/>
-        <v>-10400000</v>
+        <v>-13000000</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>473</v>
@@ -28873,7 +28906,7 @@
       </c>
       <c r="D115" s="11">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E115" s="11">
         <f t="shared" si="4"/>
@@ -28881,7 +28914,7 @@
       </c>
       <c r="F115" s="25">
         <f t="shared" si="5"/>
-        <v>-561000000</v>
+        <v>-704000000</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>520</v>
@@ -28899,7 +28932,7 @@
       </c>
       <c r="D116" s="11">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E116" s="11">
         <f t="shared" si="4"/>
@@ -28907,7 +28940,7 @@
       </c>
       <c r="F116" s="11">
         <f t="shared" si="5"/>
-        <v>-10200000</v>
+        <v>-12800000</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>473</v>
@@ -28928,7 +28961,7 @@
       </c>
       <c r="D117" s="11">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E117" s="11">
         <f t="shared" si="4"/>
@@ -28936,7 +28969,7 @@
       </c>
       <c r="F117" s="11">
         <f t="shared" si="5"/>
-        <v>-22074500</v>
+        <v>-27931000</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>522</v>
@@ -28954,7 +28987,7 @@
       </c>
       <c r="D118" s="11">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E118" s="11">
         <f t="shared" si="4"/>
@@ -28962,7 +28995,7 @@
       </c>
       <c r="F118" s="11">
         <f t="shared" si="5"/>
-        <v>-9800000</v>
+        <v>-12400000</v>
       </c>
       <c r="G118" s="11" t="s">
         <v>523</v>
@@ -28983,7 +29016,7 @@
       </c>
       <c r="D119" s="11">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E119" s="11">
         <f t="shared" si="4"/>
@@ -28991,7 +29024,7 @@
       </c>
       <c r="F119" s="11">
         <f t="shared" si="5"/>
-        <v>-6645650</v>
+        <v>-8654800</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>526</v>
@@ -29009,7 +29042,7 @@
       </c>
       <c r="D120" s="11">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E120" s="11">
         <f t="shared" si="4"/>
@@ -29017,7 +29050,7 @@
       </c>
       <c r="F120" s="11">
         <f t="shared" si="5"/>
-        <v>-13760</v>
+        <v>-17920</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>527</v>
@@ -29035,7 +29068,7 @@
       </c>
       <c r="D121" s="11">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E121" s="11">
         <f t="shared" si="4"/>
@@ -29043,7 +29076,7 @@
       </c>
       <c r="F121" s="11">
         <f t="shared" si="5"/>
-        <v>-18144000</v>
+        <v>-23760000</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>529</v>
@@ -29061,7 +29094,7 @@
       </c>
       <c r="D122" s="11">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E122" s="11">
         <f t="shared" si="4"/>
@@ -29069,7 +29102,7 @@
       </c>
       <c r="F122" s="11">
         <f t="shared" si="5"/>
-        <v>2591505</v>
+        <v>3554064</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>531</v>
@@ -29087,7 +29120,7 @@
       </c>
       <c r="D123" s="11">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E123" s="11">
         <f t="shared" si="4"/>
@@ -29095,7 +29128,7 @@
       </c>
       <c r="F123" s="11">
         <f t="shared" si="5"/>
-        <v>-780000</v>
+        <v>-1456000</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>558</v>
@@ -29113,7 +29146,7 @@
       </c>
       <c r="D124" s="11">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E124" s="11">
         <f t="shared" si="4"/>
@@ -29121,7 +29154,7 @@
       </c>
       <c r="F124" s="11">
         <f t="shared" si="5"/>
-        <v>3561</v>
+        <v>18992</v>
       </c>
       <c r="G124" s="11" t="s">
         <v>613</v>
@@ -29139,7 +29172,7 @@
       </c>
       <c r="D125" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E125" s="11">
         <f t="shared" si="4"/>
@@ -29147,7 +29180,7 @@
       </c>
       <c r="F125" s="11">
         <f t="shared" si="5"/>
-        <v>4800000</v>
+        <v>36000000</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>611</v>
@@ -29165,7 +29198,7 @@
       </c>
       <c r="D126" s="11">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E126" s="11">
         <f t="shared" si="4"/>
@@ -29173,7 +29206,7 @@
       </c>
       <c r="F126" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>17456400</v>
       </c>
       <c r="G126" s="11" t="s">
         <v>622</v>
@@ -29187,11 +29220,11 @@
         <v>1342800</v>
       </c>
       <c r="C127" s="11">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D127" s="11">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E127" s="11">
         <f t="shared" si="4"/>
@@ -29199,21 +29232,25 @@
       </c>
       <c r="F127" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>17456400</v>
       </c>
       <c r="G127" s="11" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="11" t="s">
+        <v>630</v>
+      </c>
       <c r="B128" s="3">
-        <v>0</v>
-      </c>
-      <c r="C128" s="11"/>
+        <v>-200000</v>
+      </c>
+      <c r="C128" s="11">
+        <v>2</v>
+      </c>
       <c r="D128" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E128" s="11">
         <f t="shared" si="4"/>
@@ -29221,9 +29258,11 @@
       </c>
       <c r="F128" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G128" s="11"/>
+        <v>-400000</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="11"/>
@@ -29419,14 +29458,14 @@
       <c r="A139" s="11"/>
       <c r="B139" s="31">
         <f>SUM(B2:B137)</f>
-        <v>5132691</v>
+        <v>4932691</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="31">
         <f>SUM(F2:F137)</f>
-        <v>4308671947</v>
+        <v>4374996930</v>
       </c>
       <c r="G139" s="11"/>
     </row>
@@ -29460,7 +29499,7 @@
       <c r="E142" s="11"/>
       <c r="F142" s="3">
         <f>F139/D2</f>
-        <v>12035396.5</v>
+        <v>11792444.555256065</v>
       </c>
       <c r="G142" s="11"/>
     </row>
@@ -29489,8 +29528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29508,10 +29547,9 @@
     <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -29693,11 +29731,11 @@
       </c>
       <c r="F6" s="65">
         <f>K23</f>
-        <v>172043165.78082192</v>
+        <v>171563165.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>643011.78917810321</v>
+        <v>1123011.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -29817,11 +29855,11 @@
       </c>
       <c r="K9" s="46">
         <f>'مسکن ایلیا'!B139</f>
-        <v>5132691</v>
+        <v>4932691</v>
       </c>
       <c r="L9" s="3">
         <f>K9</f>
-        <v>5132691</v>
+        <v>4932691</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" ref="M9:M22" si="4">K9-L9</f>
@@ -30156,14 +30194,14 @@
         <v>470</v>
       </c>
       <c r="K17" s="46">
-        <v>600000</v>
+        <v>320000</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="4"/>
-        <v>600000</v>
+        <v>320000</v>
       </c>
       <c r="N17" s="27"/>
       <c r="O17" s="11" t="s">
@@ -30453,15 +30491,15 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>172043165.78082192</v>
+        <v>171563165.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>61262485.520547941</v>
+        <v>61062485.520547941</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
-        <v>110780680.26027396</v>
+        <v>110500680.26027396</v>
       </c>
       <c r="N23" s="27"/>
       <c r="O23" s="11" t="s">
@@ -30505,15 +30543,15 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>100160974</v>
+        <v>99680974</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12</f>
-        <v>21207691</v>
+        <v>21007691</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17</f>
-        <v>78903283</v>
+        <v>78623283</v>
       </c>
       <c r="N24" s="27"/>
       <c r="O24" s="11"/>
@@ -31780,12 +31818,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:G6">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G62">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finance file updated 18/4/1396
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="تیر 96" sheetId="23" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="633">
   <si>
     <t>18/1/95</t>
   </si>
@@ -1928,6 +1928,12 @@
   </si>
   <si>
     <t>16/4/1396</t>
+  </si>
+  <si>
+    <t>18/4/1396</t>
+  </si>
+  <si>
+    <t>خرید تخم مرغ و ... از جامبو</t>
   </si>
 </sst>
 </file>
@@ -2278,7 +2284,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2286,26 +2292,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -26078,9 +26064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
+      <selection pane="bottomLeft" activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26130,7 +26116,7 @@
       </c>
       <c r="D2" s="11">
         <f>D3+C2</f>
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -26138,7 +26124,7 @@
       </c>
       <c r="F2" s="11">
         <f>B2*(D2-E2)</f>
-        <v>35779000</v>
+        <v>35972400</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>1</v>
@@ -26156,7 +26142,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D66" si="0">D4+C3</f>
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E66" si="1">IF(B3&gt;0,1,0)</f>
@@ -26164,7 +26150,7 @@
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F66" si="2">B3*(D3-E3)</f>
-        <v>1104000000</v>
+        <v>1110000000</v>
       </c>
       <c r="G3" s="11"/>
     </row>
@@ -26180,7 +26166,7 @@
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" si="1"/>
@@ -26188,7 +26174,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" si="2"/>
-        <v>-73200000</v>
+        <v>-73600000</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -26204,7 +26190,7 @@
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="1"/>
@@ -26212,7 +26198,7 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="2"/>
-        <v>-36400000</v>
+        <v>-36600000</v>
       </c>
       <c r="G5" s="11"/>
     </row>
@@ -26228,7 +26214,7 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
@@ -26236,7 +26222,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="2"/>
-        <v>-19965000</v>
+        <v>-20075000</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -26252,7 +26238,7 @@
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
@@ -26260,7 +26246,7 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="2"/>
-        <v>-72400000</v>
+        <v>-72800000</v>
       </c>
       <c r="G7" s="11"/>
     </row>
@@ -26276,7 +26262,7 @@
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
@@ -26284,7 +26270,7 @@
       </c>
       <c r="F8" s="11">
         <f t="shared" si="2"/>
-        <v>-71600000</v>
+        <v>-72000000</v>
       </c>
       <c r="G8" s="11"/>
     </row>
@@ -26300,7 +26286,7 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
@@ -26308,7 +26294,7 @@
       </c>
       <c r="F9" s="11">
         <f t="shared" si="2"/>
-        <v>-331724500</v>
+        <v>-333625500</v>
       </c>
       <c r="G9" s="11"/>
     </row>
@@ -26324,7 +26310,7 @@
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
@@ -26332,7 +26318,7 @@
       </c>
       <c r="F10" s="11">
         <f t="shared" si="2"/>
-        <v>694000000</v>
+        <v>698000000</v>
       </c>
       <c r="G10" s="11"/>
     </row>
@@ -26348,7 +26334,7 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
@@ -26356,7 +26342,7 @@
       </c>
       <c r="F11" s="11">
         <f t="shared" si="2"/>
-        <v>-368490000</v>
+        <v>-370620000</v>
       </c>
       <c r="G11" s="11"/>
     </row>
@@ -26372,7 +26358,7 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
@@ -26380,7 +26366,7 @@
       </c>
       <c r="F12" s="11">
         <f t="shared" si="2"/>
-        <v>-15435000</v>
+        <v>-15525000</v>
       </c>
       <c r="G12" s="11"/>
     </row>
@@ -26396,7 +26382,7 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
@@ -26404,7 +26390,7 @@
       </c>
       <c r="F13" s="11">
         <f t="shared" si="2"/>
-        <v>-684239400</v>
+        <v>-688240800</v>
       </c>
       <c r="G13" s="11"/>
     </row>
@@ -26420,7 +26406,7 @@
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
@@ -26428,7 +26414,7 @@
       </c>
       <c r="F14" s="11">
         <f t="shared" si="2"/>
-        <v>-67600000</v>
+        <v>-68000000</v>
       </c>
       <c r="G14" s="11"/>
     </row>
@@ -26444,7 +26430,7 @@
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="1"/>
@@ -26452,7 +26438,7 @@
       </c>
       <c r="F15" s="11">
         <f t="shared" si="2"/>
-        <v>670000000</v>
+        <v>674000000</v>
       </c>
       <c r="G15" s="11"/>
     </row>
@@ -26468,7 +26454,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
@@ -26476,7 +26462,7 @@
       </c>
       <c r="F16" s="11">
         <f t="shared" si="2"/>
-        <v>670000000</v>
+        <v>674000000</v>
       </c>
       <c r="G16" s="11"/>
     </row>
@@ -26492,7 +26478,7 @@
       </c>
       <c r="D17" s="11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="1"/>
@@ -26500,7 +26486,7 @@
       </c>
       <c r="F17" s="11">
         <f t="shared" si="2"/>
-        <v>402000000</v>
+        <v>404400000</v>
       </c>
       <c r="G17" s="11"/>
     </row>
@@ -26516,7 +26502,7 @@
       </c>
       <c r="D18" s="11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
@@ -26524,7 +26510,7 @@
       </c>
       <c r="F18" s="11">
         <f t="shared" si="2"/>
-        <v>335000000</v>
+        <v>337000000</v>
       </c>
       <c r="G18" s="11"/>
     </row>
@@ -26540,7 +26526,7 @@
       </c>
       <c r="D19" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="1"/>
@@ -26548,7 +26534,7 @@
       </c>
       <c r="F19" s="11">
         <f t="shared" si="2"/>
-        <v>1002000000</v>
+        <v>1008000000</v>
       </c>
       <c r="G19" s="11"/>
       <c r="L19" t="s">
@@ -26567,7 +26553,7 @@
       </c>
       <c r="D20" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="1"/>
@@ -26575,7 +26561,7 @@
       </c>
       <c r="F20" s="11">
         <f t="shared" si="2"/>
-        <v>-144954500</v>
+        <v>-145819900</v>
       </c>
       <c r="G20" s="11"/>
     </row>
@@ -26591,7 +26577,7 @@
       </c>
       <c r="D21" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="1"/>
@@ -26599,7 +26585,7 @@
       </c>
       <c r="F21" s="11">
         <f t="shared" si="2"/>
-        <v>-144954500</v>
+        <v>-145819900</v>
       </c>
       <c r="G21" s="11"/>
     </row>
@@ -26615,7 +26601,7 @@
       </c>
       <c r="D22" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="1"/>
@@ -26623,7 +26609,7 @@
       </c>
       <c r="F22" s="11">
         <f t="shared" si="2"/>
-        <v>-144954500</v>
+        <v>-145819900</v>
       </c>
       <c r="G22" s="11"/>
     </row>
@@ -26639,7 +26625,7 @@
       </c>
       <c r="D23" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="1"/>
@@ -26647,7 +26633,7 @@
       </c>
       <c r="F23" s="11">
         <f t="shared" si="2"/>
-        <v>-144954500</v>
+        <v>-145819900</v>
       </c>
       <c r="G23" s="11"/>
     </row>
@@ -26663,7 +26649,7 @@
       </c>
       <c r="D24" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="1"/>
@@ -26671,7 +26657,7 @@
       </c>
       <c r="F24" s="11">
         <f t="shared" si="2"/>
-        <v>-144954500</v>
+        <v>-145819900</v>
       </c>
       <c r="G24" s="11"/>
     </row>
@@ -26687,7 +26673,7 @@
       </c>
       <c r="D25" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="1"/>
@@ -26695,7 +26681,7 @@
       </c>
       <c r="F25" s="11">
         <f t="shared" si="2"/>
-        <v>-67000000</v>
+        <v>-67400000</v>
       </c>
       <c r="G25" s="11"/>
     </row>
@@ -26711,7 +26697,7 @@
       </c>
       <c r="D26" s="11">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="1"/>
@@ -26719,7 +26705,7 @@
       </c>
       <c r="F26" s="11">
         <f t="shared" si="2"/>
-        <v>999000000</v>
+        <v>1005000000</v>
       </c>
       <c r="G26" s="11"/>
     </row>
@@ -26735,7 +26721,7 @@
       </c>
       <c r="D27" s="11">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="1"/>
@@ -26743,7 +26729,7 @@
       </c>
       <c r="F27" s="11">
         <f t="shared" si="2"/>
-        <v>-66400000</v>
+        <v>-66800000</v>
       </c>
       <c r="G27" s="11"/>
     </row>
@@ -26759,7 +26745,7 @@
       </c>
       <c r="D28" s="11">
         <f t="shared" si="0"/>
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E28" s="11">
         <f t="shared" si="1"/>
@@ -26767,7 +26753,7 @@
       </c>
       <c r="F28" s="11">
         <f t="shared" si="2"/>
-        <v>660000000</v>
+        <v>664000000</v>
       </c>
       <c r="G28" s="11"/>
     </row>
@@ -26783,7 +26769,7 @@
       </c>
       <c r="D29" s="11">
         <f t="shared" si="0"/>
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E29" s="11">
         <f t="shared" si="1"/>
@@ -26791,7 +26777,7 @@
       </c>
       <c r="F29" s="11">
         <f t="shared" si="2"/>
-        <v>-2310264000</v>
+        <v>-2324265600</v>
       </c>
       <c r="G29" s="11"/>
     </row>
@@ -26807,7 +26793,7 @@
       </c>
       <c r="D30" s="11">
         <f t="shared" si="0"/>
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" si="1"/>
@@ -26815,7 +26801,7 @@
       </c>
       <c r="F30" s="11">
         <f t="shared" si="2"/>
-        <v>-987296100</v>
+        <v>-993297900</v>
       </c>
       <c r="G30" s="11"/>
     </row>
@@ -26831,7 +26817,7 @@
       </c>
       <c r="D31" s="11">
         <f t="shared" si="0"/>
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="1"/>
@@ -26839,7 +26825,7 @@
       </c>
       <c r="F31" s="11">
         <f t="shared" si="2"/>
-        <v>-556255200</v>
+        <v>-559647000</v>
       </c>
       <c r="G31" s="11"/>
     </row>
@@ -26855,7 +26841,7 @@
       </c>
       <c r="D32" s="11">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="1"/>
@@ -26863,7 +26849,7 @@
       </c>
       <c r="F32" s="11">
         <f t="shared" si="2"/>
-        <v>322153200</v>
+        <v>324141800</v>
       </c>
       <c r="G32" s="11"/>
     </row>
@@ -26879,7 +26865,7 @@
       </c>
       <c r="D33" s="11">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="1"/>
@@ -26887,7 +26873,7 @@
       </c>
       <c r="F33" s="11">
         <f t="shared" si="2"/>
-        <v>11194029</v>
+        <v>11264211</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>383</v>
@@ -26905,7 +26891,7 @@
       </c>
       <c r="D34" s="11">
         <f t="shared" si="0"/>
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E34" s="11">
         <f t="shared" si="1"/>
@@ -26913,7 +26899,7 @@
       </c>
       <c r="F34" s="11">
         <f t="shared" si="2"/>
-        <v>-271150000</v>
+        <v>-272850000</v>
       </c>
       <c r="G34" s="11"/>
     </row>
@@ -26929,7 +26915,7 @@
       </c>
       <c r="D35" s="11">
         <f t="shared" si="0"/>
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="1"/>
@@ -26937,7 +26923,7 @@
       </c>
       <c r="F35" s="11">
         <f t="shared" si="2"/>
-        <v>-59245500</v>
+        <v>-59626500</v>
       </c>
       <c r="G35" s="11"/>
     </row>
@@ -26953,7 +26939,7 @@
       </c>
       <c r="D36" s="11">
         <f t="shared" si="0"/>
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E36" s="11">
         <f t="shared" si="1"/>
@@ -26961,7 +26947,7 @@
       </c>
       <c r="F36" s="11">
         <f t="shared" si="2"/>
-        <v>61800000</v>
+        <v>62200000</v>
       </c>
       <c r="G36" s="11"/>
     </row>
@@ -26977,7 +26963,7 @@
       </c>
       <c r="D37" s="11">
         <f t="shared" si="0"/>
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E37" s="11">
         <f t="shared" si="1"/>
@@ -26985,7 +26971,7 @@
       </c>
       <c r="F37" s="11">
         <f t="shared" si="2"/>
-        <v>-62000000</v>
+        <v>-62400000</v>
       </c>
       <c r="G37" s="11"/>
     </row>
@@ -27001,7 +26987,7 @@
       </c>
       <c r="D38" s="11">
         <f t="shared" si="0"/>
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E38" s="11">
         <f t="shared" si="1"/>
@@ -27009,7 +26995,7 @@
       </c>
       <c r="F38" s="11">
         <f t="shared" si="2"/>
-        <v>86331322</v>
+        <v>86932934</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>403</v>
@@ -27027,7 +27013,7 @@
       </c>
       <c r="D39" s="11">
         <f t="shared" si="0"/>
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E39" s="11">
         <f t="shared" si="1"/>
@@ -27035,7 +27021,7 @@
       </c>
       <c r="F39" s="11">
         <f t="shared" si="2"/>
-        <v>-27265000</v>
+        <v>-27455000</v>
       </c>
       <c r="G39" s="11"/>
     </row>
@@ -27051,7 +27037,7 @@
       </c>
       <c r="D40" s="11">
         <f t="shared" si="0"/>
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="1"/>
@@ -27059,7 +27045,7 @@
       </c>
       <c r="F40" s="11">
         <f t="shared" si="2"/>
-        <v>-25285561</v>
+        <v>-25461767</v>
       </c>
       <c r="G40" s="11"/>
     </row>
@@ -27075,7 +27061,7 @@
       </c>
       <c r="D41" s="11">
         <f t="shared" si="0"/>
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" si="1"/>
@@ -27083,7 +27069,7 @@
       </c>
       <c r="F41" s="11">
         <f t="shared" si="2"/>
-        <v>-33840000</v>
+        <v>-34080000</v>
       </c>
       <c r="G41" s="11"/>
     </row>
@@ -27099,7 +27085,7 @@
       </c>
       <c r="D42" s="11">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E42" s="11">
         <f t="shared" si="1"/>
@@ -27107,7 +27093,7 @@
       </c>
       <c r="F42" s="11">
         <f t="shared" si="2"/>
-        <v>259052836</v>
+        <v>261053244</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>404</v>
@@ -27125,7 +27111,7 @@
       </c>
       <c r="D43" s="11">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="1"/>
@@ -27133,7 +27119,7 @@
       </c>
       <c r="F43" s="11">
         <f t="shared" si="2"/>
-        <v>-20480000</v>
+        <v>-20640000</v>
       </c>
       <c r="G43" s="11"/>
     </row>
@@ -27149,7 +27135,7 @@
       </c>
       <c r="D44" s="11">
         <f t="shared" si="0"/>
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="1"/>
@@ -27157,7 +27143,7 @@
       </c>
       <c r="F44" s="11">
         <f t="shared" si="2"/>
-        <v>-53179308</v>
+        <v>-53601366</v>
       </c>
       <c r="G44" s="11"/>
     </row>
@@ -27173,7 +27159,7 @@
       </c>
       <c r="D45" s="11">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="1"/>
@@ -27181,7 +27167,7 @@
       </c>
       <c r="F45" s="11">
         <f t="shared" si="2"/>
-        <v>-50200000</v>
+        <v>-50600000</v>
       </c>
       <c r="G45" s="11"/>
     </row>
@@ -27197,7 +27183,7 @@
       </c>
       <c r="D46" s="11">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="1"/>
@@ -27205,7 +27191,7 @@
       </c>
       <c r="F46" s="11">
         <f t="shared" si="2"/>
-        <v>-23750000</v>
+        <v>-23940000</v>
       </c>
       <c r="G46" s="11"/>
     </row>
@@ -27221,7 +27207,7 @@
       </c>
       <c r="D47" s="11">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="1"/>
@@ -27229,7 +27215,7 @@
       </c>
       <c r="F47" s="11">
         <f t="shared" si="2"/>
-        <v>-11160000</v>
+        <v>-11250000</v>
       </c>
       <c r="G47" s="11"/>
     </row>
@@ -27245,7 +27231,7 @@
       </c>
       <c r="D48" s="11">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="1"/>
@@ -27253,7 +27239,7 @@
       </c>
       <c r="F48" s="11">
         <f t="shared" si="2"/>
-        <v>-15916640</v>
+        <v>-16045000</v>
       </c>
       <c r="G48" s="11"/>
     </row>
@@ -27269,7 +27255,7 @@
       </c>
       <c r="D49" s="11">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E49" s="11">
         <f t="shared" si="1"/>
@@ -27277,7 +27263,7 @@
       </c>
       <c r="F49" s="11">
         <f t="shared" si="2"/>
-        <v>-6733580</v>
+        <v>-6788548</v>
       </c>
       <c r="G49" s="11"/>
     </row>
@@ -27293,7 +27279,7 @@
       </c>
       <c r="D50" s="11">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E50" s="11">
         <f t="shared" si="1"/>
@@ -27301,7 +27287,7 @@
       </c>
       <c r="F50" s="11">
         <f t="shared" si="2"/>
-        <v>-34404000</v>
+        <v>-34686000</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -27317,7 +27303,7 @@
       </c>
       <c r="D51" s="11">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E51" s="11">
         <f t="shared" si="1"/>
@@ -27325,7 +27311,7 @@
       </c>
       <c r="F51" s="11">
         <f t="shared" si="2"/>
-        <v>-6526024</v>
+        <v>-6579516</v>
       </c>
       <c r="G51" s="11"/>
     </row>
@@ -27341,7 +27327,7 @@
       </c>
       <c r="D52" s="11">
         <f t="shared" si="0"/>
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E52" s="11">
         <f t="shared" si="1"/>
@@ -27349,7 +27335,7 @@
       </c>
       <c r="F52" s="11">
         <f t="shared" si="2"/>
-        <v>-12951900</v>
+        <v>-13058500</v>
       </c>
       <c r="G52" s="11"/>
     </row>
@@ -27365,7 +27351,7 @@
       </c>
       <c r="D53" s="11">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E53" s="11">
         <f t="shared" si="1"/>
@@ -27373,7 +27359,7 @@
       </c>
       <c r="F53" s="11">
         <f t="shared" si="2"/>
-        <v>241000000</v>
+        <v>243000000</v>
       </c>
       <c r="G53" s="11"/>
     </row>
@@ -27389,7 +27375,7 @@
       </c>
       <c r="D54" s="11">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E54" s="11">
         <f t="shared" si="1"/>
@@ -27397,7 +27383,7 @@
       </c>
       <c r="F54" s="11">
         <f t="shared" si="2"/>
-        <v>-4956000</v>
+        <v>-4998000</v>
       </c>
       <c r="G54" s="11"/>
     </row>
@@ -27413,7 +27399,7 @@
       </c>
       <c r="D55" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E55" s="11">
         <f t="shared" si="1"/>
@@ -27421,7 +27407,7 @@
       </c>
       <c r="F55" s="11">
         <f t="shared" si="2"/>
-        <v>-230417500</v>
+        <v>-232378500</v>
       </c>
       <c r="G55" s="11"/>
     </row>
@@ -27437,7 +27423,7 @@
       </c>
       <c r="D56" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="1"/>
@@ -27445,7 +27431,7 @@
       </c>
       <c r="F56" s="11">
         <f t="shared" si="2"/>
-        <v>-10575000</v>
+        <v>-10665000</v>
       </c>
       <c r="G56" s="11"/>
     </row>
@@ -27461,7 +27447,7 @@
       </c>
       <c r="D57" s="11">
         <f t="shared" si="0"/>
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E57" s="11">
         <f t="shared" si="1"/>
@@ -27469,7 +27455,7 @@
       </c>
       <c r="F57" s="11">
         <f t="shared" si="2"/>
-        <v>664146769</v>
+        <v>670157147</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>405</v>
@@ -27487,7 +27473,7 @@
       </c>
       <c r="D58" s="11">
         <f t="shared" si="0"/>
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E58" s="11">
         <f t="shared" si="1"/>
@@ -27495,7 +27481,7 @@
       </c>
       <c r="F58" s="11">
         <f t="shared" si="2"/>
-        <v>442000000</v>
+        <v>446000000</v>
       </c>
       <c r="G58" s="11"/>
     </row>
@@ -27511,7 +27497,7 @@
       </c>
       <c r="D59" s="11">
         <f t="shared" si="0"/>
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E59" s="11">
         <f t="shared" si="1"/>
@@ -27519,7 +27505,7 @@
       </c>
       <c r="F59" s="11">
         <f t="shared" si="2"/>
-        <v>440000000</v>
+        <v>444000000</v>
       </c>
       <c r="G59" s="11"/>
     </row>
@@ -27535,7 +27521,7 @@
       </c>
       <c r="D60" s="11">
         <f t="shared" si="0"/>
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E60" s="11">
         <f t="shared" si="1"/>
@@ -27543,7 +27529,7 @@
       </c>
       <c r="F60" s="11">
         <f t="shared" si="2"/>
-        <v>-1547331500</v>
+        <v>-1561334500</v>
       </c>
       <c r="G60" s="11"/>
     </row>
@@ -27559,7 +27545,7 @@
       </c>
       <c r="D61" s="11">
         <f t="shared" si="0"/>
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E61" s="11">
         <f t="shared" si="1"/>
@@ -27567,7 +27553,7 @@
       </c>
       <c r="F61" s="11">
         <f t="shared" si="2"/>
-        <v>588000000</v>
+        <v>594000000</v>
       </c>
       <c r="G61" s="11"/>
     </row>
@@ -27583,7 +27569,7 @@
       </c>
       <c r="D62" s="11">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E62" s="11">
         <f t="shared" si="1"/>
@@ -27591,7 +27577,7 @@
       </c>
       <c r="F62" s="11">
         <f t="shared" si="2"/>
-        <v>-5313364</v>
+        <v>-5367582</v>
       </c>
       <c r="G62" s="11"/>
     </row>
@@ -27607,7 +27593,7 @@
       </c>
       <c r="D63" s="11">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E63" s="11">
         <f t="shared" si="1"/>
@@ -27615,7 +27601,7 @@
       </c>
       <c r="F63" s="11">
         <f t="shared" si="2"/>
-        <v>-6465844</v>
+        <v>-6531822</v>
       </c>
       <c r="G63" s="11"/>
     </row>
@@ -27631,7 +27617,7 @@
       </c>
       <c r="D64" s="11">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E64" s="11">
         <f t="shared" si="1"/>
@@ -27639,7 +27625,7 @@
       </c>
       <c r="F64" s="11">
         <f t="shared" si="2"/>
-        <v>585000000</v>
+        <v>591000000</v>
       </c>
       <c r="G64" s="11"/>
     </row>
@@ -27655,7 +27641,7 @@
       </c>
       <c r="D65" s="11">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E65" s="11">
         <f t="shared" si="1"/>
@@ -27663,7 +27649,7 @@
       </c>
       <c r="F65" s="11">
         <f t="shared" si="2"/>
-        <v>579150000</v>
+        <v>585090000</v>
       </c>
       <c r="G65" s="11"/>
     </row>
@@ -27679,7 +27665,7 @@
       </c>
       <c r="D66" s="11">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E66" s="11">
         <f t="shared" si="1"/>
@@ -27687,7 +27673,7 @@
       </c>
       <c r="F66" s="11">
         <f t="shared" si="2"/>
-        <v>195000000</v>
+        <v>197000000</v>
       </c>
       <c r="G66" s="11"/>
     </row>
@@ -27703,7 +27689,7 @@
       </c>
       <c r="D67" s="11">
         <f t="shared" ref="D67:D130" si="3">D68+C67</f>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E67" s="11">
         <f t="shared" ref="E67:E130" si="4">IF(B67&gt;0,1,0)</f>
@@ -27711,7 +27697,7 @@
       </c>
       <c r="F67" s="11">
         <f t="shared" ref="F67:F137" si="5">B67*(D67-E67)</f>
-        <v>5850000</v>
+        <v>5910000</v>
       </c>
       <c r="G67" s="11"/>
     </row>
@@ -27727,7 +27713,7 @@
       </c>
       <c r="D68" s="11">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E68" s="11">
         <f t="shared" si="4"/>
@@ -27735,7 +27721,7 @@
       </c>
       <c r="F68" s="11">
         <f t="shared" si="5"/>
-        <v>5820000000</v>
+        <v>5880000000</v>
       </c>
       <c r="G68" s="11"/>
     </row>
@@ -27751,7 +27737,7 @@
       </c>
       <c r="D69" s="11">
         <f t="shared" si="3"/>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E69" s="11">
         <f t="shared" si="4"/>
@@ -27759,7 +27745,7 @@
       </c>
       <c r="F69" s="11">
         <f t="shared" si="5"/>
-        <v>-38800000</v>
+        <v>-39200000</v>
       </c>
       <c r="G69" s="11"/>
     </row>
@@ -27775,7 +27761,7 @@
       </c>
       <c r="D70" s="11">
         <f t="shared" si="3"/>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E70" s="11">
         <f t="shared" si="4"/>
@@ -27783,7 +27769,7 @@
       </c>
       <c r="F70" s="11">
         <f t="shared" si="5"/>
-        <v>270200000</v>
+        <v>273000000</v>
       </c>
       <c r="G70" s="11"/>
     </row>
@@ -27799,7 +27785,7 @@
       </c>
       <c r="D71" s="11">
         <f t="shared" si="3"/>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E71" s="11">
         <f t="shared" si="4"/>
@@ -27807,7 +27793,7 @@
       </c>
       <c r="F71" s="11">
         <f t="shared" si="5"/>
-        <v>501800000</v>
+        <v>507000000</v>
       </c>
       <c r="G71" s="11"/>
     </row>
@@ -27823,7 +27809,7 @@
       </c>
       <c r="D72" s="11">
         <f t="shared" si="3"/>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E72" s="11">
         <f t="shared" si="4"/>
@@ -27831,7 +27817,7 @@
       </c>
       <c r="F72" s="11">
         <f t="shared" si="5"/>
-        <v>-194000000</v>
+        <v>-196000000</v>
       </c>
       <c r="G72" s="11"/>
     </row>
@@ -27847,7 +27833,7 @@
       </c>
       <c r="D73" s="11">
         <f t="shared" si="3"/>
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E73" s="11">
         <f t="shared" si="4"/>
@@ -27855,7 +27841,7 @@
       </c>
       <c r="F73" s="11">
         <f t="shared" si="5"/>
-        <v>2865000000</v>
+        <v>2895000000</v>
       </c>
       <c r="G73" s="11"/>
     </row>
@@ -27871,7 +27857,7 @@
       </c>
       <c r="D74" s="11">
         <f t="shared" si="3"/>
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E74" s="11">
         <f t="shared" si="4"/>
@@ -27879,7 +27865,7 @@
       </c>
       <c r="F74" s="11">
         <f t="shared" si="5"/>
-        <v>-2805785400</v>
+        <v>-2835793800</v>
       </c>
       <c r="G74" s="11"/>
     </row>
@@ -27895,7 +27881,7 @@
       </c>
       <c r="D75" s="11">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E75" s="11">
         <f t="shared" si="4"/>
@@ -27903,7 +27889,7 @@
       </c>
       <c r="F75" s="11">
         <f t="shared" si="5"/>
-        <v>-555000000</v>
+        <v>-561000000</v>
       </c>
       <c r="G75" s="11"/>
     </row>
@@ -27919,7 +27905,7 @@
       </c>
       <c r="D76" s="11">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E76" s="11">
         <f t="shared" si="4"/>
@@ -27927,7 +27913,7 @@
       </c>
       <c r="F76" s="11">
         <f t="shared" si="5"/>
-        <v>-37000000</v>
+        <v>-37400000</v>
       </c>
       <c r="G76" s="11"/>
     </row>
@@ -27943,7 +27929,7 @@
       </c>
       <c r="D77" s="11">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E77" s="11">
         <f t="shared" si="4"/>
@@ -27951,7 +27937,7 @@
       </c>
       <c r="F77" s="11">
         <f t="shared" si="5"/>
-        <v>-2220555000</v>
+        <v>-2244561000</v>
       </c>
       <c r="G77" s="11"/>
     </row>
@@ -27967,7 +27953,7 @@
       </c>
       <c r="D78" s="11">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E78" s="11">
         <f t="shared" si="4"/>
@@ -27975,7 +27961,7 @@
       </c>
       <c r="F78" s="11">
         <f t="shared" si="5"/>
-        <v>-543162900</v>
+        <v>-549164700</v>
       </c>
       <c r="G78" s="11"/>
     </row>
@@ -27991,7 +27977,7 @@
       </c>
       <c r="D79" s="11">
         <f t="shared" si="3"/>
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E79" s="11">
         <f t="shared" si="4"/>
@@ -27999,7 +27985,7 @@
       </c>
       <c r="F79" s="11">
         <f t="shared" si="5"/>
-        <v>4025000000</v>
+        <v>4071000000</v>
       </c>
       <c r="G79" s="11"/>
     </row>
@@ -28015,7 +28001,7 @@
       </c>
       <c r="D80" s="11">
         <f t="shared" si="3"/>
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E80" s="11">
         <f t="shared" si="4"/>
@@ -28023,7 +28009,7 @@
       </c>
       <c r="F80" s="11">
         <f t="shared" si="5"/>
-        <v>-102685500</v>
+        <v>-103886500</v>
       </c>
       <c r="G80" s="11"/>
     </row>
@@ -28039,7 +28025,7 @@
       </c>
       <c r="D81" s="11">
         <f t="shared" si="3"/>
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E81" s="11">
         <f t="shared" si="4"/>
@@ -28047,7 +28033,7 @@
       </c>
       <c r="F81" s="11">
         <f t="shared" si="5"/>
-        <v>-34200000</v>
+        <v>-34600000</v>
       </c>
       <c r="G81" s="11"/>
     </row>
@@ -28063,7 +28049,7 @@
       </c>
       <c r="D82" s="11">
         <f t="shared" si="3"/>
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E82" s="11">
         <f t="shared" si="4"/>
@@ -28071,7 +28057,7 @@
       </c>
       <c r="F82" s="11">
         <f t="shared" si="5"/>
-        <v>47864349</v>
+        <v>48430791</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>242</v>
@@ -28089,7 +28075,7 @@
       </c>
       <c r="D83" s="11">
         <f t="shared" si="3"/>
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E83" s="11">
         <f t="shared" si="4"/>
@@ -28097,7 +28083,7 @@
       </c>
       <c r="F83" s="11">
         <f t="shared" si="5"/>
-        <v>-34000000</v>
+        <v>-34400000</v>
       </c>
       <c r="G83" s="11"/>
     </row>
@@ -28113,7 +28099,7 @@
       </c>
       <c r="D84" s="11">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E84" s="11">
         <f t="shared" si="4"/>
@@ -28121,7 +28107,7 @@
       </c>
       <c r="F84" s="11">
         <f t="shared" si="5"/>
-        <v>334000000</v>
+        <v>338000000</v>
       </c>
       <c r="G84" s="11"/>
     </row>
@@ -28137,7 +28123,7 @@
       </c>
       <c r="D85" s="11">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E85" s="11">
         <f t="shared" si="4"/>
@@ -28145,7 +28131,7 @@
       </c>
       <c r="F85" s="11">
         <f t="shared" si="5"/>
-        <v>-33000000</v>
+        <v>-33400000</v>
       </c>
       <c r="G85" s="11"/>
     </row>
@@ -28161,7 +28147,7 @@
       </c>
       <c r="D86" s="11">
         <f t="shared" si="3"/>
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E86" s="11">
         <f t="shared" si="4"/>
@@ -28169,7 +28155,7 @@
       </c>
       <c r="F86" s="11">
         <f t="shared" si="5"/>
-        <v>-31800000</v>
+        <v>-32200000</v>
       </c>
       <c r="G86" s="11"/>
     </row>
@@ -28185,7 +28171,7 @@
       </c>
       <c r="D87" s="11">
         <f t="shared" si="3"/>
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E87" s="11">
         <f t="shared" si="4"/>
@@ -28193,7 +28179,7 @@
       </c>
       <c r="F87" s="11">
         <f t="shared" si="5"/>
-        <v>-208025000</v>
+        <v>-210675000</v>
       </c>
       <c r="G87" s="11"/>
     </row>
@@ -28209,7 +28195,7 @@
       </c>
       <c r="D88" s="11">
         <f t="shared" si="3"/>
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E88" s="11">
         <f t="shared" si="4"/>
@@ -28217,7 +28203,7 @@
       </c>
       <c r="F88" s="11">
         <f t="shared" si="5"/>
-        <v>-71000000</v>
+        <v>-72000000</v>
       </c>
       <c r="G88" s="11"/>
     </row>
@@ -28233,7 +28219,7 @@
       </c>
       <c r="D89" s="11">
         <f t="shared" si="3"/>
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E89" s="11">
         <f t="shared" si="4"/>
@@ -28241,7 +28227,7 @@
       </c>
       <c r="F89" s="11">
         <f t="shared" si="5"/>
-        <v>-17040000</v>
+        <v>-17280000</v>
       </c>
       <c r="G89" s="11"/>
     </row>
@@ -28257,7 +28243,7 @@
       </c>
       <c r="D90" s="11">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E90" s="11">
         <f t="shared" si="4"/>
@@ -28265,7 +28251,7 @@
       </c>
       <c r="F90" s="11">
         <f t="shared" si="5"/>
-        <v>59520495</v>
+        <v>60376905</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>264</v>
@@ -28283,7 +28269,7 @@
       </c>
       <c r="D91" s="11">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E91" s="11">
         <f t="shared" si="4"/>
@@ -28291,7 +28277,7 @@
       </c>
       <c r="F91" s="11">
         <f t="shared" si="5"/>
-        <v>-411274000</v>
+        <v>-417278000</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>345</v>
@@ -28309,7 +28295,7 @@
       </c>
       <c r="D92" s="11">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E92" s="11">
         <f t="shared" si="4"/>
@@ -28317,7 +28303,7 @@
       </c>
       <c r="F92" s="11">
         <f t="shared" si="5"/>
-        <v>-27675000</v>
+        <v>-28085000</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>346</v>
@@ -28335,7 +28321,7 @@
       </c>
       <c r="D93" s="11">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E93" s="11">
         <f t="shared" si="4"/>
@@ -28343,7 +28329,7 @@
       </c>
       <c r="F93" s="11">
         <f t="shared" si="5"/>
-        <v>-47317500</v>
+        <v>-48018500</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>343</v>
@@ -28361,7 +28347,7 @@
       </c>
       <c r="D94" s="11">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E94" s="11">
         <f t="shared" si="4"/>
@@ -28369,7 +28355,7 @@
       </c>
       <c r="F94" s="11">
         <f t="shared" si="5"/>
-        <v>123000000</v>
+        <v>125000000</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>341</v>
@@ -28387,7 +28373,7 @@
       </c>
       <c r="D95" s="11">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E95" s="11">
         <f t="shared" si="4"/>
@@ -28395,7 +28381,7 @@
       </c>
       <c r="F95" s="11">
         <f t="shared" si="5"/>
-        <v>1062000000</v>
+        <v>1080000000</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>353</v>
@@ -28414,7 +28400,7 @@
       </c>
       <c r="D96" s="11">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E96" s="11">
         <f t="shared" si="4"/>
@@ -28422,7 +28408,7 @@
       </c>
       <c r="F96" s="11">
         <f t="shared" si="5"/>
-        <v>-3042000000</v>
+        <v>-3094000000</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>355</v>
@@ -28440,7 +28426,7 @@
       </c>
       <c r="D97" s="11">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E97" s="11">
         <f t="shared" si="4"/>
@@ -28448,7 +28434,7 @@
       </c>
       <c r="F97" s="11">
         <f t="shared" si="5"/>
-        <v>-3042000000</v>
+        <v>-3094000000</v>
       </c>
       <c r="G97" s="11"/>
     </row>
@@ -28464,7 +28450,7 @@
       </c>
       <c r="D98" s="11">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E98" s="11">
         <f t="shared" si="4"/>
@@ -28472,7 +28458,7 @@
       </c>
       <c r="F98" s="11">
         <f t="shared" si="5"/>
-        <v>3016000000</v>
+        <v>3068000000</v>
       </c>
       <c r="G98" s="11"/>
     </row>
@@ -28488,7 +28474,7 @@
       </c>
       <c r="D99" s="11">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E99" s="11">
         <f t="shared" si="4"/>
@@ -28496,7 +28482,7 @@
       </c>
       <c r="F99" s="11">
         <f t="shared" si="5"/>
-        <v>-23400000</v>
+        <v>-23800000</v>
       </c>
       <c r="G99" s="11"/>
       <c r="I99" t="s">
@@ -28515,7 +28501,7 @@
       </c>
       <c r="D100" s="11">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E100" s="11">
         <f t="shared" si="4"/>
@@ -28523,7 +28509,7 @@
       </c>
       <c r="F100" s="11">
         <f t="shared" si="5"/>
-        <v>3328800000</v>
+        <v>3387200000</v>
       </c>
       <c r="G100" s="11"/>
     </row>
@@ -28539,7 +28525,7 @@
       </c>
       <c r="D101" s="11">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E101" s="11">
         <f t="shared" si="4"/>
@@ -28547,7 +28533,7 @@
       </c>
       <c r="F101" s="11">
         <f t="shared" si="5"/>
-        <v>43594005</v>
+        <v>44393895</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>408</v>
@@ -28565,7 +28551,7 @@
       </c>
       <c r="D102" s="11">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E102" s="11">
         <f t="shared" si="4"/>
@@ -28573,7 +28559,7 @@
       </c>
       <c r="F102" s="11">
         <f t="shared" si="5"/>
-        <v>216000000</v>
+        <v>220000000</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>410</v>
@@ -28591,7 +28577,7 @@
       </c>
       <c r="D103" s="11">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E103" s="11">
         <f t="shared" si="4"/>
@@ -28599,7 +28585,7 @@
       </c>
       <c r="F103" s="11">
         <f t="shared" si="5"/>
-        <v>802500000</v>
+        <v>817500000</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>418</v>
@@ -28617,7 +28603,7 @@
       </c>
       <c r="D104" s="11">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E104" s="11">
         <f t="shared" si="4"/>
@@ -28625,7 +28611,7 @@
       </c>
       <c r="F104" s="11">
         <f t="shared" si="5"/>
-        <v>-7128000000</v>
+        <v>-7260000000</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>432</v>
@@ -28643,7 +28629,7 @@
       </c>
       <c r="D105" s="11">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E105" s="11">
         <f t="shared" si="4"/>
@@ -28651,7 +28637,7 @@
       </c>
       <c r="F105" s="11">
         <f t="shared" si="5"/>
-        <v>-15660000</v>
+        <v>-15950000</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>433</v>
@@ -28669,7 +28655,7 @@
       </c>
       <c r="D106" s="11">
         <f t="shared" si="3"/>
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E106" s="11">
         <f t="shared" si="4"/>
@@ -28677,7 +28663,7 @@
       </c>
       <c r="F106" s="11">
         <f t="shared" si="5"/>
-        <v>630000000</v>
+        <v>642000000</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>434</v>
@@ -28695,7 +28681,7 @@
       </c>
       <c r="D107" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E107" s="11">
         <f t="shared" si="4"/>
@@ -28703,7 +28689,7 @@
       </c>
       <c r="F107" s="11">
         <f t="shared" si="5"/>
-        <v>-624613600</v>
+        <v>-636625400</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>444</v>
@@ -28721,7 +28707,7 @@
       </c>
       <c r="D108" s="11">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E108" s="11">
         <f t="shared" si="4"/>
@@ -28729,7 +28715,7 @@
       </c>
       <c r="F108" s="11">
         <f t="shared" si="5"/>
-        <v>600000000</v>
+        <v>612000000</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>452</v>
@@ -28747,7 +28733,7 @@
       </c>
       <c r="D109" s="11">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E109" s="11">
         <f t="shared" si="4"/>
@@ -28755,7 +28741,7 @@
       </c>
       <c r="F109" s="11">
         <f t="shared" si="5"/>
-        <v>-10680000</v>
+        <v>-10920000</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>473</v>
@@ -28773,7 +28759,7 @@
       </c>
       <c r="D110" s="11">
         <f t="shared" si="3"/>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E110" s="11">
         <f t="shared" si="4"/>
@@ -28781,7 +28767,7 @@
       </c>
       <c r="F110" s="11">
         <f t="shared" si="5"/>
-        <v>348000000</v>
+        <v>356000000</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>475</v>
@@ -28799,7 +28785,7 @@
       </c>
       <c r="D111" s="11">
         <f t="shared" si="3"/>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E111" s="11">
         <f t="shared" si="4"/>
@@ -28807,7 +28793,7 @@
       </c>
       <c r="F111" s="11">
         <f t="shared" si="5"/>
-        <v>240800000</v>
+        <v>246400000</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>480</v>
@@ -28825,7 +28811,7 @@
       </c>
       <c r="D112" s="11">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E112" s="11">
         <f t="shared" si="4"/>
@@ -28833,7 +28819,7 @@
       </c>
       <c r="F112" s="11">
         <f t="shared" si="5"/>
-        <v>-16600000</v>
+        <v>-17000000</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>486</v>
@@ -28851,7 +28837,7 @@
       </c>
       <c r="D113" s="11">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E113" s="11">
         <f t="shared" si="4"/>
@@ -28859,7 +28845,7 @@
       </c>
       <c r="F113" s="11">
         <f t="shared" si="5"/>
-        <v>5857110</v>
+        <v>6001730</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>519</v>
@@ -28877,7 +28863,7 @@
       </c>
       <c r="D114" s="11">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E114" s="11">
         <f t="shared" si="4"/>
@@ -28885,7 +28871,7 @@
       </c>
       <c r="F114" s="11">
         <f t="shared" si="5"/>
-        <v>-13000000</v>
+        <v>-13400000</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>473</v>
@@ -28906,7 +28892,7 @@
       </c>
       <c r="D115" s="11">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E115" s="11">
         <f t="shared" si="4"/>
@@ -28914,7 +28900,7 @@
       </c>
       <c r="F115" s="25">
         <f t="shared" si="5"/>
-        <v>-704000000</v>
+        <v>-726000000</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>520</v>
@@ -28932,7 +28918,7 @@
       </c>
       <c r="D116" s="11">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E116" s="11">
         <f t="shared" si="4"/>
@@ -28940,7 +28926,7 @@
       </c>
       <c r="F116" s="11">
         <f t="shared" si="5"/>
-        <v>-12800000</v>
+        <v>-13200000</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>473</v>
@@ -28961,7 +28947,7 @@
       </c>
       <c r="D117" s="11">
         <f t="shared" si="3"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E117" s="11">
         <f t="shared" si="4"/>
@@ -28969,7 +28955,7 @@
       </c>
       <c r="F117" s="11">
         <f t="shared" si="5"/>
-        <v>-27931000</v>
+        <v>-28832000</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>522</v>
@@ -28987,7 +28973,7 @@
       </c>
       <c r="D118" s="11">
         <f t="shared" si="3"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E118" s="11">
         <f t="shared" si="4"/>
@@ -28995,7 +28981,7 @@
       </c>
       <c r="F118" s="11">
         <f t="shared" si="5"/>
-        <v>-12400000</v>
+        <v>-12800000</v>
       </c>
       <c r="G118" s="11" t="s">
         <v>523</v>
@@ -29016,7 +29002,7 @@
       </c>
       <c r="D119" s="11">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E119" s="11">
         <f t="shared" si="4"/>
@@ -29024,7 +29010,7 @@
       </c>
       <c r="F119" s="11">
         <f t="shared" si="5"/>
-        <v>-8654800</v>
+        <v>-8963900</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>526</v>
@@ -29042,7 +29028,7 @@
       </c>
       <c r="D120" s="11">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E120" s="11">
         <f t="shared" si="4"/>
@@ -29050,7 +29036,7 @@
       </c>
       <c r="F120" s="11">
         <f t="shared" si="5"/>
-        <v>-17920</v>
+        <v>-18560</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>527</v>
@@ -29068,7 +29054,7 @@
       </c>
       <c r="D121" s="11">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E121" s="11">
         <f t="shared" si="4"/>
@@ -29076,7 +29062,7 @@
       </c>
       <c r="F121" s="11">
         <f t="shared" si="5"/>
-        <v>-23760000</v>
+        <v>-24624000</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>529</v>
@@ -29094,7 +29080,7 @@
       </c>
       <c r="D122" s="11">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E122" s="11">
         <f t="shared" si="4"/>
@@ -29102,7 +29088,7 @@
       </c>
       <c r="F122" s="11">
         <f t="shared" si="5"/>
-        <v>3554064</v>
+        <v>3702150</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>531</v>
@@ -29120,7 +29106,7 @@
       </c>
       <c r="D123" s="11">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E123" s="11">
         <f t="shared" si="4"/>
@@ -29128,7 +29114,7 @@
       </c>
       <c r="F123" s="11">
         <f t="shared" si="5"/>
-        <v>-1456000</v>
+        <v>-1560000</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>558</v>
@@ -29146,7 +29132,7 @@
       </c>
       <c r="D124" s="11">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E124" s="11">
         <f t="shared" si="4"/>
@@ -29154,7 +29140,7 @@
       </c>
       <c r="F124" s="11">
         <f t="shared" si="5"/>
-        <v>18992</v>
+        <v>21366</v>
       </c>
       <c r="G124" s="11" t="s">
         <v>613</v>
@@ -29172,7 +29158,7 @@
       </c>
       <c r="D125" s="11">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E125" s="11">
         <f t="shared" si="4"/>
@@ -29180,7 +29166,7 @@
       </c>
       <c r="F125" s="11">
         <f t="shared" si="5"/>
-        <v>36000000</v>
+        <v>40800000</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>611</v>
@@ -29198,7 +29184,7 @@
       </c>
       <c r="D126" s="11">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E126" s="11">
         <f t="shared" si="4"/>
@@ -29206,7 +29192,7 @@
       </c>
       <c r="F126" s="11">
         <f t="shared" si="5"/>
-        <v>17456400</v>
+        <v>20142000</v>
       </c>
       <c r="G126" s="11" t="s">
         <v>622</v>
@@ -29224,7 +29210,7 @@
       </c>
       <c r="D127" s="11">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E127" s="11">
         <f t="shared" si="4"/>
@@ -29232,7 +29218,7 @@
       </c>
       <c r="F127" s="11">
         <f t="shared" si="5"/>
-        <v>17456400</v>
+        <v>20142000</v>
       </c>
       <c r="G127" s="11" t="s">
         <v>623</v>
@@ -29250,7 +29236,7 @@
       </c>
       <c r="D128" s="11">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E128" s="11">
         <f t="shared" si="4"/>
@@ -29258,23 +29244,25 @@
       </c>
       <c r="F128" s="11">
         <f t="shared" si="5"/>
-        <v>-400000</v>
+        <v>-800000</v>
       </c>
       <c r="G128" s="11" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
+      <c r="A129" s="11" t="s">
+        <v>631</v>
+      </c>
       <c r="B129" s="3">
-        <v>0</v>
+        <v>-15618</v>
       </c>
       <c r="C129" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D129" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E129" s="11">
         <f t="shared" si="4"/>
@@ -29282,9 +29270,11 @@
       </c>
       <c r="F129" s="11">
         <f>B129*(D129-E129)</f>
-        <v>0</v>
-      </c>
-      <c r="G129" s="11"/>
+        <v>-31236</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>632</v>
+      </c>
       <c r="K129" t="s">
         <v>25</v>
       </c>
@@ -29458,14 +29448,14 @@
       <c r="A139" s="11"/>
       <c r="B139" s="31">
         <f>SUM(B2:B137)</f>
-        <v>4932691</v>
+        <v>4917073</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="31">
         <f>SUM(F2:F137)</f>
-        <v>4374996930</v>
+        <v>4384831076</v>
       </c>
       <c r="G139" s="11"/>
     </row>
@@ -29499,7 +29489,7 @@
       <c r="E142" s="11"/>
       <c r="F142" s="3">
         <f>F139/D2</f>
-        <v>11792444.555256065</v>
+        <v>11755579.292225201</v>
       </c>
       <c r="G142" s="11"/>
     </row>
@@ -29528,8 +29518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29731,11 +29721,11 @@
       </c>
       <c r="F6" s="65">
         <f>K23</f>
-        <v>171563165.78082192</v>
+        <v>171512547.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>1123011.7891781032</v>
+        <v>1173629.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -29855,11 +29845,11 @@
       </c>
       <c r="K9" s="46">
         <f>'مسکن ایلیا'!B139</f>
-        <v>4932691</v>
+        <v>4917073</v>
       </c>
       <c r="L9" s="3">
         <f>K9</f>
-        <v>4932691</v>
+        <v>4917073</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" ref="M9:M22" si="4">K9-L9</f>
@@ -30138,11 +30128,11 @@
         <v>469</v>
       </c>
       <c r="K16" s="46">
-        <v>75000</v>
+        <v>40000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>75000</v>
+        <v>40000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
@@ -30491,11 +30481,11 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>171563165.78082192</v>
+        <v>171512547.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>61062485.520547941</v>
+        <v>61011867.520547941</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
@@ -30543,11 +30533,11 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>99680974</v>
+        <v>99630356</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12</f>
-        <v>21007691</v>
+        <v>20957073</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17</f>
@@ -31818,12 +31808,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:G6">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G62">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finance file updated 20/4/1396 at 09:55
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="تیر 96" sheetId="23" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="635">
   <si>
     <t>18/1/95</t>
   </si>
@@ -1937,6 +1937,9 @@
   </si>
   <si>
     <t>طلب علی(500 خانه، 500 علیرضا، 150 ماجدی)</t>
+  </si>
+  <si>
+    <t>دستی برای دکتر رفتن دادم</t>
   </si>
 </sst>
 </file>
@@ -3703,9 +3706,11 @@
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D33" s="45">
-        <v>0</v>
-      </c>
-      <c r="E33" s="44"/>
+        <v>-25000</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>634</v>
+      </c>
       <c r="P33" t="s">
         <v>60</v>
       </c>
@@ -3760,7 +3765,7 @@
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <f>SUM(D30:D39)</f>
-        <v>8236102</v>
+        <v>8211102</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -23945,7 +23950,7 @@
   <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -24023,7 +24028,7 @@
       </c>
       <c r="E2" s="11">
         <f>D2+E3</f>
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="F2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -24031,7 +24036,7 @@
       </c>
       <c r="G2" s="11">
         <f>B2*(E2-F2)</f>
-        <v>10850000</v>
+        <v>11100000</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -24065,7 +24070,7 @@
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E67" si="0">D3+E4</f>
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F38" si="1">IF(B3&gt;0,1,0)</f>
@@ -24073,7 +24078,7 @@
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G23" si="2">B3*(E3-F3)</f>
-        <v>639000000</v>
+        <v>654000000</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="28"/>
@@ -24107,7 +24112,7 @@
       </c>
       <c r="E4" s="11">
         <f t="shared" si="0"/>
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" si="1"/>
@@ -24115,7 +24120,7 @@
       </c>
       <c r="G4" s="11">
         <f t="shared" si="2"/>
-        <v>636000000</v>
+        <v>651000000</v>
       </c>
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
@@ -24142,7 +24147,7 @@
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
@@ -24150,7 +24155,7 @@
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>3180000000</v>
+        <v>3255000000</v>
       </c>
       <c r="L5" t="s">
         <v>129</v>
@@ -24189,7 +24194,7 @@
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
@@ -24197,7 +24202,7 @@
       </c>
       <c r="G6" s="11">
         <f t="shared" si="2"/>
-        <v>633000000</v>
+        <v>648000000</v>
       </c>
       <c r="K6" t="s">
         <v>288</v>
@@ -24236,7 +24241,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
@@ -24244,7 +24249,7 @@
       </c>
       <c r="G7" s="11">
         <f t="shared" si="2"/>
-        <v>-633000000</v>
+        <v>-648000000</v>
       </c>
       <c r="K7" t="s">
         <v>289</v>
@@ -24286,7 +24291,7 @@
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
@@ -24294,7 +24299,7 @@
       </c>
       <c r="G8" s="11">
         <f t="shared" si="2"/>
-        <v>-42200000</v>
+        <v>-43200000</v>
       </c>
       <c r="K8" t="s">
         <v>290</v>
@@ -24336,7 +24341,7 @@
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
@@ -24344,7 +24349,7 @@
       </c>
       <c r="G9" s="11">
         <f>B9*(E9-F9)</f>
-        <v>630000000</v>
+        <v>645000000</v>
       </c>
       <c r="K9" t="s">
         <v>291</v>
@@ -24383,7 +24388,7 @@
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
@@ -24391,7 +24396,7 @@
       </c>
       <c r="G10" s="11">
         <f t="shared" si="2"/>
-        <v>627000000</v>
+        <v>642000000</v>
       </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
@@ -24418,7 +24423,7 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="1"/>
@@ -24426,7 +24431,7 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="2"/>
-        <v>5225000000</v>
+        <v>5350000000</v>
       </c>
       <c r="K11" t="s">
         <v>296</v>
@@ -24459,7 +24464,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="1"/>
@@ -24467,7 +24472,7 @@
       </c>
       <c r="G12" s="11">
         <f t="shared" si="2"/>
-        <v>205655980</v>
+        <v>210647630</v>
       </c>
       <c r="K12" t="s">
         <v>297</v>
@@ -24500,7 +24505,7 @@
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" si="1"/>
@@ -24508,7 +24513,7 @@
       </c>
       <c r="G13" s="11">
         <f t="shared" si="2"/>
-        <v>618000000</v>
+        <v>633000000</v>
       </c>
       <c r="Q13" s="27"/>
       <c r="R13" s="27"/>
@@ -24535,7 +24540,7 @@
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="1"/>
@@ -24543,7 +24548,7 @@
       </c>
       <c r="G14" s="11">
         <f t="shared" si="2"/>
-        <v>245365776</v>
+        <v>251321256</v>
       </c>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
@@ -24570,7 +24575,7 @@
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="1"/>
@@ -24578,7 +24583,7 @@
       </c>
       <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>388000000</v>
+        <v>398000000</v>
       </c>
       <c r="U15" s="27"/>
       <c r="V15" s="28"/>
@@ -24601,7 +24606,7 @@
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
@@ -24609,7 +24614,7 @@
       </c>
       <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>546000000</v>
+        <v>561000000</v>
       </c>
       <c r="U16" s="27"/>
       <c r="V16" s="28"/>
@@ -24632,7 +24637,7 @@
       </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="1"/>
@@ -24640,7 +24645,7 @@
       </c>
       <c r="G17" s="11">
         <f t="shared" si="2"/>
-        <v>543000000</v>
+        <v>558000000</v>
       </c>
       <c r="U17" s="27"/>
       <c r="V17" s="28"/>
@@ -24663,7 +24668,7 @@
       </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" si="1"/>
@@ -24671,7 +24676,7 @@
       </c>
       <c r="G18" s="11">
         <f t="shared" si="2"/>
-        <v>342000000</v>
+        <v>351500000</v>
       </c>
       <c r="U18" s="27"/>
       <c r="V18" s="28"/>
@@ -24696,7 +24701,7 @@
       </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="1"/>
@@ -24704,7 +24709,7 @@
       </c>
       <c r="G19" s="11">
         <f t="shared" si="2"/>
-        <v>132744645</v>
+        <v>136767210</v>
       </c>
       <c r="U19" s="27"/>
       <c r="V19" s="28"/>
@@ -24729,7 +24734,7 @@
       </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="1"/>
@@ -24737,7 +24742,7 @@
       </c>
       <c r="G20" s="11">
         <f t="shared" si="2"/>
-        <v>492000000</v>
+        <v>507000000</v>
       </c>
       <c r="U20" s="27"/>
       <c r="V20" s="28"/>
@@ -24762,7 +24767,7 @@
       </c>
       <c r="E21" s="11">
         <f>D21+E22</f>
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="1"/>
@@ -24770,7 +24775,7 @@
       </c>
       <c r="G21" s="11">
         <f t="shared" si="2"/>
-        <v>79000000</v>
+        <v>81500000</v>
       </c>
       <c r="U21" s="27"/>
       <c r="V21" s="28"/>
@@ -24795,7 +24800,7 @@
       </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" si="1"/>
@@ -24803,7 +24808,7 @@
       </c>
       <c r="G22" s="11">
         <f t="shared" si="2"/>
-        <v>-435000000</v>
+        <v>-450000000</v>
       </c>
       <c r="U22" s="27"/>
       <c r="V22" s="28"/>
@@ -24828,7 +24833,7 @@
       </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="1"/>
@@ -24836,7 +24841,7 @@
       </c>
       <c r="G23" s="11">
         <f t="shared" si="2"/>
-        <v>408000000</v>
+        <v>423000000</v>
       </c>
       <c r="U23" s="27"/>
       <c r="V23" s="28"/>
@@ -24861,7 +24866,7 @@
       </c>
       <c r="E24" s="11">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="1"/>
@@ -24869,7 +24874,7 @@
       </c>
       <c r="G24" s="11">
         <f>B24*(E24-F24)</f>
-        <v>85794648</v>
+        <v>88948863</v>
       </c>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -24894,7 +24899,7 @@
       </c>
       <c r="E25" s="11">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" si="1"/>
@@ -24902,7 +24907,7 @@
       </c>
       <c r="G25" s="11">
         <f t="shared" ref="G25:G30" si="3">B25*(E25-F25)</f>
-        <v>-432121500</v>
+        <v>-448126000</v>
       </c>
       <c r="U25" s="27"/>
       <c r="V25" s="27"/>
@@ -24927,7 +24932,7 @@
       </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" si="1"/>
@@ -24935,7 +24940,7 @@
       </c>
       <c r="G26" s="11">
         <f t="shared" si="3"/>
-        <v>-399119700</v>
+        <v>-414124200</v>
       </c>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
@@ -24960,7 +24965,7 @@
       </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="1"/>
@@ -24968,7 +24973,7 @@
       </c>
       <c r="G27" s="11">
         <f t="shared" si="3"/>
-        <v>130000000</v>
+        <v>135000000</v>
       </c>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
@@ -24993,7 +24998,7 @@
       </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" si="1"/>
@@ -25001,7 +25006,7 @@
       </c>
       <c r="G28" s="11">
         <f t="shared" si="3"/>
-        <v>780000000</v>
+        <v>810000000</v>
       </c>
       <c r="U28" s="27"/>
       <c r="V28" s="27"/>
@@ -25026,7 +25031,7 @@
       </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="1"/>
@@ -25034,7 +25039,7 @@
       </c>
       <c r="G29" s="11">
         <f t="shared" si="3"/>
-        <v>754000000</v>
+        <v>783000000</v>
       </c>
       <c r="U29" s="27"/>
       <c r="V29" s="30"/>
@@ -25059,7 +25064,7 @@
       </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="1"/>
@@ -25067,7 +25072,7 @@
       </c>
       <c r="G30" s="11">
         <f t="shared" si="3"/>
-        <v>-655000</v>
+        <v>-680000</v>
       </c>
       <c r="U30" s="27"/>
       <c r="V30" s="27"/>
@@ -25092,7 +25097,7 @@
       </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="1"/>
@@ -25100,7 +25105,7 @@
       </c>
       <c r="G31" s="11">
         <f>B31*(E31-F31)</f>
-        <v>-3380000000</v>
+        <v>-3510000000</v>
       </c>
       <c r="U31" s="27"/>
       <c r="V31" s="27"/>
@@ -25125,7 +25130,7 @@
       </c>
       <c r="E32" s="11">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" si="1"/>
@@ -25133,7 +25138,7 @@
       </c>
       <c r="G32" s="11">
         <f>B32*(E32-F32)</f>
-        <v>-3353600000</v>
+        <v>-3484600000</v>
       </c>
       <c r="U32" s="27"/>
       <c r="V32" s="27"/>
@@ -25158,7 +25163,7 @@
       </c>
       <c r="E33" s="11">
         <f t="shared" si="0"/>
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" si="1"/>
@@ -25166,7 +25171,7 @@
       </c>
       <c r="G33" s="11">
         <f>B33*(E33-F33)</f>
-        <v>35316540</v>
+        <v>36951565</v>
       </c>
       <c r="U33" s="27"/>
       <c r="V33" s="27"/>
@@ -25191,7 +25196,7 @@
       </c>
       <c r="E34" s="11">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" si="1"/>
@@ -25199,7 +25204,7 @@
       </c>
       <c r="G34" s="11">
         <f t="shared" ref="G34:G67" si="4">B34*(E34-F34)</f>
-        <v>2556000000</v>
+        <v>2698000000</v>
       </c>
       <c r="V34" s="27"/>
       <c r="W34" s="28"/>
@@ -25220,7 +25225,7 @@
       </c>
       <c r="E35" s="11">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" si="1"/>
@@ -25228,7 +25233,7 @@
       </c>
       <c r="G35" s="12">
         <f t="shared" si="4"/>
-        <v>990000000</v>
+        <v>1045000000</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -25246,7 +25251,7 @@
       </c>
       <c r="E36" s="11">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" si="1"/>
@@ -25254,7 +25259,7 @@
       </c>
       <c r="G36" s="11">
         <f t="shared" si="4"/>
-        <v>31402575</v>
+        <v>33496080</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -25272,7 +25277,7 @@
       </c>
       <c r="E37" s="11">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F37" s="11">
         <f t="shared" si="1"/>
@@ -25280,7 +25285,7 @@
       </c>
       <c r="G37" s="11">
         <f t="shared" si="4"/>
-        <v>-68400</v>
+        <v>-72900</v>
       </c>
       <c r="J37" s="67"/>
     </row>
@@ -25299,7 +25304,7 @@
       </c>
       <c r="E38" s="11">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F38" s="11">
         <f t="shared" si="1"/>
@@ -25307,7 +25312,7 @@
       </c>
       <c r="G38" s="12">
         <f t="shared" si="4"/>
-        <v>148000000</v>
+        <v>158000000</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -25327,7 +25332,7 @@
       </c>
       <c r="E39" s="11">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F39" s="11">
         <f>IF(B39&gt;0,1,0)</f>
@@ -25335,7 +25340,7 @@
       </c>
       <c r="G39" s="11">
         <f t="shared" si="4"/>
-        <v>148000000</v>
+        <v>158000000</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -25353,7 +25358,7 @@
       </c>
       <c r="E40" s="11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F40" s="11">
         <f>IF(B40&gt;0,1,0)</f>
@@ -25361,7 +25366,7 @@
       </c>
       <c r="G40" s="11">
         <f t="shared" si="4"/>
-        <v>-12200000</v>
+        <v>-13200000</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -25379,7 +25384,7 @@
       </c>
       <c r="E41" s="11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F41" s="11">
         <f>IF(B41&gt;0,1,0)</f>
@@ -25387,7 +25392,7 @@
       </c>
       <c r="G41" s="11">
         <f t="shared" si="4"/>
-        <v>-37820000</v>
+        <v>-40920000</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -25405,7 +25410,7 @@
       </c>
       <c r="E42" s="11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" ref="F42:F67" si="5">IF(B42&gt;0,1,0)</f>
@@ -25413,7 +25418,7 @@
       </c>
       <c r="G42" s="11">
         <f t="shared" si="4"/>
-        <v>-7320000</v>
+        <v>-7920000</v>
       </c>
       <c r="J42" s="7"/>
     </row>
@@ -25432,7 +25437,7 @@
       </c>
       <c r="E43" s="11">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="5"/>
@@ -25440,7 +25445,7 @@
       </c>
       <c r="G43" s="11">
         <f t="shared" si="4"/>
-        <v>37700000</v>
+        <v>40950000</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -25458,7 +25463,7 @@
       </c>
       <c r="E44" s="11">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F44" s="11">
         <f t="shared" si="5"/>
@@ -25466,7 +25471,7 @@
       </c>
       <c r="G44" s="11">
         <f t="shared" si="4"/>
-        <v>-295000</v>
+        <v>-320000</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -25484,7 +25489,7 @@
       </c>
       <c r="E45" s="11">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F45" s="11">
         <f t="shared" si="5"/>
@@ -25492,7 +25497,7 @@
       </c>
       <c r="G45" s="11">
         <f t="shared" si="4"/>
-        <v>1682000000</v>
+        <v>1827000000</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -25510,7 +25515,7 @@
       </c>
       <c r="E46" s="11">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F46" s="11">
         <f t="shared" si="5"/>
@@ -25518,7 +25523,7 @@
       </c>
       <c r="G46" s="11">
         <f t="shared" si="4"/>
-        <v>-11000000</v>
+        <v>-12000000</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -25536,7 +25541,7 @@
       </c>
       <c r="E47" s="11">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F47" s="11">
         <f t="shared" si="5"/>
@@ -25544,7 +25549,7 @@
       </c>
       <c r="G47" s="11">
         <f t="shared" si="4"/>
-        <v>-10400000</v>
+        <v>-11400000</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -25562,7 +25567,7 @@
       </c>
       <c r="E48" s="11">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="5"/>
@@ -25570,7 +25575,7 @@
       </c>
       <c r="G48" s="11">
         <f t="shared" si="4"/>
-        <v>-10200000</v>
+        <v>-11200000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -25588,7 +25593,7 @@
       </c>
       <c r="E49" s="11">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F49" s="11">
         <f t="shared" si="5"/>
@@ -25596,7 +25601,7 @@
       </c>
       <c r="G49" s="11">
         <f t="shared" si="4"/>
-        <v>135000000</v>
+        <v>150000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -25614,7 +25619,7 @@
       </c>
       <c r="E50" s="11">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" si="5"/>
@@ -25622,7 +25627,7 @@
       </c>
       <c r="G50" s="12">
         <f t="shared" si="4"/>
-        <v>135000000</v>
+        <v>150000000</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -25640,7 +25645,7 @@
       </c>
       <c r="E51" s="11">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" si="5"/>
@@ -25648,7 +25653,7 @@
       </c>
       <c r="G51" s="11">
         <f t="shared" si="4"/>
-        <v>33695068</v>
+        <v>37524053</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -25666,7 +25671,7 @@
       </c>
       <c r="E52" s="11">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" si="5"/>
@@ -25674,7 +25679,7 @@
       </c>
       <c r="G52" s="11">
         <f t="shared" si="4"/>
-        <v>-9000000</v>
+        <v>-10000000</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -25692,7 +25697,7 @@
       </c>
       <c r="E53" s="11">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F53" s="11">
         <f t="shared" si="5"/>
@@ -25700,7 +25705,7 @@
       </c>
       <c r="G53" s="11">
         <f t="shared" si="4"/>
-        <v>-15219000</v>
+        <v>-17221500</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -25718,7 +25723,7 @@
       </c>
       <c r="E54" s="11">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F54" s="11">
         <f t="shared" si="5"/>
@@ -25726,7 +25731,7 @@
       </c>
       <c r="G54" s="11">
         <f t="shared" si="4"/>
-        <v>-29014500</v>
+        <v>-34017000</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -25744,7 +25749,7 @@
       </c>
       <c r="E55" s="11">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F55" s="11">
         <f t="shared" si="5"/>
@@ -25752,7 +25757,7 @@
       </c>
       <c r="G55" s="11">
         <f t="shared" si="4"/>
-        <v>-920000000</v>
+        <v>-1120000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -25766,11 +25771,11 @@
         <v>612</v>
       </c>
       <c r="D56" s="11">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F56" s="11">
         <f t="shared" si="5"/>
@@ -25778,7 +25783,7 @@
       </c>
       <c r="G56" s="11">
         <f t="shared" si="4"/>
-        <v>11253476</v>
+        <v>15581736</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -25999,7 +26004,7 @@
       <c r="F68" s="11"/>
       <c r="G68" s="31">
         <f>SUM(G2:G67)</f>
-        <v>13535545608</v>
+        <v>13858286793</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -26033,7 +26038,7 @@
       <c r="F71" s="11"/>
       <c r="G71" s="3">
         <f>G68/E2</f>
-        <v>62089658.752293579</v>
+        <v>62144783.825112104</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -26067,7 +26072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G131" sqref="G131"/>
     </sheetView>
@@ -29527,8 +29532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29730,11 +29735,11 @@
       </c>
       <c r="F6" s="65">
         <f>K23</f>
-        <v>171504547.78082192</v>
+        <v>171453547.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>1181629.7891781032</v>
+        <v>1232629.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -30088,11 +30093,11 @@
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>-8250000</v>
+        <v>-8200000</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="4"/>
-        <v>8250000</v>
+        <v>8200000</v>
       </c>
       <c r="N15" s="27"/>
       <c r="O15" s="11"/>
@@ -30136,11 +30141,11 @@
         <v>468</v>
       </c>
       <c r="K16" s="46">
-        <v>82000</v>
+        <v>31000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>82000</v>
+        <v>31000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
@@ -30489,15 +30494,15 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>171504547.78082192</v>
+        <v>171453547.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>61003867.520547941</v>
+        <v>61002867.520547941</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
-        <v>110500680.26027396</v>
+        <v>110450680.26027396</v>
       </c>
       <c r="N23" s="27"/>
       <c r="O23" s="11" t="s">
@@ -30541,11 +30546,11 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>99472356</v>
+        <v>99421356</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12</f>
-        <v>20799073</v>
+        <v>20748073</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17</f>
@@ -32748,10 +32753,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32767,7 +32772,7 @@
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>180</v>
       </c>
@@ -32784,7 +32789,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -32806,7 +32811,7 @@
         <v>2902500000</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -32828,7 +32833,7 @@
         <v>1212500000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -32850,7 +32855,7 @@
         <v>18500000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -32872,7 +32877,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -32894,7 +32899,7 @@
         <v>477000000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>473</v>
       </c>
@@ -32916,7 +32921,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="18">
         <f t="shared" si="1"/>
@@ -32928,7 +32933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="18">
         <f t="shared" si="1"/>
@@ -32940,7 +32945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18">
         <f t="shared" si="1"/>
@@ -32952,7 +32957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="18">
         <f t="shared" si="1"/>
@@ -32961,7 +32966,7 @@
       <c r="D11" s="18"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18">
         <f t="shared" si="1"/>
@@ -32982,7 +32987,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18">
         <f t="shared" si="1"/>
@@ -33007,8 +33012,12 @@
         <f>$R$13*$O$13/O13</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <f>O13*R13*30.5</f>
+        <v>13176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="18">
         <f t="shared" si="1"/>
@@ -33033,8 +33042,12 @@
         <f>$R$13*$O$13/O14</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <f t="shared" ref="U14:U19" si="4">O14*R14*30.5</f>
+        <v>13542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="18">
         <f t="shared" si="1"/>
@@ -33056,11 +33069,15 @@
         <v>38</v>
       </c>
       <c r="S15">
-        <f t="shared" ref="S15:S19" si="4">$R$13*$O$13/O15</f>
+        <f t="shared" ref="S15:S19" si="5">$R$13*$O$13/O15</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <f t="shared" si="4"/>
+        <v>13908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
       <c r="C16" s="18">
         <f t="shared" si="1"/>
@@ -33082,11 +33099,15 @@
         <v>20.5</v>
       </c>
       <c r="S16">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+        <v>11254.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="18">
         <f t="shared" si="1"/>
@@ -33108,11 +33129,15 @@
         <v>14.666666666666666</v>
       </c>
       <c r="S17">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+        <v>10736</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="C18" s="18">
         <f t="shared" si="1"/>
@@ -33134,11 +33159,15 @@
         <v>11.75</v>
       </c>
       <c r="S18">
+        <f t="shared" si="5"/>
+        <v>14.4</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="4"/>
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+        <v>10751.25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="18">
         <f t="shared" si="1"/>
@@ -33160,11 +33189,15 @@
         <v>10</v>
       </c>
       <c r="S19">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+        <v>10980</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F20" s="18">
         <f>SUM(F2:F15)</f>
         <v>4619500000</v>
@@ -33179,12 +33212,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="P21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F22" s="18">
         <f>F20*H20/36500</f>
         <v>3037479.4520547944</v>
@@ -33193,7 +33226,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G28" s="11" t="s">
         <v>598</v>
       </c>
@@ -33207,7 +33240,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G29" s="11">
         <f>$I$41-I29</f>
         <v>53500</v>
@@ -33222,9 +33255,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G30" s="11">
-        <f t="shared" ref="G30:G35" si="5">$I$41-I30</f>
+        <f t="shared" ref="G30:G35" si="6">$I$41-I30</f>
         <v>18500</v>
       </c>
       <c r="H30" s="11" t="s">
@@ -33237,9 +33270,9 @@
         <v>589</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G31" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="H31" s="11" t="s">
@@ -33252,9 +33285,9 @@
         <v>495</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G32" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33500</v>
       </c>
       <c r="H32" s="68">
@@ -33269,7 +33302,7 @@
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G33" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -33284,7 +33317,7 @@
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G34" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="H34" s="11" t="s">
@@ -33299,7 +33332,7 @@
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G35" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="H35" s="11" t="s">

</xml_diff>

<commit_message>
finance file updated 20/4/1396 at 20:46
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="تیر 96" sheetId="23" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="637">
   <si>
     <t>18/1/95</t>
   </si>
@@ -1940,6 +1940,12 @@
   </si>
   <si>
     <t>دستی برای دکتر رفتن دادم</t>
+  </si>
+  <si>
+    <t>20/4/1396</t>
+  </si>
+  <si>
+    <t>از عابربانک گرفتم، 150 بابت بخشی از 30 کیلو برنج</t>
   </si>
 </sst>
 </file>
@@ -26072,9 +26078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G131" sqref="G131"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26124,7 +26130,7 @@
       </c>
       <c r="D2" s="11">
         <f>D3+C2</f>
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -26132,7 +26138,7 @@
       </c>
       <c r="F2" s="11">
         <f>B2*(D2-E2)</f>
-        <v>36069100</v>
+        <v>36165800</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>1</v>
@@ -26150,7 +26156,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D66" si="0">D4+C3</f>
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E66" si="1">IF(B3&gt;0,1,0)</f>
@@ -26158,7 +26164,7 @@
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F66" si="2">B3*(D3-E3)</f>
-        <v>1113000000</v>
+        <v>1116000000</v>
       </c>
       <c r="G3" s="11"/>
     </row>
@@ -26174,7 +26180,7 @@
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" si="1"/>
@@ -26182,7 +26188,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" si="2"/>
-        <v>-73800000</v>
+        <v>-74000000</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -26198,7 +26204,7 @@
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="1"/>
@@ -26206,7 +26212,7 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="2"/>
-        <v>-36700000</v>
+        <v>-36800000</v>
       </c>
       <c r="G5" s="11"/>
     </row>
@@ -26222,7 +26228,7 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
@@ -26230,7 +26236,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="2"/>
-        <v>-20130000</v>
+        <v>-20185000</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -26246,7 +26252,7 @@
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
@@ -26254,7 +26260,7 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="2"/>
-        <v>-73000000</v>
+        <v>-73200000</v>
       </c>
       <c r="G7" s="11"/>
     </row>
@@ -26270,7 +26276,7 @@
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
@@ -26278,7 +26284,7 @@
       </c>
       <c r="F8" s="11">
         <f t="shared" si="2"/>
-        <v>-72200000</v>
+        <v>-72400000</v>
       </c>
       <c r="G8" s="11"/>
     </row>
@@ -26294,7 +26300,7 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
@@ -26302,7 +26308,7 @@
       </c>
       <c r="F9" s="11">
         <f t="shared" si="2"/>
-        <v>-334576000</v>
+        <v>-335526500</v>
       </c>
       <c r="G9" s="11"/>
     </row>
@@ -26318,7 +26324,7 @@
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
@@ -26326,7 +26332,7 @@
       </c>
       <c r="F10" s="11">
         <f t="shared" si="2"/>
-        <v>700000000</v>
+        <v>702000000</v>
       </c>
       <c r="G10" s="11"/>
     </row>
@@ -26342,7 +26348,7 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
@@ -26350,7 +26356,7 @@
       </c>
       <c r="F11" s="11">
         <f t="shared" si="2"/>
-        <v>-371685000</v>
+        <v>-372750000</v>
       </c>
       <c r="G11" s="11"/>
     </row>
@@ -26366,7 +26372,7 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" si="0"/>
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
@@ -26374,7 +26380,7 @@
       </c>
       <c r="F12" s="11">
         <f t="shared" si="2"/>
-        <v>-15570000</v>
+        <v>-15615000</v>
       </c>
       <c r="G12" s="11"/>
     </row>
@@ -26390,7 +26396,7 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
@@ -26398,7 +26404,7 @@
       </c>
       <c r="F13" s="11">
         <f t="shared" si="2"/>
-        <v>-690241500</v>
+        <v>-692242200</v>
       </c>
       <c r="G13" s="11"/>
     </row>
@@ -26414,7 +26420,7 @@
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
@@ -26422,7 +26428,7 @@
       </c>
       <c r="F14" s="11">
         <f t="shared" si="2"/>
-        <v>-68200000</v>
+        <v>-68400000</v>
       </c>
       <c r="G14" s="11"/>
     </row>
@@ -26438,7 +26444,7 @@
       </c>
       <c r="D15" s="11">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="1"/>
@@ -26446,7 +26452,7 @@
       </c>
       <c r="F15" s="11">
         <f t="shared" si="2"/>
-        <v>676000000</v>
+        <v>678000000</v>
       </c>
       <c r="G15" s="11"/>
     </row>
@@ -26462,7 +26468,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
@@ -26470,7 +26476,7 @@
       </c>
       <c r="F16" s="11">
         <f t="shared" si="2"/>
-        <v>676000000</v>
+        <v>678000000</v>
       </c>
       <c r="G16" s="11"/>
     </row>
@@ -26486,7 +26492,7 @@
       </c>
       <c r="D17" s="11">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="1"/>
@@ -26494,7 +26500,7 @@
       </c>
       <c r="F17" s="11">
         <f t="shared" si="2"/>
-        <v>405600000</v>
+        <v>406800000</v>
       </c>
       <c r="G17" s="11"/>
     </row>
@@ -26510,7 +26516,7 @@
       </c>
       <c r="D18" s="11">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="1"/>
@@ -26518,7 +26524,7 @@
       </c>
       <c r="F18" s="11">
         <f t="shared" si="2"/>
-        <v>338000000</v>
+        <v>339000000</v>
       </c>
       <c r="G18" s="11"/>
     </row>
@@ -26534,7 +26540,7 @@
       </c>
       <c r="D19" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="1"/>
@@ -26542,7 +26548,7 @@
       </c>
       <c r="F19" s="11">
         <f t="shared" si="2"/>
-        <v>1011000000</v>
+        <v>1014000000</v>
       </c>
       <c r="G19" s="11"/>
       <c r="L19" t="s">
@@ -26561,7 +26567,7 @@
       </c>
       <c r="D20" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="1"/>
@@ -26569,7 +26575,7 @@
       </c>
       <c r="F20" s="11">
         <f t="shared" si="2"/>
-        <v>-146252600</v>
+        <v>-146685300</v>
       </c>
       <c r="G20" s="11"/>
     </row>
@@ -26585,7 +26591,7 @@
       </c>
       <c r="D21" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="1"/>
@@ -26593,7 +26599,7 @@
       </c>
       <c r="F21" s="11">
         <f t="shared" si="2"/>
-        <v>-146252600</v>
+        <v>-146685300</v>
       </c>
       <c r="G21" s="11"/>
     </row>
@@ -26609,7 +26615,7 @@
       </c>
       <c r="D22" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="1"/>
@@ -26617,7 +26623,7 @@
       </c>
       <c r="F22" s="11">
         <f t="shared" si="2"/>
-        <v>-146252600</v>
+        <v>-146685300</v>
       </c>
       <c r="G22" s="11"/>
     </row>
@@ -26633,7 +26639,7 @@
       </c>
       <c r="D23" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="1"/>
@@ -26641,7 +26647,7 @@
       </c>
       <c r="F23" s="11">
         <f t="shared" si="2"/>
-        <v>-146252600</v>
+        <v>-146685300</v>
       </c>
       <c r="G23" s="11"/>
     </row>
@@ -26657,7 +26663,7 @@
       </c>
       <c r="D24" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="1"/>
@@ -26665,7 +26671,7 @@
       </c>
       <c r="F24" s="11">
         <f t="shared" si="2"/>
-        <v>-146252600</v>
+        <v>-146685300</v>
       </c>
       <c r="G24" s="11"/>
     </row>
@@ -26681,7 +26687,7 @@
       </c>
       <c r="D25" s="11">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="1"/>
@@ -26689,7 +26695,7 @@
       </c>
       <c r="F25" s="11">
         <f t="shared" si="2"/>
-        <v>-67600000</v>
+        <v>-67800000</v>
       </c>
       <c r="G25" s="11"/>
     </row>
@@ -26705,7 +26711,7 @@
       </c>
       <c r="D26" s="11">
         <f t="shared" si="0"/>
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="1"/>
@@ -26713,7 +26719,7 @@
       </c>
       <c r="F26" s="11">
         <f t="shared" si="2"/>
-        <v>1008000000</v>
+        <v>1011000000</v>
       </c>
       <c r="G26" s="11"/>
     </row>
@@ -26729,7 +26735,7 @@
       </c>
       <c r="D27" s="11">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="1"/>
@@ -26737,7 +26743,7 @@
       </c>
       <c r="F27" s="11">
         <f t="shared" si="2"/>
-        <v>-67000000</v>
+        <v>-67200000</v>
       </c>
       <c r="G27" s="11"/>
     </row>
@@ -26753,7 +26759,7 @@
       </c>
       <c r="D28" s="11">
         <f t="shared" si="0"/>
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E28" s="11">
         <f t="shared" si="1"/>
@@ -26761,7 +26767,7 @@
       </c>
       <c r="F28" s="11">
         <f t="shared" si="2"/>
-        <v>666000000</v>
+        <v>668000000</v>
       </c>
       <c r="G28" s="11"/>
     </row>
@@ -26777,7 +26783,7 @@
       </c>
       <c r="D29" s="11">
         <f t="shared" si="0"/>
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E29" s="11">
         <f t="shared" si="1"/>
@@ -26785,7 +26791,7 @@
       </c>
       <c r="F29" s="11">
         <f t="shared" si="2"/>
-        <v>-2331266400</v>
+        <v>-2338267200</v>
       </c>
       <c r="G29" s="11"/>
     </row>
@@ -26801,7 +26807,7 @@
       </c>
       <c r="D30" s="11">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" si="1"/>
@@ -26809,7 +26815,7 @@
       </c>
       <c r="F30" s="11">
         <f t="shared" si="2"/>
-        <v>-996298800</v>
+        <v>-999299700</v>
       </c>
       <c r="G30" s="11"/>
     </row>
@@ -26825,7 +26831,7 @@
       </c>
       <c r="D31" s="11">
         <f t="shared" si="0"/>
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="1"/>
@@ -26833,7 +26839,7 @@
       </c>
       <c r="F31" s="11">
         <f t="shared" si="2"/>
-        <v>-561342900</v>
+        <v>-563038800</v>
       </c>
       <c r="G31" s="11"/>
     </row>
@@ -26849,7 +26855,7 @@
       </c>
       <c r="D32" s="11">
         <f t="shared" si="0"/>
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="1"/>
@@ -26857,7 +26863,7 @@
       </c>
       <c r="F32" s="11">
         <f t="shared" si="2"/>
-        <v>325136100</v>
+        <v>326130400</v>
       </c>
       <c r="G32" s="11"/>
     </row>
@@ -26873,7 +26879,7 @@
       </c>
       <c r="D33" s="11">
         <f t="shared" si="0"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="1"/>
@@ -26881,7 +26887,7 @@
       </c>
       <c r="F33" s="11">
         <f t="shared" si="2"/>
-        <v>11299302</v>
+        <v>11334393</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>382</v>
@@ -26899,7 +26905,7 @@
       </c>
       <c r="D34" s="11">
         <f t="shared" si="0"/>
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E34" s="11">
         <f t="shared" si="1"/>
@@ -26907,7 +26913,7 @@
       </c>
       <c r="F34" s="11">
         <f t="shared" si="2"/>
-        <v>-273700000</v>
+        <v>-274550000</v>
       </c>
       <c r="G34" s="11"/>
     </row>
@@ -26923,7 +26929,7 @@
       </c>
       <c r="D35" s="11">
         <f t="shared" si="0"/>
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="1"/>
@@ -26931,7 +26937,7 @@
       </c>
       <c r="F35" s="11">
         <f t="shared" si="2"/>
-        <v>-59817000</v>
+        <v>-60007500</v>
       </c>
       <c r="G35" s="11"/>
     </row>
@@ -26947,7 +26953,7 @@
       </c>
       <c r="D36" s="11">
         <f t="shared" si="0"/>
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E36" s="11">
         <f t="shared" si="1"/>
@@ -26955,7 +26961,7 @@
       </c>
       <c r="F36" s="11">
         <f t="shared" si="2"/>
-        <v>62400000</v>
+        <v>62600000</v>
       </c>
       <c r="G36" s="11"/>
     </row>
@@ -26971,7 +26977,7 @@
       </c>
       <c r="D37" s="11">
         <f t="shared" si="0"/>
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E37" s="11">
         <f t="shared" si="1"/>
@@ -26979,7 +26985,7 @@
       </c>
       <c r="F37" s="11">
         <f t="shared" si="2"/>
-        <v>-62600000</v>
+        <v>-62800000</v>
       </c>
       <c r="G37" s="11"/>
     </row>
@@ -26995,7 +27001,7 @@
       </c>
       <c r="D38" s="11">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E38" s="11">
         <f t="shared" si="1"/>
@@ -27003,7 +27009,7 @@
       </c>
       <c r="F38" s="11">
         <f t="shared" si="2"/>
-        <v>87233740</v>
+        <v>87534546</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>402</v>
@@ -27021,7 +27027,7 @@
       </c>
       <c r="D39" s="11">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E39" s="11">
         <f t="shared" si="1"/>
@@ -27029,7 +27035,7 @@
       </c>
       <c r="F39" s="11">
         <f t="shared" si="2"/>
-        <v>-27550000</v>
+        <v>-27645000</v>
       </c>
       <c r="G39" s="11"/>
     </row>
@@ -27045,7 +27051,7 @@
       </c>
       <c r="D40" s="11">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="1"/>
@@ -27053,7 +27059,7 @@
       </c>
       <c r="F40" s="11">
         <f t="shared" si="2"/>
-        <v>-25549870</v>
+        <v>-25637973</v>
       </c>
       <c r="G40" s="11"/>
     </row>
@@ -27069,7 +27075,7 @@
       </c>
       <c r="D41" s="11">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" si="1"/>
@@ -27077,7 +27083,7 @@
       </c>
       <c r="F41" s="11">
         <f t="shared" si="2"/>
-        <v>-34200000</v>
+        <v>-34320000</v>
       </c>
       <c r="G41" s="11"/>
     </row>
@@ -27093,7 +27099,7 @@
       </c>
       <c r="D42" s="11">
         <f t="shared" si="0"/>
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E42" s="11">
         <f t="shared" si="1"/>
@@ -27101,7 +27107,7 @@
       </c>
       <c r="F42" s="11">
         <f t="shared" si="2"/>
-        <v>262053448</v>
+        <v>263053652</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>403</v>
@@ -27119,7 +27125,7 @@
       </c>
       <c r="D43" s="11">
         <f t="shared" si="0"/>
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="1"/>
@@ -27127,7 +27133,7 @@
       </c>
       <c r="F43" s="11">
         <f t="shared" si="2"/>
-        <v>-20720000</v>
+        <v>-20800000</v>
       </c>
       <c r="G43" s="11"/>
     </row>
@@ -27143,7 +27149,7 @@
       </c>
       <c r="D44" s="11">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="1"/>
@@ -27151,7 +27157,7 @@
       </c>
       <c r="F44" s="11">
         <f t="shared" si="2"/>
-        <v>-53812395</v>
+        <v>-54023424</v>
       </c>
       <c r="G44" s="11"/>
     </row>
@@ -27167,7 +27173,7 @@
       </c>
       <c r="D45" s="11">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="1"/>
@@ -27175,7 +27181,7 @@
       </c>
       <c r="F45" s="11">
         <f t="shared" si="2"/>
-        <v>-50800000</v>
+        <v>-51000000</v>
       </c>
       <c r="G45" s="11"/>
     </row>
@@ -27191,7 +27197,7 @@
       </c>
       <c r="D46" s="11">
         <f t="shared" si="0"/>
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="1"/>
@@ -27199,7 +27205,7 @@
       </c>
       <c r="F46" s="11">
         <f t="shared" si="2"/>
-        <v>-24035000</v>
+        <v>-24130000</v>
       </c>
       <c r="G46" s="11"/>
     </row>
@@ -27215,7 +27221,7 @@
       </c>
       <c r="D47" s="11">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="1"/>
@@ -27223,7 +27229,7 @@
       </c>
       <c r="F47" s="11">
         <f t="shared" si="2"/>
-        <v>-11295000</v>
+        <v>-11340000</v>
       </c>
       <c r="G47" s="11"/>
     </row>
@@ -27239,7 +27245,7 @@
       </c>
       <c r="D48" s="11">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="1"/>
@@ -27247,7 +27253,7 @@
       </c>
       <c r="F48" s="11">
         <f t="shared" si="2"/>
-        <v>-16109180</v>
+        <v>-16173360</v>
       </c>
       <c r="G48" s="11"/>
     </row>
@@ -27263,7 +27269,7 @@
       </c>
       <c r="D49" s="11">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E49" s="11">
         <f t="shared" si="1"/>
@@ -27271,7 +27277,7 @@
       </c>
       <c r="F49" s="11">
         <f t="shared" si="2"/>
-        <v>-6816032</v>
+        <v>-6843516</v>
       </c>
       <c r="G49" s="11"/>
     </row>
@@ -27287,7 +27293,7 @@
       </c>
       <c r="D50" s="11">
         <f t="shared" si="0"/>
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E50" s="11">
         <f t="shared" si="1"/>
@@ -27295,7 +27301,7 @@
       </c>
       <c r="F50" s="11">
         <f t="shared" si="2"/>
-        <v>-34827000</v>
+        <v>-34968000</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -27311,7 +27317,7 @@
       </c>
       <c r="D51" s="11">
         <f t="shared" si="0"/>
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E51" s="11">
         <f t="shared" si="1"/>
@@ -27319,7 +27325,7 @@
       </c>
       <c r="F51" s="11">
         <f t="shared" si="2"/>
-        <v>-6606262</v>
+        <v>-6633008</v>
       </c>
       <c r="G51" s="11"/>
     </row>
@@ -27335,7 +27341,7 @@
       </c>
       <c r="D52" s="11">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E52" s="11">
         <f t="shared" si="1"/>
@@ -27343,7 +27349,7 @@
       </c>
       <c r="F52" s="11">
         <f t="shared" si="2"/>
-        <v>-13111800</v>
+        <v>-13165100</v>
       </c>
       <c r="G52" s="11"/>
     </row>
@@ -27359,7 +27365,7 @@
       </c>
       <c r="D53" s="11">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E53" s="11">
         <f t="shared" si="1"/>
@@ -27367,7 +27373,7 @@
       </c>
       <c r="F53" s="11">
         <f t="shared" si="2"/>
-        <v>244000000</v>
+        <v>245000000</v>
       </c>
       <c r="G53" s="11"/>
     </row>
@@ -27383,7 +27389,7 @@
       </c>
       <c r="D54" s="11">
         <f t="shared" si="0"/>
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E54" s="11">
         <f t="shared" si="1"/>
@@ -27391,7 +27397,7 @@
       </c>
       <c r="F54" s="11">
         <f t="shared" si="2"/>
-        <v>-5019000</v>
+        <v>-5040000</v>
       </c>
       <c r="G54" s="11"/>
     </row>
@@ -27407,7 +27413,7 @@
       </c>
       <c r="D55" s="11">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E55" s="11">
         <f t="shared" si="1"/>
@@ -27415,7 +27421,7 @@
       </c>
       <c r="F55" s="11">
         <f t="shared" si="2"/>
-        <v>-233359000</v>
+        <v>-234339500</v>
       </c>
       <c r="G55" s="11"/>
     </row>
@@ -27431,7 +27437,7 @@
       </c>
       <c r="D56" s="11">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="1"/>
@@ -27439,7 +27445,7 @@
       </c>
       <c r="F56" s="11">
         <f t="shared" si="2"/>
-        <v>-10710000</v>
+        <v>-10755000</v>
       </c>
       <c r="G56" s="11"/>
     </row>
@@ -27455,7 +27461,7 @@
       </c>
       <c r="D57" s="11">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E57" s="11">
         <f t="shared" si="1"/>
@@ -27463,7 +27469,7 @@
       </c>
       <c r="F57" s="11">
         <f t="shared" si="2"/>
-        <v>673162336</v>
+        <v>676167525</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>404</v>
@@ -27481,7 +27487,7 @@
       </c>
       <c r="D58" s="11">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E58" s="11">
         <f t="shared" si="1"/>
@@ -27489,7 +27495,7 @@
       </c>
       <c r="F58" s="11">
         <f t="shared" si="2"/>
-        <v>448000000</v>
+        <v>450000000</v>
       </c>
       <c r="G58" s="11"/>
     </row>
@@ -27505,7 +27511,7 @@
       </c>
       <c r="D59" s="11">
         <f t="shared" si="0"/>
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E59" s="11">
         <f t="shared" si="1"/>
@@ -27513,7 +27519,7 @@
       </c>
       <c r="F59" s="11">
         <f t="shared" si="2"/>
-        <v>446000000</v>
+        <v>448000000</v>
       </c>
       <c r="G59" s="11"/>
     </row>
@@ -27529,7 +27535,7 @@
       </c>
       <c r="D60" s="11">
         <f t="shared" si="0"/>
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E60" s="11">
         <f t="shared" si="1"/>
@@ -27537,7 +27543,7 @@
       </c>
       <c r="F60" s="11">
         <f t="shared" si="2"/>
-        <v>-1568336000</v>
+        <v>-1575337500</v>
       </c>
       <c r="G60" s="11"/>
     </row>
@@ -27553,7 +27559,7 @@
       </c>
       <c r="D61" s="11">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E61" s="11">
         <f t="shared" si="1"/>
@@ -27561,7 +27567,7 @@
       </c>
       <c r="F61" s="11">
         <f t="shared" si="2"/>
-        <v>597000000</v>
+        <v>600000000</v>
       </c>
       <c r="G61" s="11"/>
     </row>
@@ -27577,7 +27583,7 @@
       </c>
       <c r="D62" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E62" s="11">
         <f t="shared" si="1"/>
@@ -27585,7 +27591,7 @@
       </c>
       <c r="F62" s="11">
         <f t="shared" si="2"/>
-        <v>-5394691</v>
+        <v>-5421800</v>
       </c>
       <c r="G62" s="11"/>
     </row>
@@ -27601,7 +27607,7 @@
       </c>
       <c r="D63" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E63" s="11">
         <f t="shared" si="1"/>
@@ -27609,7 +27615,7 @@
       </c>
       <c r="F63" s="11">
         <f t="shared" si="2"/>
-        <v>-6564811</v>
+        <v>-6597800</v>
       </c>
       <c r="G63" s="11"/>
     </row>
@@ -27625,7 +27631,7 @@
       </c>
       <c r="D64" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E64" s="11">
         <f t="shared" si="1"/>
@@ -27633,7 +27639,7 @@
       </c>
       <c r="F64" s="11">
         <f t="shared" si="2"/>
-        <v>594000000</v>
+        <v>597000000</v>
       </c>
       <c r="G64" s="11"/>
     </row>
@@ -27649,7 +27655,7 @@
       </c>
       <c r="D65" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E65" s="11">
         <f t="shared" si="1"/>
@@ -27657,7 +27663,7 @@
       </c>
       <c r="F65" s="11">
         <f t="shared" si="2"/>
-        <v>588060000</v>
+        <v>591030000</v>
       </c>
       <c r="G65" s="11"/>
     </row>
@@ -27673,7 +27679,7 @@
       </c>
       <c r="D66" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E66" s="11">
         <f t="shared" si="1"/>
@@ -27681,7 +27687,7 @@
       </c>
       <c r="F66" s="11">
         <f t="shared" si="2"/>
-        <v>198000000</v>
+        <v>199000000</v>
       </c>
       <c r="G66" s="11"/>
     </row>
@@ -27697,7 +27703,7 @@
       </c>
       <c r="D67" s="11">
         <f t="shared" ref="D67:D130" si="3">D68+C67</f>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E67" s="11">
         <f t="shared" ref="E67:E130" si="4">IF(B67&gt;0,1,0)</f>
@@ -27705,7 +27711,7 @@
       </c>
       <c r="F67" s="11">
         <f t="shared" ref="F67:F137" si="5">B67*(D67-E67)</f>
-        <v>5940000</v>
+        <v>5970000</v>
       </c>
       <c r="G67" s="11"/>
     </row>
@@ -27721,7 +27727,7 @@
       </c>
       <c r="D68" s="11">
         <f t="shared" si="3"/>
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E68" s="11">
         <f t="shared" si="4"/>
@@ -27729,7 +27735,7 @@
       </c>
       <c r="F68" s="11">
         <f t="shared" si="5"/>
-        <v>5910000000</v>
+        <v>5940000000</v>
       </c>
       <c r="G68" s="11"/>
     </row>
@@ -27745,7 +27751,7 @@
       </c>
       <c r="D69" s="11">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E69" s="11">
         <f t="shared" si="4"/>
@@ -27753,7 +27759,7 @@
       </c>
       <c r="F69" s="11">
         <f t="shared" si="5"/>
-        <v>-39400000</v>
+        <v>-39600000</v>
       </c>
       <c r="G69" s="11"/>
     </row>
@@ -27769,7 +27775,7 @@
       </c>
       <c r="D70" s="11">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E70" s="11">
         <f t="shared" si="4"/>
@@ -27777,7 +27783,7 @@
       </c>
       <c r="F70" s="11">
         <f t="shared" si="5"/>
-        <v>274400000</v>
+        <v>275800000</v>
       </c>
       <c r="G70" s="11"/>
     </row>
@@ -27793,7 +27799,7 @@
       </c>
       <c r="D71" s="11">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E71" s="11">
         <f t="shared" si="4"/>
@@ -27801,7 +27807,7 @@
       </c>
       <c r="F71" s="11">
         <f t="shared" si="5"/>
-        <v>509600000</v>
+        <v>512200000</v>
       </c>
       <c r="G71" s="11"/>
     </row>
@@ -27817,7 +27823,7 @@
       </c>
       <c r="D72" s="11">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E72" s="11">
         <f t="shared" si="4"/>
@@ -27825,7 +27831,7 @@
       </c>
       <c r="F72" s="11">
         <f t="shared" si="5"/>
-        <v>-197000000</v>
+        <v>-198000000</v>
       </c>
       <c r="G72" s="11"/>
     </row>
@@ -27841,7 +27847,7 @@
       </c>
       <c r="D73" s="11">
         <f t="shared" si="3"/>
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E73" s="11">
         <f t="shared" si="4"/>
@@ -27849,7 +27855,7 @@
       </c>
       <c r="F73" s="11">
         <f t="shared" si="5"/>
-        <v>2910000000</v>
+        <v>2925000000</v>
       </c>
       <c r="G73" s="11"/>
     </row>
@@ -27865,7 +27871,7 @@
       </c>
       <c r="D74" s="11">
         <f t="shared" si="3"/>
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E74" s="11">
         <f t="shared" si="4"/>
@@ -27873,7 +27879,7 @@
       </c>
       <c r="F74" s="11">
         <f t="shared" si="5"/>
-        <v>-2850798000</v>
+        <v>-2865802200</v>
       </c>
       <c r="G74" s="11"/>
     </row>
@@ -27889,7 +27895,7 @@
       </c>
       <c r="D75" s="11">
         <f t="shared" si="3"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E75" s="11">
         <f t="shared" si="4"/>
@@ -27897,7 +27903,7 @@
       </c>
       <c r="F75" s="11">
         <f t="shared" si="5"/>
-        <v>-564000000</v>
+        <v>-567000000</v>
       </c>
       <c r="G75" s="11"/>
     </row>
@@ -27913,7 +27919,7 @@
       </c>
       <c r="D76" s="11">
         <f t="shared" si="3"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E76" s="11">
         <f t="shared" si="4"/>
@@ -27921,7 +27927,7 @@
       </c>
       <c r="F76" s="11">
         <f t="shared" si="5"/>
-        <v>-37600000</v>
+        <v>-37800000</v>
       </c>
       <c r="G76" s="11"/>
     </row>
@@ -27937,7 +27943,7 @@
       </c>
       <c r="D77" s="11">
         <f t="shared" si="3"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E77" s="11">
         <f t="shared" si="4"/>
@@ -27945,7 +27951,7 @@
       </c>
       <c r="F77" s="11">
         <f t="shared" si="5"/>
-        <v>-2256564000</v>
+        <v>-2268567000</v>
       </c>
       <c r="G77" s="11"/>
     </row>
@@ -27961,7 +27967,7 @@
       </c>
       <c r="D78" s="11">
         <f t="shared" si="3"/>
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E78" s="11">
         <f t="shared" si="4"/>
@@ -27969,7 +27975,7 @@
       </c>
       <c r="F78" s="11">
         <f t="shared" si="5"/>
-        <v>-552165600</v>
+        <v>-555166500</v>
       </c>
       <c r="G78" s="11"/>
     </row>
@@ -27985,7 +27991,7 @@
       </c>
       <c r="D79" s="11">
         <f t="shared" si="3"/>
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E79" s="11">
         <f t="shared" si="4"/>
@@ -27993,7 +27999,7 @@
       </c>
       <c r="F79" s="11">
         <f t="shared" si="5"/>
-        <v>4094000000</v>
+        <v>4117000000</v>
       </c>
       <c r="G79" s="11"/>
     </row>
@@ -28009,7 +28015,7 @@
       </c>
       <c r="D80" s="11">
         <f t="shared" si="3"/>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E80" s="11">
         <f t="shared" si="4"/>
@@ -28017,7 +28023,7 @@
       </c>
       <c r="F80" s="11">
         <f t="shared" si="5"/>
-        <v>-104487000</v>
+        <v>-105087500</v>
       </c>
       <c r="G80" s="11"/>
     </row>
@@ -28033,7 +28039,7 @@
       </c>
       <c r="D81" s="11">
         <f t="shared" si="3"/>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E81" s="11">
         <f t="shared" si="4"/>
@@ -28041,7 +28047,7 @@
       </c>
       <c r="F81" s="11">
         <f t="shared" si="5"/>
-        <v>-34800000</v>
+        <v>-35000000</v>
       </c>
       <c r="G81" s="11"/>
     </row>
@@ -28057,7 +28063,7 @@
       </c>
       <c r="D82" s="11">
         <f t="shared" si="3"/>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E82" s="11">
         <f t="shared" si="4"/>
@@ -28065,7 +28071,7 @@
       </c>
       <c r="F82" s="11">
         <f t="shared" si="5"/>
-        <v>48714012</v>
+        <v>48997233</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>242</v>
@@ -28083,7 +28089,7 @@
       </c>
       <c r="D83" s="11">
         <f t="shared" si="3"/>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E83" s="11">
         <f t="shared" si="4"/>
@@ -28091,7 +28097,7 @@
       </c>
       <c r="F83" s="11">
         <f t="shared" si="5"/>
-        <v>-34600000</v>
+        <v>-34800000</v>
       </c>
       <c r="G83" s="11"/>
     </row>
@@ -28107,7 +28113,7 @@
       </c>
       <c r="D84" s="11">
         <f t="shared" si="3"/>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E84" s="11">
         <f t="shared" si="4"/>
@@ -28115,7 +28121,7 @@
       </c>
       <c r="F84" s="11">
         <f t="shared" si="5"/>
-        <v>340000000</v>
+        <v>342000000</v>
       </c>
       <c r="G84" s="11"/>
     </row>
@@ -28131,7 +28137,7 @@
       </c>
       <c r="D85" s="11">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E85" s="11">
         <f t="shared" si="4"/>
@@ -28139,7 +28145,7 @@
       </c>
       <c r="F85" s="11">
         <f t="shared" si="5"/>
-        <v>-33600000</v>
+        <v>-33800000</v>
       </c>
       <c r="G85" s="11"/>
     </row>
@@ -28155,7 +28161,7 @@
       </c>
       <c r="D86" s="11">
         <f t="shared" si="3"/>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E86" s="11">
         <f t="shared" si="4"/>
@@ -28163,7 +28169,7 @@
       </c>
       <c r="F86" s="11">
         <f t="shared" si="5"/>
-        <v>-32400000</v>
+        <v>-32600000</v>
       </c>
       <c r="G86" s="11"/>
     </row>
@@ -28179,7 +28185,7 @@
       </c>
       <c r="D87" s="11">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E87" s="11">
         <f t="shared" si="4"/>
@@ -28187,7 +28193,7 @@
       </c>
       <c r="F87" s="11">
         <f t="shared" si="5"/>
-        <v>-212000000</v>
+        <v>-213325000</v>
       </c>
       <c r="G87" s="11"/>
     </row>
@@ -28203,7 +28209,7 @@
       </c>
       <c r="D88" s="11">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E88" s="11">
         <f t="shared" si="4"/>
@@ -28211,7 +28217,7 @@
       </c>
       <c r="F88" s="11">
         <f t="shared" si="5"/>
-        <v>-72500000</v>
+        <v>-73000000</v>
       </c>
       <c r="G88" s="11"/>
     </row>
@@ -28227,7 +28233,7 @@
       </c>
       <c r="D89" s="11">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E89" s="11">
         <f t="shared" si="4"/>
@@ -28235,7 +28241,7 @@
       </c>
       <c r="F89" s="11">
         <f t="shared" si="5"/>
-        <v>-17400000</v>
+        <v>-17520000</v>
       </c>
       <c r="G89" s="11"/>
     </row>
@@ -28251,7 +28257,7 @@
       </c>
       <c r="D90" s="11">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E90" s="11">
         <f t="shared" si="4"/>
@@ -28259,7 +28265,7 @@
       </c>
       <c r="F90" s="11">
         <f t="shared" si="5"/>
-        <v>60805110</v>
+        <v>61233315</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>264</v>
@@ -28277,7 +28283,7 @@
       </c>
       <c r="D91" s="11">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E91" s="11">
         <f t="shared" si="4"/>
@@ -28285,7 +28291,7 @@
       </c>
       <c r="F91" s="11">
         <f t="shared" si="5"/>
-        <v>-420280000</v>
+        <v>-423282000</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>344</v>
@@ -28303,7 +28309,7 @@
       </c>
       <c r="D92" s="11">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E92" s="11">
         <f t="shared" si="4"/>
@@ -28311,7 +28317,7 @@
       </c>
       <c r="F92" s="11">
         <f t="shared" si="5"/>
-        <v>-28290000</v>
+        <v>-28495000</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>345</v>
@@ -28329,7 +28335,7 @@
       </c>
       <c r="D93" s="11">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E93" s="11">
         <f t="shared" si="4"/>
@@ -28337,7 +28343,7 @@
       </c>
       <c r="F93" s="11">
         <f t="shared" si="5"/>
-        <v>-48369000</v>
+        <v>-48719500</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>342</v>
@@ -28355,7 +28361,7 @@
       </c>
       <c r="D94" s="11">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E94" s="11">
         <f t="shared" si="4"/>
@@ -28363,7 +28369,7 @@
       </c>
       <c r="F94" s="11">
         <f t="shared" si="5"/>
-        <v>126000000</v>
+        <v>127000000</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>340</v>
@@ -28381,7 +28387,7 @@
       </c>
       <c r="D95" s="11">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E95" s="11">
         <f t="shared" si="4"/>
@@ -28389,7 +28395,7 @@
       </c>
       <c r="F95" s="11">
         <f t="shared" si="5"/>
-        <v>1089000000</v>
+        <v>1098000000</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>352</v>
@@ -28408,7 +28414,7 @@
       </c>
       <c r="D96" s="11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E96" s="11">
         <f t="shared" si="4"/>
@@ -28416,7 +28422,7 @@
       </c>
       <c r="F96" s="11">
         <f t="shared" si="5"/>
-        <v>-3120000000</v>
+        <v>-3146000000</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>354</v>
@@ -28434,7 +28440,7 @@
       </c>
       <c r="D97" s="11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E97" s="11">
         <f t="shared" si="4"/>
@@ -28442,7 +28448,7 @@
       </c>
       <c r="F97" s="11">
         <f t="shared" si="5"/>
-        <v>-3120000000</v>
+        <v>-3146000000</v>
       </c>
       <c r="G97" s="11"/>
     </row>
@@ -28458,7 +28464,7 @@
       </c>
       <c r="D98" s="11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E98" s="11">
         <f t="shared" si="4"/>
@@ -28466,7 +28472,7 @@
       </c>
       <c r="F98" s="11">
         <f t="shared" si="5"/>
-        <v>3094000000</v>
+        <v>3120000000</v>
       </c>
       <c r="G98" s="11"/>
     </row>
@@ -28482,7 +28488,7 @@
       </c>
       <c r="D99" s="11">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E99" s="11">
         <f t="shared" si="4"/>
@@ -28490,7 +28496,7 @@
       </c>
       <c r="F99" s="11">
         <f t="shared" si="5"/>
-        <v>-24000000</v>
+        <v>-24200000</v>
       </c>
       <c r="G99" s="11"/>
       <c r="I99" t="s">
@@ -28509,7 +28515,7 @@
       </c>
       <c r="D100" s="11">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E100" s="11">
         <f t="shared" si="4"/>
@@ -28517,7 +28523,7 @@
       </c>
       <c r="F100" s="11">
         <f t="shared" si="5"/>
-        <v>3416400000</v>
+        <v>3445600000</v>
       </c>
       <c r="G100" s="11"/>
     </row>
@@ -28533,7 +28539,7 @@
       </c>
       <c r="D101" s="11">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E101" s="11">
         <f t="shared" si="4"/>
@@ -28541,7 +28547,7 @@
       </c>
       <c r="F101" s="11">
         <f t="shared" si="5"/>
-        <v>44793840</v>
+        <v>45193785</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>407</v>
@@ -28559,7 +28565,7 @@
       </c>
       <c r="D102" s="11">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E102" s="11">
         <f t="shared" si="4"/>
@@ -28567,7 +28573,7 @@
       </c>
       <c r="F102" s="11">
         <f t="shared" si="5"/>
-        <v>222000000</v>
+        <v>224000000</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>409</v>
@@ -28585,7 +28591,7 @@
       </c>
       <c r="D103" s="11">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E103" s="11">
         <f t="shared" si="4"/>
@@ -28593,7 +28599,7 @@
       </c>
       <c r="F103" s="11">
         <f t="shared" si="5"/>
-        <v>825000000</v>
+        <v>832500000</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>417</v>
@@ -28611,7 +28617,7 @@
       </c>
       <c r="D104" s="11">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E104" s="11">
         <f t="shared" si="4"/>
@@ -28619,7 +28625,7 @@
       </c>
       <c r="F104" s="11">
         <f t="shared" si="5"/>
-        <v>-7326000000</v>
+        <v>-7392000000</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>431</v>
@@ -28637,7 +28643,7 @@
       </c>
       <c r="D105" s="11">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E105" s="11">
         <f t="shared" si="4"/>
@@ -28645,7 +28651,7 @@
       </c>
       <c r="F105" s="11">
         <f t="shared" si="5"/>
-        <v>-16095000</v>
+        <v>-16240000</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>432</v>
@@ -28663,7 +28669,7 @@
       </c>
       <c r="D106" s="11">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E106" s="11">
         <f t="shared" si="4"/>
@@ -28671,7 +28677,7 @@
       </c>
       <c r="F106" s="11">
         <f t="shared" si="5"/>
-        <v>648000000</v>
+        <v>654000000</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>433</v>
@@ -28689,7 +28695,7 @@
       </c>
       <c r="D107" s="11">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E107" s="11">
         <f t="shared" si="4"/>
@@ -28697,7 +28703,7 @@
       </c>
       <c r="F107" s="11">
         <f t="shared" si="5"/>
-        <v>-642631300</v>
+        <v>-648637200</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>443</v>
@@ -28715,7 +28721,7 @@
       </c>
       <c r="D108" s="11">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E108" s="11">
         <f t="shared" si="4"/>
@@ -28723,7 +28729,7 @@
       </c>
       <c r="F108" s="11">
         <f t="shared" si="5"/>
-        <v>618000000</v>
+        <v>624000000</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>451</v>
@@ -28741,7 +28747,7 @@
       </c>
       <c r="D109" s="11">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E109" s="11">
         <f t="shared" si="4"/>
@@ -28749,7 +28755,7 @@
       </c>
       <c r="F109" s="11">
         <f t="shared" si="5"/>
-        <v>-11040000</v>
+        <v>-11160000</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>472</v>
@@ -28767,7 +28773,7 @@
       </c>
       <c r="D110" s="11">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E110" s="11">
         <f t="shared" si="4"/>
@@ -28775,7 +28781,7 @@
       </c>
       <c r="F110" s="11">
         <f t="shared" si="5"/>
-        <v>360000000</v>
+        <v>364000000</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>474</v>
@@ -28793,7 +28799,7 @@
       </c>
       <c r="D111" s="11">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E111" s="11">
         <f t="shared" si="4"/>
@@ -28801,7 +28807,7 @@
       </c>
       <c r="F111" s="11">
         <f t="shared" si="5"/>
-        <v>249200000</v>
+        <v>252000000</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>479</v>
@@ -28819,7 +28825,7 @@
       </c>
       <c r="D112" s="11">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E112" s="11">
         <f t="shared" si="4"/>
@@ -28827,7 +28833,7 @@
       </c>
       <c r="F112" s="11">
         <f t="shared" si="5"/>
-        <v>-17200000</v>
+        <v>-17400000</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>485</v>
@@ -28845,7 +28851,7 @@
       </c>
       <c r="D113" s="11">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E113" s="11">
         <f t="shared" si="4"/>
@@ -28853,7 +28859,7 @@
       </c>
       <c r="F113" s="11">
         <f t="shared" si="5"/>
-        <v>6074040</v>
+        <v>6146350</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>518</v>
@@ -28871,7 +28877,7 @@
       </c>
       <c r="D114" s="11">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E114" s="11">
         <f t="shared" si="4"/>
@@ -28879,7 +28885,7 @@
       </c>
       <c r="F114" s="11">
         <f t="shared" si="5"/>
-        <v>-13600000</v>
+        <v>-13800000</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>472</v>
@@ -28900,7 +28906,7 @@
       </c>
       <c r="D115" s="11">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E115" s="11">
         <f t="shared" si="4"/>
@@ -28908,7 +28914,7 @@
       </c>
       <c r="F115" s="25">
         <f t="shared" si="5"/>
-        <v>-737000000</v>
+        <v>-748000000</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>519</v>
@@ -28926,7 +28932,7 @@
       </c>
       <c r="D116" s="11">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E116" s="11">
         <f t="shared" si="4"/>
@@ -28934,7 +28940,7 @@
       </c>
       <c r="F116" s="11">
         <f t="shared" si="5"/>
-        <v>-13400000</v>
+        <v>-13600000</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>472</v>
@@ -28955,7 +28961,7 @@
       </c>
       <c r="D117" s="11">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E117" s="11">
         <f t="shared" si="4"/>
@@ -28963,7 +28969,7 @@
       </c>
       <c r="F117" s="11">
         <f t="shared" si="5"/>
-        <v>-29282500</v>
+        <v>-29733000</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>521</v>
@@ -28981,7 +28987,7 @@
       </c>
       <c r="D118" s="11">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E118" s="11">
         <f t="shared" si="4"/>
@@ -28989,7 +28995,7 @@
       </c>
       <c r="F118" s="11">
         <f t="shared" si="5"/>
-        <v>-13000000</v>
+        <v>-13200000</v>
       </c>
       <c r="G118" s="11" t="s">
         <v>522</v>
@@ -29010,7 +29016,7 @@
       </c>
       <c r="D119" s="11">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E119" s="11">
         <f t="shared" si="4"/>
@@ -29018,7 +29024,7 @@
       </c>
       <c r="F119" s="11">
         <f t="shared" si="5"/>
-        <v>-9118450</v>
+        <v>-9273000</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>525</v>
@@ -29036,7 +29042,7 @@
       </c>
       <c r="D120" s="11">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E120" s="11">
         <f t="shared" si="4"/>
@@ -29044,7 +29050,7 @@
       </c>
       <c r="F120" s="11">
         <f t="shared" si="5"/>
-        <v>-18880</v>
+        <v>-19200</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>526</v>
@@ -29062,7 +29068,7 @@
       </c>
       <c r="D121" s="11">
         <f t="shared" si="3"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E121" s="11">
         <f t="shared" si="4"/>
@@ -29070,7 +29076,7 @@
       </c>
       <c r="F121" s="11">
         <f t="shared" si="5"/>
-        <v>-25056000</v>
+        <v>-25488000</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>528</v>
@@ -29088,7 +29094,7 @@
       </c>
       <c r="D122" s="11">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E122" s="11">
         <f t="shared" si="4"/>
@@ -29096,7 +29102,7 @@
       </c>
       <c r="F122" s="11">
         <f t="shared" si="5"/>
-        <v>3776193</v>
+        <v>3850236</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>530</v>
@@ -29114,7 +29120,7 @@
       </c>
       <c r="D123" s="11">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E123" s="11">
         <f t="shared" si="4"/>
@@ -29122,7 +29128,7 @@
       </c>
       <c r="F123" s="11">
         <f t="shared" si="5"/>
-        <v>-1612000</v>
+        <v>-1664000</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>557</v>
@@ -29140,7 +29146,7 @@
       </c>
       <c r="D124" s="11">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E124" s="11">
         <f t="shared" si="4"/>
@@ -29148,7 +29154,7 @@
       </c>
       <c r="F124" s="11">
         <f t="shared" si="5"/>
-        <v>22553</v>
+        <v>23740</v>
       </c>
       <c r="G124" s="11" t="s">
         <v>612</v>
@@ -29166,7 +29172,7 @@
       </c>
       <c r="D125" s="11">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E125" s="11">
         <f t="shared" si="4"/>
@@ -29174,7 +29180,7 @@
       </c>
       <c r="F125" s="11">
         <f t="shared" si="5"/>
-        <v>43200000</v>
+        <v>45600000</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>610</v>
@@ -29192,7 +29198,7 @@
       </c>
       <c r="D126" s="11">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E126" s="11">
         <f t="shared" si="4"/>
@@ -29200,7 +29206,7 @@
       </c>
       <c r="F126" s="11">
         <f t="shared" si="5"/>
-        <v>21484800</v>
+        <v>22827600</v>
       </c>
       <c r="G126" s="11" t="s">
         <v>621</v>
@@ -29218,7 +29224,7 @@
       </c>
       <c r="D127" s="11">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E127" s="11">
         <f t="shared" si="4"/>
@@ -29226,7 +29232,7 @@
       </c>
       <c r="F127" s="11">
         <f t="shared" si="5"/>
-        <v>21484800</v>
+        <v>22827600</v>
       </c>
       <c r="G127" s="11" t="s">
         <v>622</v>
@@ -29244,7 +29250,7 @@
       </c>
       <c r="D128" s="11">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E128" s="11">
         <f t="shared" si="4"/>
@@ -29252,7 +29258,7 @@
       </c>
       <c r="F128" s="11">
         <f t="shared" si="5"/>
-        <v>-1000000</v>
+        <v>-1200000</v>
       </c>
       <c r="G128" s="11" t="s">
         <v>158</v>
@@ -29270,7 +29276,7 @@
       </c>
       <c r="D129" s="11">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E129" s="11">
         <f t="shared" si="4"/>
@@ -29278,7 +29284,7 @@
       </c>
       <c r="F129" s="11">
         <f>B129*(D129-E129)</f>
-        <v>-46854</v>
+        <v>-62472</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>631</v>
@@ -29295,11 +29301,11 @@
         <v>-200000</v>
       </c>
       <c r="C130" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D130" s="11">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E130" s="11">
         <f t="shared" si="4"/>
@@ -29307,19 +29313,25 @@
       </c>
       <c r="F130" s="11">
         <f t="shared" si="5"/>
-        <v>-400000</v>
+        <v>-600000</v>
       </c>
       <c r="G130" s="11" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="11"/>
+      <c r="A131" s="11" t="s">
+        <v>635</v>
+      </c>
+      <c r="B131" s="3">
+        <v>-200000</v>
+      </c>
+      <c r="C131" s="11">
+        <v>2</v>
+      </c>
       <c r="D131" s="11">
         <f t="shared" ref="D131:D137" si="6">D132+C131</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E131" s="11">
         <f t="shared" ref="E131:E137" si="7">IF(B131&gt;0,1,0)</f>
@@ -29327,9 +29339,11 @@
       </c>
       <c r="F131" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G131" s="11"/>
+        <v>-400000</v>
+      </c>
+      <c r="G131" s="11" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>
@@ -29462,14 +29476,14 @@
       <c r="A139" s="11"/>
       <c r="B139" s="31">
         <f>SUM(B2:B137)</f>
-        <v>4717073</v>
+        <v>4517073</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="31">
         <f>SUM(F2:F137)</f>
-        <v>4389348149</v>
+        <v>4393665222</v>
       </c>
       <c r="G139" s="11"/>
     </row>
@@ -29503,7 +29517,7 @@
       <c r="E142" s="11"/>
       <c r="F142" s="3">
         <f>F139/D2</f>
-        <v>11736224.997326203</v>
+        <v>11716440.592</v>
       </c>
       <c r="G142" s="11"/>
     </row>
@@ -29532,7 +29546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -29735,11 +29749,11 @@
       </c>
       <c r="F6" s="65">
         <f>K23</f>
-        <v>171453547.78082192</v>
+        <v>171263547.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>1232629.7891781032</v>
+        <v>1422629.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -29859,11 +29873,11 @@
       </c>
       <c r="K9" s="46">
         <f>'مسکن ایلیا'!B139</f>
-        <v>4717073</v>
+        <v>4517073</v>
       </c>
       <c r="L9" s="3">
         <f>K9</f>
-        <v>4717073</v>
+        <v>4517073</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" ref="M9:M22" si="4">K9-L9</f>
@@ -30141,11 +30155,11 @@
         <v>468</v>
       </c>
       <c r="K16" s="46">
-        <v>31000</v>
+        <v>41000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>31000</v>
+        <v>41000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
@@ -30494,11 +30508,11 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>171453547.78082192</v>
+        <v>171263547.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>61002867.520547941</v>
+        <v>60812867.520547941</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
@@ -30546,11 +30560,11 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>99421356</v>
+        <v>99231356</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12</f>
-        <v>20748073</v>
+        <v>20558073</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17</f>

</xml_diff>

<commit_message>
finance updated 22/4/1396 at 16:43
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -29581,7 +29581,7 @@
   <dimension ref="A1:W67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30948,6 +30948,10 @@
       <c r="F33" s="3"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
+      <c r="L33" s="7">
+        <f>M31-L31</f>
+        <v>542465.75342465751</v>
+      </c>
       <c r="O33" s="33" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
finance updated 28/4/1396 11:00
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -29351,7 +29351,7 @@
         <v>1</v>
       </c>
       <c r="D131" s="11">
-        <f t="shared" ref="D131:D146" si="6">D132+C131</f>
+        <f t="shared" ref="D131:D134" si="6">D132+C131</f>
         <v>7</v>
       </c>
       <c r="E131" s="11">
@@ -29765,7 +29765,7 @@
   <dimension ref="A1:W67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29967,11 +29967,11 @@
       </c>
       <c r="F6" s="63">
         <f>K23</f>
-        <v>170518047.78082192</v>
+        <v>170638047.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>2168129.7891781032</v>
+        <v>2048129.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -30373,11 +30373,11 @@
         <v>468</v>
       </c>
       <c r="K16" s="46">
-        <v>5000</v>
+        <v>125000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>5000</v>
+        <v>125000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
@@ -30726,11 +30726,11 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>170518047.78082192</v>
+        <v>170638047.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>60067367.520547941</v>
+        <v>60187367.520547941</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
@@ -30778,11 +30778,11 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>98485856</v>
+        <v>98605856</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12</f>
-        <v>19812573</v>
+        <v>19932573</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17</f>

</xml_diff>

<commit_message>
updated 31/4/1396 at 9:39
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="653">
   <si>
     <t>18/1/95</t>
   </si>
@@ -1991,6 +1991,9 @@
   </si>
   <si>
     <t>انتقال به کارت ایلیا 12 میلیون و 200 هم نقدی</t>
+  </si>
+  <si>
+    <t>182 تا آخر مرداد</t>
   </si>
 </sst>
 </file>
@@ -24014,7 +24017,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25880,7 +25883,7 @@
         <v>650</v>
       </c>
       <c r="B58" s="41">
-        <v>-12200000</v>
+        <v>-12200500</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>651</v>
@@ -26075,7 +26078,7 @@
       <c r="A68" s="11"/>
       <c r="B68" s="31">
         <f>SUM(B2:B66)</f>
-        <v>2148237</v>
+        <v>2147737</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -29837,8 +29840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30040,11 +30043,11 @@
       </c>
       <c r="F6" s="63">
         <f>K23</f>
-        <v>170318047.78082192</v>
+        <v>170317547.78082192</v>
       </c>
       <c r="G6" s="31">
         <f>E6-F6</f>
-        <v>2368129.7891781032</v>
+        <v>2368629.7891781032</v>
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="2" t="s">
@@ -30276,14 +30279,14 @@
       </c>
       <c r="K12" s="46">
         <f>'مسکن مریم یاران'!B68</f>
-        <v>2148237</v>
+        <v>2147737</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>2148237</v>
+        <v>2147737</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -30798,7 +30801,7 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>170318047.78082192</v>
+        <v>170317547.78082192</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
@@ -30806,7 +30809,7 @@
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
-        <v>110350680.26027396</v>
+        <v>110350180.26027396</v>
       </c>
       <c r="N23" s="27"/>
       <c r="O23" s="11" t="s">
@@ -30850,7 +30853,7 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>98285856</v>
+        <v>98285356</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12+L10</f>
@@ -30858,7 +30861,7 @@
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17+M9</f>
-        <v>78223283</v>
+        <v>78222783</v>
       </c>
       <c r="N24" s="27"/>
       <c r="O24" s="11"/>
@@ -31164,7 +31167,9 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
+      <c r="K32" s="27" t="s">
+        <v>652</v>
+      </c>
       <c r="L32" s="58"/>
       <c r="M32" s="58"/>
       <c r="N32" s="58"/>

</xml_diff>

<commit_message>
updated 3/5/1396 at 22:33
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="مرداد 96" sheetId="24" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="688">
   <si>
     <t>18/1/95</t>
   </si>
@@ -2088,6 +2088,18 @@
   </si>
   <si>
     <t xml:space="preserve">حواله اچ سی </t>
+  </si>
+  <si>
+    <t>کفش ایلیا و پاپیون و جوراب</t>
+  </si>
+  <si>
+    <t>2/5/1396</t>
+  </si>
+  <si>
+    <t>مریم خرید کرد لباس برای عروسی</t>
+  </si>
+  <si>
+    <t>طبق گفته مریم سارا برای لباس کارت کشید</t>
   </si>
 </sst>
 </file>
@@ -2776,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,7 +2846,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>608</v>
+        <v>648</v>
       </c>
       <c r="B2" s="3">
         <f>'تیر 96'!B24</f>
@@ -2878,7 +2890,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>605</v>
+        <v>654</v>
       </c>
       <c r="B3" s="42">
         <v>384551</v>
@@ -2920,21 +2932,23 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>616</v>
+        <v>685</v>
       </c>
       <c r="B4" s="18">
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>800000</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="20"/>
+        <v>-800000</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="F4">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
@@ -2942,11 +2956,11 @@
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>23200000</v>
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-23200000</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -3686,11 +3700,11 @@
       </c>
       <c r="C24" s="3">
         <f>SUM(C2:C22)</f>
-        <v>12004426</v>
+        <v>12804426</v>
       </c>
       <c r="D24" s="3">
         <f>SUM(D2:D22)</f>
-        <v>32531973</v>
+        <v>31731973</v>
       </c>
       <c r="E24" s="2"/>
       <c r="O24">
@@ -3710,11 +3724,11 @@
       </c>
       <c r="H25" s="18">
         <f>SUM(H2:H23)</f>
-        <v>372026298</v>
+        <v>395226298</v>
       </c>
       <c r="I25" s="18">
         <f>SUM(I2:I23)</f>
-        <v>1008217520</v>
+        <v>985017520</v>
       </c>
       <c r="O25">
         <v>24</v>
@@ -3798,11 +3812,11 @@
       </c>
       <c r="H30" s="18">
         <f>G30*H25/G25</f>
-        <v>103650.58916148538</v>
+        <v>110114.36250620324</v>
       </c>
       <c r="I30" s="18">
         <f>G30*I25/G25</f>
-        <v>280900.41083851462</v>
+        <v>274436.63749379676</v>
       </c>
       <c r="O30">
         <v>29</v>
@@ -3816,9 +3830,11 @@
     </row>
     <row r="31" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="45">
-        <v>0</v>
-      </c>
-      <c r="E31" s="57"/>
+        <v>-65000</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>684</v>
+      </c>
       <c r="G31" s="9" t="s">
         <v>415</v>
       </c>
@@ -3913,7 +3929,7 @@
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <f>SUM(D30:D39)</f>
-        <v>8478102</v>
+        <v>8413102</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -15166,8 +15182,8 @@
   <dimension ref="A1:O136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D138" sqref="D138:M168"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L129" sqref="L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15244,7 +15260,7 @@
       </c>
       <c r="G2" s="39">
         <f>G3+F2</f>
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H2" s="39">
         <f>IF(B2&gt;0,1,0)</f>
@@ -15252,11 +15268,11 @@
       </c>
       <c r="I2" s="11">
         <f>B2*(G2-H2)</f>
-        <v>7832300</v>
+        <v>7849000</v>
       </c>
       <c r="J2" s="56">
         <f>C2*(G2-H2)</f>
-        <v>7832300</v>
+        <v>7849000</v>
       </c>
       <c r="K2" s="56">
         <f>D2*(G2-H2)</f>
@@ -15285,7 +15301,7 @@
       </c>
       <c r="G3" s="39">
         <f t="shared" ref="G3:G66" si="1">G4+F3</f>
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H3" s="39">
         <f t="shared" ref="H3:H66" si="2">IF(B3&gt;0,1,0)</f>
@@ -15293,15 +15309,15 @@
       </c>
       <c r="I3" s="11">
         <f t="shared" ref="I3:I66" si="3">B3*(G3-H3)</f>
-        <v>9313200000</v>
+        <v>9333100000</v>
       </c>
       <c r="J3" s="56">
         <f t="shared" ref="J3:J66" si="4">C3*(G3-H3)</f>
-        <v>5329116000</v>
+        <v>5340503000</v>
       </c>
       <c r="K3" s="56">
         <f t="shared" ref="K3:K66" si="5">D3*(G3-H3)</f>
-        <v>3984084000</v>
+        <v>3992597000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -15326,7 +15342,7 @@
       </c>
       <c r="G4" s="39">
         <f t="shared" si="1"/>
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H4" s="39">
         <f t="shared" si="2"/>
@@ -15338,11 +15354,11 @@
       </c>
       <c r="J4" s="56">
         <f t="shared" si="4"/>
-        <v>3986500</v>
+        <v>3995000</v>
       </c>
       <c r="K4" s="56">
         <f t="shared" si="5"/>
-        <v>-3986500</v>
+        <v>-3995000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -15367,7 +15383,7 @@
       </c>
       <c r="G5" s="39">
         <f t="shared" si="1"/>
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="H5" s="39">
         <f t="shared" si="2"/>
@@ -15375,7 +15391,7 @@
       </c>
       <c r="I5" s="11">
         <f t="shared" si="3"/>
-        <v>932000000</v>
+        <v>934000000</v>
       </c>
       <c r="J5" s="56">
         <f t="shared" si="4"/>
@@ -15383,7 +15399,7 @@
       </c>
       <c r="K5" s="56">
         <f t="shared" si="5"/>
-        <v>932000000</v>
+        <v>934000000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -15408,7 +15424,7 @@
       </c>
       <c r="G6" s="39">
         <f t="shared" si="1"/>
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H6" s="39">
         <f t="shared" si="2"/>
@@ -15416,7 +15432,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" si="3"/>
-        <v>-2300000</v>
+        <v>-2305000</v>
       </c>
       <c r="J6" s="56">
         <f t="shared" si="4"/>
@@ -15424,7 +15440,7 @@
       </c>
       <c r="K6" s="56">
         <f t="shared" si="5"/>
-        <v>-2300000</v>
+        <v>-2305000</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -15449,7 +15465,7 @@
       </c>
       <c r="G7" s="39">
         <f t="shared" si="1"/>
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H7" s="39">
         <f t="shared" si="2"/>
@@ -15457,7 +15473,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" si="3"/>
-        <v>-547428000</v>
+        <v>-548628500</v>
       </c>
       <c r="J7" s="56">
         <f t="shared" si="4"/>
@@ -15465,7 +15481,7 @@
       </c>
       <c r="K7" s="56">
         <f t="shared" si="5"/>
-        <v>-547428000</v>
+        <v>-548628500</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -15490,7 +15506,7 @@
       </c>
       <c r="G8" s="39">
         <f t="shared" si="1"/>
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H8" s="39">
         <f t="shared" si="2"/>
@@ -15498,7 +15514,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" si="3"/>
-        <v>-91000000</v>
+        <v>-91200000</v>
       </c>
       <c r="J8" s="56">
         <f t="shared" si="4"/>
@@ -15506,7 +15522,7 @@
       </c>
       <c r="K8" s="56">
         <f t="shared" si="5"/>
-        <v>-91000000</v>
+        <v>-91200000</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -15531,7 +15547,7 @@
       </c>
       <c r="G9" s="39">
         <f t="shared" si="1"/>
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H9" s="39">
         <f t="shared" si="2"/>
@@ -15539,7 +15555,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" si="3"/>
-        <v>-319591500</v>
+        <v>-320297000</v>
       </c>
       <c r="J9" s="56">
         <f t="shared" si="4"/>
@@ -15547,7 +15563,7 @@
       </c>
       <c r="K9" s="56">
         <f t="shared" si="5"/>
-        <v>-319591500</v>
+        <v>-320297000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -15572,7 +15588,7 @@
       </c>
       <c r="G10" s="39">
         <f t="shared" si="1"/>
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H10" s="39">
         <f t="shared" si="2"/>
@@ -15580,7 +15596,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" si="3"/>
-        <v>-88800000</v>
+        <v>-89000000</v>
       </c>
       <c r="J10" s="56">
         <f t="shared" si="4"/>
@@ -15588,7 +15604,7 @@
       </c>
       <c r="K10" s="56">
         <f t="shared" si="5"/>
-        <v>-88800000</v>
+        <v>-89000000</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -15613,7 +15629,7 @@
       </c>
       <c r="G11" s="39">
         <f t="shared" si="1"/>
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H11" s="39">
         <f t="shared" si="2"/>
@@ -15621,7 +15637,7 @@
       </c>
       <c r="I11" s="11">
         <f t="shared" si="3"/>
-        <v>443000000</v>
+        <v>444000000</v>
       </c>
       <c r="J11" s="56">
         <f t="shared" si="4"/>
@@ -15629,7 +15645,7 @@
       </c>
       <c r="K11" s="56">
         <f t="shared" si="5"/>
-        <v>443000000</v>
+        <v>444000000</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -15654,7 +15670,7 @@
       </c>
       <c r="G12" s="39">
         <f t="shared" si="1"/>
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H12" s="39">
         <f t="shared" si="2"/>
@@ -15662,7 +15678,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" si="3"/>
-        <v>-132000000</v>
+        <v>-132300000</v>
       </c>
       <c r="J12" s="56">
         <f t="shared" si="4"/>
@@ -15670,7 +15686,7 @@
       </c>
       <c r="K12" s="56">
         <f t="shared" si="5"/>
-        <v>-132000000</v>
+        <v>-132300000</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -15695,7 +15711,7 @@
       </c>
       <c r="G13" s="39">
         <f t="shared" si="1"/>
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H13" s="39">
         <f t="shared" si="2"/>
@@ -15703,7 +15719,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" si="3"/>
-        <v>-26970000</v>
+        <v>-27032000</v>
       </c>
       <c r="J13" s="56">
         <f t="shared" si="4"/>
@@ -15711,7 +15727,7 @@
       </c>
       <c r="K13" s="56">
         <f t="shared" si="5"/>
-        <v>-26970000</v>
+        <v>-27032000</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -15736,7 +15752,7 @@
       </c>
       <c r="G14" s="39">
         <f t="shared" si="1"/>
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H14" s="39">
         <f t="shared" si="2"/>
@@ -15744,7 +15760,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" si="3"/>
-        <v>868000000</v>
+        <v>870000000</v>
       </c>
       <c r="J14" s="56">
         <f t="shared" si="4"/>
@@ -15752,7 +15768,7 @@
       </c>
       <c r="K14" s="56">
         <f t="shared" si="5"/>
-        <v>868000000</v>
+        <v>870000000</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -15777,7 +15793,7 @@
       </c>
       <c r="G15" s="39">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H15" s="39">
         <f t="shared" si="2"/>
@@ -15785,7 +15801,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" si="3"/>
-        <v>779400000</v>
+        <v>781200000</v>
       </c>
       <c r="J15" s="56">
         <f t="shared" si="4"/>
@@ -15793,7 +15809,7 @@
       </c>
       <c r="K15" s="56">
         <f t="shared" si="5"/>
-        <v>779400000</v>
+        <v>781200000</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -15818,7 +15834,7 @@
       </c>
       <c r="G16" s="39">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H16" s="39">
         <f t="shared" si="2"/>
@@ -15826,7 +15842,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" si="3"/>
-        <v>-86800000</v>
+        <v>-87000000</v>
       </c>
       <c r="J16" s="56">
         <f t="shared" si="4"/>
@@ -15834,7 +15850,7 @@
       </c>
       <c r="K16" s="56">
         <f t="shared" si="5"/>
-        <v>-86800000</v>
+        <v>-87000000</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -15859,7 +15875,7 @@
       </c>
       <c r="G17" s="39">
         <f t="shared" si="1"/>
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H17" s="39">
         <f t="shared" si="2"/>
@@ -15867,7 +15883,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" si="3"/>
-        <v>-860000000</v>
+        <v>-862000000</v>
       </c>
       <c r="J17" s="56">
         <f t="shared" si="4"/>
@@ -15875,7 +15891,7 @@
       </c>
       <c r="K17" s="56">
         <f t="shared" si="5"/>
-        <v>-860000000</v>
+        <v>-862000000</v>
       </c>
       <c r="L17" t="s">
         <v>25</v>
@@ -15903,7 +15919,7 @@
       </c>
       <c r="G18" s="39">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H18" s="39">
         <f t="shared" si="2"/>
@@ -15911,7 +15927,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" si="3"/>
-        <v>-128700000</v>
+        <v>-129000000</v>
       </c>
       <c r="J18" s="56">
         <f t="shared" si="4"/>
@@ -15919,7 +15935,7 @@
       </c>
       <c r="K18" s="56">
         <f t="shared" si="5"/>
-        <v>-128700000</v>
+        <v>-129000000</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -15944,7 +15960,7 @@
       </c>
       <c r="G19" s="39">
         <f t="shared" si="1"/>
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H19" s="39">
         <f t="shared" si="2"/>
@@ -15952,7 +15968,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" si="3"/>
-        <v>-85600000</v>
+        <v>-85800000</v>
       </c>
       <c r="J19" s="56">
         <f t="shared" si="4"/>
@@ -15960,7 +15976,7 @@
       </c>
       <c r="K19" s="56">
         <f t="shared" si="5"/>
-        <v>-85600000</v>
+        <v>-85800000</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -15985,7 +16001,7 @@
       </c>
       <c r="G20" s="39">
         <f t="shared" si="1"/>
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H20" s="39">
         <f t="shared" si="2"/>
@@ -15993,15 +16009,15 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" si="3"/>
-        <v>115212825</v>
+        <v>115483914</v>
       </c>
       <c r="J20" s="56">
         <f t="shared" si="4"/>
-        <v>62667100</v>
+        <v>62814552</v>
       </c>
       <c r="K20" s="56">
         <f t="shared" si="5"/>
-        <v>52545725</v>
+        <v>52669362</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -16026,7 +16042,7 @@
       </c>
       <c r="G21" s="39">
         <f t="shared" si="1"/>
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H21" s="39">
         <f t="shared" si="2"/>
@@ -16034,7 +16050,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" si="3"/>
-        <v>-638416800</v>
+        <v>-639922500</v>
       </c>
       <c r="J21" s="56">
         <f t="shared" si="4"/>
@@ -16042,7 +16058,7 @@
       </c>
       <c r="K21" s="56">
         <f t="shared" si="5"/>
-        <v>-638416800</v>
+        <v>-639922500</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -16067,7 +16083,7 @@
       </c>
       <c r="G22" s="39">
         <f t="shared" si="1"/>
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H22" s="39">
         <f t="shared" si="2"/>
@@ -16075,7 +16091,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" si="3"/>
-        <v>1260000000</v>
+        <v>1263000000</v>
       </c>
       <c r="J22" s="56">
         <f t="shared" si="4"/>
@@ -16083,7 +16099,7 @@
       </c>
       <c r="K22" s="56">
         <f t="shared" si="5"/>
-        <v>1260000000</v>
+        <v>1263000000</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -16108,7 +16124,7 @@
       </c>
       <c r="G23" s="39">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H23" s="39">
         <f t="shared" si="2"/>
@@ -16116,7 +16132,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" si="3"/>
-        <v>419000000</v>
+        <v>420000000</v>
       </c>
       <c r="J23" s="56">
         <f t="shared" si="4"/>
@@ -16124,7 +16140,7 @@
       </c>
       <c r="K23" s="56">
         <f t="shared" si="5"/>
-        <v>419000000</v>
+        <v>420000000</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -16149,7 +16165,7 @@
       </c>
       <c r="G24" s="39">
         <f t="shared" si="1"/>
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H24" s="39">
         <f t="shared" si="2"/>
@@ -16157,7 +16173,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" si="3"/>
-        <v>-1257377100</v>
+        <v>-1260378000</v>
       </c>
       <c r="J24" s="56">
         <f t="shared" si="4"/>
@@ -16165,7 +16181,7 @@
       </c>
       <c r="K24" s="56">
         <f t="shared" si="5"/>
-        <v>-1257377100</v>
+        <v>-1260378000</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -16190,7 +16206,7 @@
       </c>
       <c r="G25" s="39">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H25" s="39">
         <f t="shared" si="2"/>
@@ -16198,7 +16214,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" si="3"/>
-        <v>604500000</v>
+        <v>606000000</v>
       </c>
       <c r="J25" s="56">
         <f t="shared" si="4"/>
@@ -16206,7 +16222,7 @@
       </c>
       <c r="K25" s="56">
         <f t="shared" si="5"/>
-        <v>604500000</v>
+        <v>606000000</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -16231,7 +16247,7 @@
       </c>
       <c r="G26" s="39">
         <f t="shared" si="1"/>
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H26" s="39">
         <f t="shared" si="2"/>
@@ -16239,7 +16255,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" si="3"/>
-        <v>-64944000</v>
+        <v>-65108000</v>
       </c>
       <c r="J26" s="56">
         <f t="shared" si="4"/>
@@ -16247,7 +16263,7 @@
       </c>
       <c r="K26" s="56">
         <f t="shared" si="5"/>
-        <v>-64944000</v>
+        <v>-65108000</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -16272,7 +16288,7 @@
       </c>
       <c r="G27" s="39">
         <f t="shared" si="1"/>
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H27" s="39">
         <f t="shared" si="2"/>
@@ -16280,15 +16296,15 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" si="3"/>
-        <v>78560842</v>
+        <v>78760235</v>
       </c>
       <c r="J27" s="56">
         <f t="shared" si="4"/>
-        <v>42320722</v>
+        <v>42428135</v>
       </c>
       <c r="K27" s="56">
         <f t="shared" si="5"/>
-        <v>36240120</v>
+        <v>36332100</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -16313,7 +16329,7 @@
       </c>
       <c r="G28" s="39">
         <f t="shared" si="1"/>
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H28" s="39">
         <f t="shared" si="2"/>
@@ -16321,11 +16337,11 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" si="3"/>
-        <v>-86853000</v>
+        <v>-87074000</v>
       </c>
       <c r="J28" s="56">
         <f t="shared" si="4"/>
-        <v>-86853000</v>
+        <v>-87074000</v>
       </c>
       <c r="K28" s="56">
         <f t="shared" si="5"/>
@@ -16354,7 +16370,7 @@
       </c>
       <c r="G29" s="39">
         <f t="shared" si="1"/>
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H29" s="39">
         <f t="shared" si="2"/>
@@ -16362,7 +16378,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" si="3"/>
-        <v>-196696500</v>
+        <v>-197197000</v>
       </c>
       <c r="J29" s="56">
         <f t="shared" si="4"/>
@@ -16370,7 +16386,7 @@
       </c>
       <c r="K29" s="56">
         <f t="shared" si="5"/>
-        <v>-196696500</v>
+        <v>-197197000</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -16395,7 +16411,7 @@
       </c>
       <c r="G30" s="39">
         <f t="shared" si="1"/>
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H30" s="39">
         <f t="shared" si="2"/>
@@ -16403,11 +16419,11 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" si="3"/>
-        <v>-5895000000</v>
+        <v>-5910000000</v>
       </c>
       <c r="J30" s="56">
         <f t="shared" si="4"/>
-        <v>-5895000000</v>
+        <v>-5910000000</v>
       </c>
       <c r="K30" s="56">
         <f t="shared" si="5"/>
@@ -16436,7 +16452,7 @@
       </c>
       <c r="G31" s="39">
         <f t="shared" si="1"/>
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H31" s="39">
         <f t="shared" si="2"/>
@@ -16444,7 +16460,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" si="3"/>
-        <v>-1132098400</v>
+        <v>-1135109300</v>
       </c>
       <c r="J31" s="56">
         <f t="shared" si="4"/>
@@ -16452,7 +16468,7 @@
       </c>
       <c r="K31" s="56">
         <f t="shared" si="5"/>
-        <v>-1132098400</v>
+        <v>-1135109300</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -16477,7 +16493,7 @@
       </c>
       <c r="G32" s="39">
         <f t="shared" si="1"/>
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H32" s="39">
         <f t="shared" si="2"/>
@@ -16485,7 +16501,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" si="3"/>
-        <v>-1124206600</v>
+        <v>-1127212500</v>
       </c>
       <c r="J32" s="56">
         <f t="shared" si="4"/>
@@ -16493,7 +16509,7 @@
       </c>
       <c r="K32" s="56">
         <f t="shared" si="5"/>
-        <v>-1124206600</v>
+        <v>-1127212500</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -16518,7 +16534,7 @@
       </c>
       <c r="G33" s="39">
         <f t="shared" si="1"/>
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H33" s="39">
         <f t="shared" si="2"/>
@@ -16526,7 +16542,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" si="3"/>
-        <v>-334021500</v>
+        <v>-334917000</v>
       </c>
       <c r="J33" s="56">
         <f t="shared" si="4"/>
@@ -16534,7 +16550,7 @@
       </c>
       <c r="K33" s="56">
         <f t="shared" si="5"/>
-        <v>-334021500</v>
+        <v>-334917000</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -16559,7 +16575,7 @@
       </c>
       <c r="G34" s="39">
         <f t="shared" si="1"/>
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H34" s="39">
         <f t="shared" si="2"/>
@@ -16571,11 +16587,11 @@
       </c>
       <c r="J34" s="56">
         <f t="shared" si="4"/>
-        <v>373000000</v>
+        <v>374000000</v>
       </c>
       <c r="K34" s="56">
         <f t="shared" si="5"/>
-        <v>-373000000</v>
+        <v>-374000000</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -16600,7 +16616,7 @@
       </c>
       <c r="G35" s="39">
         <f t="shared" si="1"/>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H35" s="39">
         <f t="shared" si="2"/>
@@ -16608,15 +16624,15 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" si="3"/>
-        <v>19047336</v>
+        <v>19099808</v>
       </c>
       <c r="J35" s="56">
         <f t="shared" si="4"/>
-        <v>-7863669</v>
+        <v>-7885332</v>
       </c>
       <c r="K35" s="56">
         <f t="shared" si="5"/>
-        <v>26911005</v>
+        <v>26985140</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -16641,7 +16657,7 @@
       </c>
       <c r="G36" s="39">
         <f t="shared" si="1"/>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H36" s="39">
         <f t="shared" si="2"/>
@@ -16653,11 +16669,11 @@
       </c>
       <c r="J36" s="56">
         <f t="shared" si="4"/>
-        <v>7885332</v>
+        <v>7906995</v>
       </c>
       <c r="K36" s="56">
         <f t="shared" si="5"/>
-        <v>-7885332</v>
+        <v>-7906995</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -16682,7 +16698,7 @@
       </c>
       <c r="G37" s="39">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H37" s="39">
         <f t="shared" si="2"/>
@@ -16690,7 +16706,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" si="3"/>
-        <v>-19470000</v>
+        <v>-19525000</v>
       </c>
       <c r="J37" s="56">
         <f t="shared" si="4"/>
@@ -16698,7 +16714,7 @@
       </c>
       <c r="K37" s="56">
         <f t="shared" si="5"/>
-        <v>-19470000</v>
+        <v>-19525000</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -16723,7 +16739,7 @@
       </c>
       <c r="G38" s="39">
         <f t="shared" si="1"/>
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H38" s="39">
         <f t="shared" si="2"/>
@@ -16731,11 +16747,11 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" si="3"/>
-        <v>1056000000</v>
+        <v>1059000000</v>
       </c>
       <c r="J38" s="56">
         <f t="shared" si="4"/>
-        <v>1056000000</v>
+        <v>1059000000</v>
       </c>
       <c r="K38" s="56">
         <f t="shared" si="5"/>
@@ -16764,7 +16780,7 @@
       </c>
       <c r="G39" s="39">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H39" s="39">
         <f t="shared" si="2"/>
@@ -16772,11 +16788,11 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" si="3"/>
-        <v>877500000</v>
+        <v>880000000</v>
       </c>
       <c r="J39" s="56">
         <f t="shared" si="4"/>
-        <v>877500000</v>
+        <v>880000000</v>
       </c>
       <c r="K39" s="56">
         <f t="shared" si="5"/>
@@ -16805,7 +16821,7 @@
       </c>
       <c r="G40" s="39">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H40" s="39">
         <f t="shared" si="2"/>
@@ -16813,7 +16829,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" si="3"/>
-        <v>-17600000</v>
+        <v>-17650000</v>
       </c>
       <c r="J40" s="56">
         <f t="shared" si="4"/>
@@ -16821,7 +16837,7 @@
       </c>
       <c r="K40" s="56">
         <f t="shared" si="5"/>
-        <v>-17600000</v>
+        <v>-17650000</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -16846,7 +16862,7 @@
       </c>
       <c r="G41" s="39">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H41" s="39">
         <f t="shared" si="2"/>
@@ -16854,7 +16870,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" si="3"/>
-        <v>1053000000</v>
+        <v>1056000000</v>
       </c>
       <c r="J41" s="56">
         <f t="shared" si="4"/>
@@ -16862,7 +16878,7 @@
       </c>
       <c r="K41" s="56">
         <f t="shared" si="5"/>
-        <v>1053000000</v>
+        <v>1056000000</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -16887,7 +16903,7 @@
       </c>
       <c r="G42" s="39">
         <f t="shared" si="1"/>
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H42" s="39">
         <f t="shared" si="2"/>
@@ -16895,7 +16911,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" si="3"/>
-        <v>-31130800</v>
+        <v>-31220000</v>
       </c>
       <c r="J42" s="56">
         <f t="shared" si="4"/>
@@ -16903,7 +16919,7 @@
       </c>
       <c r="K42" s="56">
         <f t="shared" si="5"/>
-        <v>-31130800</v>
+        <v>-31220000</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -16928,7 +16944,7 @@
       </c>
       <c r="G43" s="39">
         <f t="shared" si="1"/>
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H43" s="39">
         <f t="shared" si="2"/>
@@ -16936,7 +16952,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" si="3"/>
-        <v>-69000000</v>
+        <v>-69200000</v>
       </c>
       <c r="J43" s="56">
         <f t="shared" si="4"/>
@@ -16944,7 +16960,7 @@
       </c>
       <c r="K43" s="56">
         <f t="shared" si="5"/>
-        <v>-69000000</v>
+        <v>-69200000</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -16969,7 +16985,7 @@
       </c>
       <c r="G44" s="39">
         <f t="shared" si="1"/>
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H44" s="39">
         <f t="shared" si="2"/>
@@ -16977,7 +16993,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" si="3"/>
-        <v>-68600000</v>
+        <v>-68800000</v>
       </c>
       <c r="J44" s="56">
         <f t="shared" si="4"/>
@@ -16985,7 +17001,7 @@
       </c>
       <c r="K44" s="56">
         <f t="shared" si="5"/>
-        <v>-68600000</v>
+        <v>-68800000</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -17010,7 +17026,7 @@
       </c>
       <c r="G45" s="39">
         <f t="shared" si="1"/>
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H45" s="39">
         <f t="shared" si="2"/>
@@ -17018,7 +17034,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" si="3"/>
-        <v>-192080000</v>
+        <v>-192640000</v>
       </c>
       <c r="J45" s="56">
         <f t="shared" si="4"/>
@@ -17026,7 +17042,7 @@
       </c>
       <c r="K45" s="56">
         <f t="shared" si="5"/>
-        <v>-192080000</v>
+        <v>-192640000</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -17051,7 +17067,7 @@
       </c>
       <c r="G46" s="39">
         <f t="shared" si="1"/>
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H46" s="39">
         <f t="shared" si="2"/>
@@ -17059,7 +17075,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" si="3"/>
-        <v>-239164500</v>
+        <v>-239870000</v>
       </c>
       <c r="J46" s="56">
         <f t="shared" si="4"/>
@@ -17067,7 +17083,7 @@
       </c>
       <c r="K46" s="56">
         <f t="shared" si="5"/>
-        <v>-239164500</v>
+        <v>-239870000</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -17092,7 +17108,7 @@
       </c>
       <c r="G47" s="39">
         <f t="shared" si="1"/>
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H47" s="39">
         <f t="shared" si="2"/>
@@ -17100,15 +17116,15 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" si="3"/>
-        <v>13679728</v>
+        <v>13720932</v>
       </c>
       <c r="J47" s="56">
         <f t="shared" si="4"/>
-        <v>2228716</v>
+        <v>2235429</v>
       </c>
       <c r="K47" s="56">
         <f t="shared" si="5"/>
-        <v>11451012</v>
+        <v>11485503</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -17133,7 +17149,7 @@
       </c>
       <c r="G48" s="39">
         <f t="shared" si="1"/>
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H48" s="39">
         <f t="shared" si="2"/>
@@ -17141,7 +17157,7 @@
       </c>
       <c r="I48" s="11">
         <f t="shared" si="3"/>
-        <v>565960400</v>
+        <v>567665100</v>
       </c>
       <c r="J48" s="56">
         <f t="shared" si="4"/>
@@ -17149,7 +17165,7 @@
       </c>
       <c r="K48" s="56">
         <f t="shared" si="5"/>
-        <v>565960400</v>
+        <v>567665100</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -17174,7 +17190,7 @@
       </c>
       <c r="G49" s="39">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H49" s="39">
         <f t="shared" si="2"/>
@@ -17182,7 +17198,7 @@
       </c>
       <c r="I49" s="11">
         <f t="shared" si="3"/>
-        <v>-50220000</v>
+        <v>-50375000</v>
       </c>
       <c r="J49" s="56">
         <f t="shared" si="4"/>
@@ -17190,7 +17206,7 @@
       </c>
       <c r="K49" s="56">
         <f t="shared" si="5"/>
-        <v>-50220000</v>
+        <v>-50375000</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -17215,7 +17231,7 @@
       </c>
       <c r="G50" s="39">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H50" s="39">
         <f t="shared" si="2"/>
@@ -17223,7 +17239,7 @@
       </c>
       <c r="I50" s="11">
         <f t="shared" si="3"/>
-        <v>-44712000</v>
+        <v>-44850000</v>
       </c>
       <c r="J50" s="56">
         <f t="shared" si="4"/>
@@ -17231,7 +17247,7 @@
       </c>
       <c r="K50" s="56">
         <f t="shared" si="5"/>
-        <v>-44712000</v>
+        <v>-44850000</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -17256,7 +17272,7 @@
       </c>
       <c r="G51" s="39">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H51" s="39">
         <f t="shared" si="2"/>
@@ -17264,7 +17280,7 @@
       </c>
       <c r="I51" s="11">
         <f t="shared" si="3"/>
-        <v>-239760000</v>
+        <v>-240500000</v>
       </c>
       <c r="J51" s="56">
         <f t="shared" si="4"/>
@@ -17272,7 +17288,7 @@
       </c>
       <c r="K51" s="56">
         <f t="shared" si="5"/>
-        <v>-239760000</v>
+        <v>-240500000</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -17297,7 +17313,7 @@
       </c>
       <c r="G52" s="39">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H52" s="39">
         <f t="shared" si="2"/>
@@ -17305,7 +17321,7 @@
       </c>
       <c r="I52" s="11">
         <f t="shared" si="3"/>
-        <v>-64800000</v>
+        <v>-65000000</v>
       </c>
       <c r="J52" s="56">
         <f t="shared" si="4"/>
@@ -17313,7 +17329,7 @@
       </c>
       <c r="K52" s="56">
         <f t="shared" si="5"/>
-        <v>-64800000</v>
+        <v>-65000000</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -17338,7 +17354,7 @@
       </c>
       <c r="G53" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H53" s="39">
         <f t="shared" si="2"/>
@@ -17346,7 +17362,7 @@
       </c>
       <c r="I53" s="11">
         <f t="shared" si="3"/>
-        <v>-340765000</v>
+        <v>-341820000</v>
       </c>
       <c r="J53" s="56">
         <f t="shared" si="4"/>
@@ -17354,7 +17370,7 @@
       </c>
       <c r="K53" s="56">
         <f t="shared" si="5"/>
-        <v>-340765000</v>
+        <v>-341820000</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -17379,7 +17395,7 @@
       </c>
       <c r="G54" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H54" s="39">
         <f t="shared" si="2"/>
@@ -17387,7 +17403,7 @@
       </c>
       <c r="I54" s="11">
         <f t="shared" si="3"/>
-        <v>-64600000</v>
+        <v>-64800000</v>
       </c>
       <c r="J54" s="56">
         <f t="shared" si="4"/>
@@ -17395,7 +17411,7 @@
       </c>
       <c r="K54" s="56">
         <f t="shared" si="5"/>
-        <v>-64600000</v>
+        <v>-64800000</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -17420,7 +17436,7 @@
       </c>
       <c r="G55" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H55" s="39">
         <f t="shared" si="2"/>
@@ -17428,7 +17444,7 @@
       </c>
       <c r="I55" s="11">
         <f t="shared" si="3"/>
-        <v>-323161500</v>
+        <v>-324162000</v>
       </c>
       <c r="J55" s="56">
         <f t="shared" si="4"/>
@@ -17436,7 +17452,7 @@
       </c>
       <c r="K55" s="56">
         <f t="shared" si="5"/>
-        <v>-323161500</v>
+        <v>-324162000</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -17461,7 +17477,7 @@
       </c>
       <c r="G56" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H56" s="39">
         <f t="shared" si="2"/>
@@ -17469,7 +17485,7 @@
       </c>
       <c r="I56" s="11">
         <f t="shared" si="3"/>
-        <v>-12274000</v>
+        <v>-12312000</v>
       </c>
       <c r="J56" s="56">
         <f t="shared" si="4"/>
@@ -17477,7 +17493,7 @@
       </c>
       <c r="K56" s="56">
         <f t="shared" si="5"/>
-        <v>-12274000</v>
+        <v>-12312000</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -17502,7 +17518,7 @@
       </c>
       <c r="G57" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H57" s="39">
         <f t="shared" si="2"/>
@@ -17510,7 +17526,7 @@
       </c>
       <c r="I57" s="11">
         <f t="shared" si="3"/>
-        <v>-33915000</v>
+        <v>-34020000</v>
       </c>
       <c r="J57" s="56">
         <f t="shared" si="4"/>
@@ -17518,7 +17534,7 @@
       </c>
       <c r="K57" s="56">
         <f t="shared" si="5"/>
-        <v>-33915000</v>
+        <v>-34020000</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -17543,7 +17559,7 @@
       </c>
       <c r="G58" s="39">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H58" s="39">
         <f t="shared" si="2"/>
@@ -17551,7 +17567,7 @@
       </c>
       <c r="I58" s="11">
         <f t="shared" si="3"/>
-        <v>-19380000</v>
+        <v>-19440000</v>
       </c>
       <c r="J58" s="56">
         <f t="shared" si="4"/>
@@ -17559,7 +17575,7 @@
       </c>
       <c r="K58" s="56">
         <f t="shared" si="5"/>
-        <v>-19380000</v>
+        <v>-19440000</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -17584,7 +17600,7 @@
       </c>
       <c r="G59" s="39">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H59" s="39">
         <f t="shared" si="2"/>
@@ -17592,11 +17608,11 @@
       </c>
       <c r="I59" s="11">
         <f t="shared" si="3"/>
-        <v>319000000</v>
+        <v>320000000</v>
       </c>
       <c r="J59" s="56">
         <f t="shared" si="4"/>
-        <v>319000000</v>
+        <v>320000000</v>
       </c>
       <c r="K59" s="56">
         <f t="shared" si="5"/>
@@ -17625,7 +17641,7 @@
       </c>
       <c r="G60" s="39">
         <f t="shared" si="1"/>
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H60" s="39">
         <f t="shared" si="2"/>
@@ -17633,11 +17649,11 @@
       </c>
       <c r="I60" s="11">
         <f t="shared" si="3"/>
-        <v>1113000000</v>
+        <v>1116500000</v>
       </c>
       <c r="J60" s="56">
         <f t="shared" si="4"/>
-        <v>1113000000</v>
+        <v>1116500000</v>
       </c>
       <c r="K60" s="56">
         <f t="shared" si="5"/>
@@ -17666,7 +17682,7 @@
       </c>
       <c r="G61" s="39">
         <f t="shared" si="1"/>
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H61" s="39">
         <f t="shared" si="2"/>
@@ -17674,11 +17690,11 @@
       </c>
       <c r="I61" s="11">
         <f t="shared" si="3"/>
-        <v>316000000</v>
+        <v>317000000</v>
       </c>
       <c r="J61" s="56">
         <f t="shared" si="4"/>
-        <v>316000000</v>
+        <v>317000000</v>
       </c>
       <c r="K61" s="56">
         <f t="shared" si="5"/>
@@ -17707,7 +17723,7 @@
       </c>
       <c r="G62" s="39">
         <f t="shared" si="1"/>
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H62" s="39">
         <f t="shared" si="2"/>
@@ -17715,11 +17731,11 @@
       </c>
       <c r="I62" s="11">
         <f t="shared" si="3"/>
-        <v>948000000</v>
+        <v>951000000</v>
       </c>
       <c r="J62" s="56">
         <f t="shared" si="4"/>
-        <v>948000000</v>
+        <v>951000000</v>
       </c>
       <c r="K62" s="56">
         <f t="shared" si="5"/>
@@ -17748,7 +17764,7 @@
       </c>
       <c r="G63" s="39">
         <f t="shared" si="1"/>
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H63" s="39">
         <f t="shared" si="2"/>
@@ -17756,7 +17772,7 @@
       </c>
       <c r="I63" s="11">
         <f t="shared" si="3"/>
-        <v>-63000000</v>
+        <v>-63200000</v>
       </c>
       <c r="J63" s="56">
         <f t="shared" si="4"/>
@@ -17764,7 +17780,7 @@
       </c>
       <c r="K63" s="56">
         <f t="shared" si="5"/>
-        <v>-63000000</v>
+        <v>-63200000</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -17789,7 +17805,7 @@
       </c>
       <c r="G64" s="39">
         <f t="shared" si="1"/>
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H64" s="39">
         <f t="shared" si="2"/>
@@ -17797,7 +17813,7 @@
       </c>
       <c r="I64" s="11">
         <f t="shared" si="3"/>
-        <v>-15500000</v>
+        <v>-15550000</v>
       </c>
       <c r="J64" s="56">
         <f t="shared" si="4"/>
@@ -17805,7 +17821,7 @@
       </c>
       <c r="K64" s="56">
         <f t="shared" si="5"/>
-        <v>-15500000</v>
+        <v>-15550000</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -17830,7 +17846,7 @@
       </c>
       <c r="G65" s="39">
         <f t="shared" si="1"/>
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H65" s="39">
         <f t="shared" si="2"/>
@@ -17838,7 +17854,7 @@
       </c>
       <c r="I65" s="11">
         <f t="shared" si="3"/>
-        <v>-61200000</v>
+        <v>-61400000</v>
       </c>
       <c r="J65" s="56">
         <f t="shared" si="4"/>
@@ -17846,7 +17862,7 @@
       </c>
       <c r="K65" s="56">
         <f t="shared" si="5"/>
-        <v>-61200000</v>
+        <v>-61400000</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -17871,7 +17887,7 @@
       </c>
       <c r="G66" s="39">
         <f t="shared" si="1"/>
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H66" s="39">
         <f t="shared" si="2"/>
@@ -17879,7 +17895,7 @@
       </c>
       <c r="I66" s="11">
         <f t="shared" si="3"/>
-        <v>-51510000</v>
+        <v>-51680000</v>
       </c>
       <c r="J66" s="56">
         <f t="shared" si="4"/>
@@ -17887,7 +17903,7 @@
       </c>
       <c r="K66" s="56">
         <f t="shared" si="5"/>
-        <v>-51510000</v>
+        <v>-51680000</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -17912,23 +17928,23 @@
       </c>
       <c r="G67" s="39">
         <f t="shared" ref="G67:G128" si="7">G68+F67</f>
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H67" s="39">
-        <f t="shared" ref="H67:H122" si="8">IF(B67&gt;0,1,0)</f>
+        <f t="shared" ref="H67:H123" si="8">IF(B67&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="I67" s="11">
         <f t="shared" ref="I67:I119" si="9">B67*(G67-H67)</f>
-        <v>27488825</v>
+        <v>27580150</v>
       </c>
       <c r="J67" s="56">
-        <f t="shared" ref="J67:J122" si="10">C67*(G67-H67)</f>
-        <v>19782623</v>
+        <f t="shared" ref="J67:J123" si="10">C67*(G67-H67)</f>
+        <v>19848346</v>
       </c>
       <c r="K67" s="56">
-        <f t="shared" ref="K67:K122" si="11">D67*(G67-H67)</f>
-        <v>7706202</v>
+        <f t="shared" ref="K67:K123" si="11">D67*(G67-H67)</f>
+        <v>7731804</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -17953,7 +17969,7 @@
       </c>
       <c r="G68" s="39">
         <f t="shared" si="7"/>
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H68" s="39">
         <f t="shared" si="8"/>
@@ -17961,7 +17977,7 @@
       </c>
       <c r="I68" s="11">
         <f t="shared" si="9"/>
-        <v>-41180000</v>
+        <v>-41325000</v>
       </c>
       <c r="J68" s="56">
         <f t="shared" si="10"/>
@@ -17969,7 +17985,7 @@
       </c>
       <c r="K68" s="56">
         <f t="shared" si="11"/>
-        <v>-41180000</v>
+        <v>-41325000</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -17994,7 +18010,7 @@
       </c>
       <c r="G69" s="39">
         <f t="shared" si="7"/>
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H69" s="39">
         <f t="shared" si="8"/>
@@ -18002,7 +18018,7 @@
       </c>
       <c r="I69" s="11">
         <f t="shared" si="9"/>
-        <v>270480000</v>
+        <v>271460000</v>
       </c>
       <c r="J69" s="56">
         <f t="shared" si="10"/>
@@ -18010,7 +18026,7 @@
       </c>
       <c r="K69" s="56">
         <f t="shared" si="11"/>
-        <v>270480000</v>
+        <v>271460000</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -18035,7 +18051,7 @@
       </c>
       <c r="G70" s="39">
         <f t="shared" si="7"/>
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H70" s="39">
         <f t="shared" si="8"/>
@@ -18043,7 +18059,7 @@
       </c>
       <c r="I70" s="11">
         <f t="shared" si="9"/>
-        <v>-12604000</v>
+        <v>-12650000</v>
       </c>
       <c r="J70" s="56">
         <f t="shared" si="10"/>
@@ -18051,7 +18067,7 @@
       </c>
       <c r="K70" s="56">
         <f t="shared" si="11"/>
-        <v>-12604000</v>
+        <v>-12650000</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -18076,7 +18092,7 @@
       </c>
       <c r="G71" s="39">
         <f t="shared" si="7"/>
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H71" s="39">
         <f t="shared" si="8"/>
@@ -18084,15 +18100,15 @@
       </c>
       <c r="I71" s="11">
         <f t="shared" si="9"/>
-        <v>31256598</v>
+        <v>31371936</v>
       </c>
       <c r="J71" s="56">
         <f t="shared" si="10"/>
-        <v>28133052</v>
+        <v>28236864</v>
       </c>
       <c r="K71" s="56">
         <f t="shared" si="11"/>
-        <v>3123546</v>
+        <v>3135072</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -18117,7 +18133,7 @@
       </c>
       <c r="G72" s="39">
         <f t="shared" si="7"/>
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H72" s="39">
         <f t="shared" si="8"/>
@@ -18125,7 +18141,7 @@
       </c>
       <c r="I72" s="11">
         <f t="shared" si="9"/>
-        <v>-41183599</v>
+        <v>-41335568</v>
       </c>
       <c r="J72" s="56">
         <f t="shared" si="10"/>
@@ -18133,7 +18149,7 @@
       </c>
       <c r="K72" s="56">
         <f t="shared" si="11"/>
-        <v>-41183599</v>
+        <v>-41335568</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -18158,7 +18174,7 @@
       </c>
       <c r="G73" s="39">
         <f t="shared" si="7"/>
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H73" s="39">
         <f t="shared" si="8"/>
@@ -18166,7 +18182,7 @@
       </c>
       <c r="I73" s="11">
         <f t="shared" si="9"/>
-        <v>-217485000</v>
+        <v>-218290500</v>
       </c>
       <c r="J73" s="56">
         <f t="shared" si="10"/>
@@ -18174,7 +18190,7 @@
       </c>
       <c r="K73" s="56">
         <f t="shared" si="11"/>
-        <v>-217485000</v>
+        <v>-218290500</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -18199,7 +18215,7 @@
       </c>
       <c r="G74" s="39">
         <f t="shared" si="7"/>
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H74" s="39">
         <f t="shared" si="8"/>
@@ -18207,7 +18223,7 @@
       </c>
       <c r="I74" s="11">
         <f t="shared" si="9"/>
-        <v>1832690000</v>
+        <v>1839685000</v>
       </c>
       <c r="J74" s="56">
         <f t="shared" si="10"/>
@@ -18215,7 +18231,7 @@
       </c>
       <c r="K74" s="56">
         <f t="shared" si="11"/>
-        <v>1832690000</v>
+        <v>1839685000</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -18240,7 +18256,7 @@
       </c>
       <c r="G75" s="39">
         <f t="shared" si="7"/>
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H75" s="39">
         <f t="shared" si="8"/>
@@ -18248,7 +18264,7 @@
       </c>
       <c r="I75" s="11">
         <f t="shared" si="9"/>
-        <v>783000000</v>
+        <v>786000000</v>
       </c>
       <c r="J75" s="56">
         <f t="shared" si="10"/>
@@ -18256,7 +18272,7 @@
       </c>
       <c r="K75" s="56">
         <f t="shared" si="11"/>
-        <v>783000000</v>
+        <v>786000000</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -18281,7 +18297,7 @@
       </c>
       <c r="G76" s="39">
         <f t="shared" si="7"/>
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H76" s="39">
         <f t="shared" si="8"/>
@@ -18289,7 +18305,7 @@
       </c>
       <c r="I76" s="11">
         <f t="shared" si="9"/>
-        <v>777000000</v>
+        <v>780000000</v>
       </c>
       <c r="J76" s="56">
         <f t="shared" si="10"/>
@@ -18297,7 +18313,7 @@
       </c>
       <c r="K76" s="56">
         <f t="shared" si="11"/>
-        <v>777000000</v>
+        <v>780000000</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -18322,7 +18338,7 @@
       </c>
       <c r="G77" s="39">
         <f t="shared" si="7"/>
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H77" s="39">
         <f t="shared" si="8"/>
@@ -18330,7 +18346,7 @@
       </c>
       <c r="I77" s="11">
         <f t="shared" si="9"/>
-        <v>774000000</v>
+        <v>777000000</v>
       </c>
       <c r="J77" s="56">
         <f t="shared" si="10"/>
@@ -18338,7 +18354,7 @@
       </c>
       <c r="K77" s="56">
         <f t="shared" si="11"/>
-        <v>774000000</v>
+        <v>777000000</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -18363,7 +18379,7 @@
       </c>
       <c r="G78" s="39">
         <f t="shared" si="7"/>
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H78" s="39">
         <f t="shared" si="8"/>
@@ -18371,11 +18387,11 @@
       </c>
       <c r="I78" s="11">
         <f t="shared" si="9"/>
-        <v>-825600000</v>
+        <v>-828800000</v>
       </c>
       <c r="J78" s="56">
         <f t="shared" si="10"/>
-        <v>-825600000</v>
+        <v>-828800000</v>
       </c>
       <c r="K78" s="56">
         <f t="shared" si="11"/>
@@ -18404,7 +18420,7 @@
       </c>
       <c r="G79" s="39">
         <f t="shared" si="7"/>
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H79" s="39">
         <f t="shared" si="8"/>
@@ -18412,11 +18428,11 @@
       </c>
       <c r="I79" s="11">
         <f t="shared" si="9"/>
-        <v>-205600000</v>
+        <v>-206400000</v>
       </c>
       <c r="J79" s="56">
         <f t="shared" si="10"/>
-        <v>-205600000</v>
+        <v>-206400000</v>
       </c>
       <c r="K79" s="56">
         <f t="shared" si="11"/>
@@ -18445,7 +18461,7 @@
       </c>
       <c r="G80" s="39">
         <f t="shared" si="7"/>
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H80" s="39">
         <f t="shared" si="8"/>
@@ -18453,7 +18469,7 @@
       </c>
       <c r="I80" s="11">
         <f t="shared" si="9"/>
-        <v>-12388608</v>
+        <v>-12437001</v>
       </c>
       <c r="J80" s="56">
         <f t="shared" si="10"/>
@@ -18461,7 +18477,7 @@
       </c>
       <c r="K80" s="56">
         <f t="shared" si="11"/>
-        <v>-12388608</v>
+        <v>-12437001</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -18486,7 +18502,7 @@
       </c>
       <c r="G81" s="39">
         <f t="shared" si="7"/>
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H81" s="39">
         <f t="shared" si="8"/>
@@ -18494,7 +18510,7 @@
       </c>
       <c r="I81" s="11">
         <f t="shared" si="9"/>
-        <v>-35700000</v>
+        <v>-35840000</v>
       </c>
       <c r="J81" s="56">
         <f t="shared" si="10"/>
@@ -18502,7 +18518,7 @@
       </c>
       <c r="K81" s="56">
         <f t="shared" si="11"/>
-        <v>-35700000</v>
+        <v>-35840000</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -18527,7 +18543,7 @@
       </c>
       <c r="G82" s="39">
         <f t="shared" si="7"/>
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H82" s="39">
         <f t="shared" si="8"/>
@@ -18535,7 +18551,7 @@
       </c>
       <c r="I82" s="11">
         <f t="shared" si="9"/>
-        <v>-63500000</v>
+        <v>-63750000</v>
       </c>
       <c r="J82" s="56">
         <f t="shared" si="10"/>
@@ -18543,7 +18559,7 @@
       </c>
       <c r="K82" s="56">
         <f t="shared" si="11"/>
-        <v>-63500000</v>
+        <v>-63750000</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -18568,7 +18584,7 @@
       </c>
       <c r="G83" s="39">
         <f t="shared" si="7"/>
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H83" s="39">
         <f t="shared" si="8"/>
@@ -18576,7 +18592,7 @@
       </c>
       <c r="I83" s="11">
         <f t="shared" si="9"/>
-        <v>-50600000</v>
+        <v>-50800000</v>
       </c>
       <c r="J83" s="56">
         <f t="shared" si="10"/>
@@ -18584,7 +18600,7 @@
       </c>
       <c r="K83" s="56">
         <f t="shared" si="11"/>
-        <v>-50600000</v>
+        <v>-50800000</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -18609,7 +18625,7 @@
       </c>
       <c r="G84" s="39">
         <f t="shared" si="7"/>
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H84" s="39">
         <f t="shared" si="8"/>
@@ -18617,7 +18633,7 @@
       </c>
       <c r="I84" s="11">
         <f t="shared" si="9"/>
-        <v>407164800</v>
+        <v>408800000</v>
       </c>
       <c r="J84" s="56">
         <f t="shared" si="10"/>
@@ -18625,7 +18641,7 @@
       </c>
       <c r="K84" s="56">
         <f t="shared" si="11"/>
-        <v>407164800</v>
+        <v>408800000</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -18650,7 +18666,7 @@
       </c>
       <c r="G85" s="39">
         <f t="shared" si="7"/>
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H85" s="39">
         <f t="shared" si="8"/>
@@ -18658,7 +18674,7 @@
       </c>
       <c r="I85" s="11">
         <f t="shared" si="9"/>
-        <v>612500000</v>
+        <v>615000000</v>
       </c>
       <c r="J85" s="56">
         <f t="shared" si="10"/>
@@ -18666,7 +18682,7 @@
       </c>
       <c r="K85" s="56">
         <f t="shared" si="11"/>
-        <v>612500000</v>
+        <v>615000000</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -18691,7 +18707,7 @@
       </c>
       <c r="G86" s="39">
         <f t="shared" si="7"/>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H86" s="39">
         <f t="shared" si="8"/>
@@ -18699,15 +18715,15 @@
       </c>
       <c r="I86" s="11">
         <f t="shared" si="9"/>
-        <v>44898300</v>
+        <v>45084600</v>
       </c>
       <c r="J86" s="56">
         <f t="shared" si="10"/>
-        <v>20472950</v>
+        <v>20557900</v>
       </c>
       <c r="K86" s="56">
         <f t="shared" si="11"/>
-        <v>24425350</v>
+        <v>24526700</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -18732,7 +18748,7 @@
       </c>
       <c r="G87" s="39">
         <f t="shared" si="7"/>
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H87" s="39">
         <f t="shared" si="8"/>
@@ -18740,7 +18756,7 @@
       </c>
       <c r="I87" s="11">
         <f t="shared" si="9"/>
-        <v>-47800000</v>
+        <v>-48000000</v>
       </c>
       <c r="J87" s="56">
         <f t="shared" si="10"/>
@@ -18748,7 +18764,7 @@
       </c>
       <c r="K87" s="56">
         <f t="shared" si="11"/>
-        <v>-47800000</v>
+        <v>-48000000</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -18773,7 +18789,7 @@
       </c>
       <c r="G88" s="39">
         <f t="shared" si="7"/>
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H88" s="39">
         <f t="shared" si="8"/>
@@ -18781,15 +18797,15 @@
       </c>
       <c r="I88" s="11">
         <f t="shared" si="9"/>
-        <v>-28084000</v>
+        <v>-28202000</v>
       </c>
       <c r="J88" s="56">
         <f t="shared" si="10"/>
-        <v>-16422000</v>
+        <v>-16491000</v>
       </c>
       <c r="K88" s="56">
         <f t="shared" si="11"/>
-        <v>-11662000</v>
+        <v>-11711000</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -18814,7 +18830,7 @@
       </c>
       <c r="G89" s="39">
         <f t="shared" si="7"/>
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H89" s="39">
         <f t="shared" si="8"/>
@@ -18822,7 +18838,7 @@
       </c>
       <c r="I89" s="11">
         <f t="shared" si="9"/>
-        <v>-736207000</v>
+        <v>-739407900</v>
       </c>
       <c r="J89" s="56">
         <f t="shared" si="10"/>
@@ -18830,7 +18846,7 @@
       </c>
       <c r="K89" s="56">
         <f t="shared" si="11"/>
-        <v>-736207000</v>
+        <v>-739407900</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -18855,7 +18871,7 @@
       </c>
       <c r="G90" s="39">
         <f t="shared" si="7"/>
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H90" s="39">
         <f t="shared" si="8"/>
@@ -18863,7 +18879,7 @@
       </c>
       <c r="I90" s="11">
         <f t="shared" si="9"/>
-        <v>-733006100</v>
+        <v>-736207000</v>
       </c>
       <c r="J90" s="56">
         <f t="shared" si="10"/>
@@ -18871,7 +18887,7 @@
       </c>
       <c r="K90" s="56">
         <f t="shared" si="11"/>
-        <v>-733006100</v>
+        <v>-736207000</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -18896,7 +18912,7 @@
       </c>
       <c r="G91" s="39">
         <f t="shared" si="7"/>
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H91" s="39">
         <f t="shared" si="8"/>
@@ -18904,7 +18920,7 @@
       </c>
       <c r="I91" s="11">
         <f t="shared" si="9"/>
-        <v>-729805200</v>
+        <v>-733006100</v>
       </c>
       <c r="J91" s="56">
         <f t="shared" si="10"/>
@@ -18912,7 +18928,7 @@
       </c>
       <c r="K91" s="56">
         <f t="shared" si="11"/>
-        <v>-729805200</v>
+        <v>-733006100</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -18937,7 +18953,7 @@
       </c>
       <c r="G92" s="39">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H92" s="39">
         <f t="shared" si="8"/>
@@ -18945,7 +18961,7 @@
       </c>
       <c r="I92" s="11">
         <f t="shared" si="9"/>
-        <v>-726604300</v>
+        <v>-729805200</v>
       </c>
       <c r="J92" s="56">
         <f t="shared" si="10"/>
@@ -18953,7 +18969,7 @@
       </c>
       <c r="K92" s="56">
         <f t="shared" si="11"/>
-        <v>-726604300</v>
+        <v>-729805200</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -18978,7 +18994,7 @@
       </c>
       <c r="G93" s="39">
         <f t="shared" si="7"/>
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H93" s="39">
         <f t="shared" si="8"/>
@@ -18986,7 +19002,7 @@
       </c>
       <c r="I93" s="11">
         <f t="shared" si="9"/>
-        <v>-723403400</v>
+        <v>-726604300</v>
       </c>
       <c r="J93" s="56">
         <f t="shared" si="10"/>
@@ -18994,7 +19010,7 @@
       </c>
       <c r="K93" s="56">
         <f t="shared" si="11"/>
-        <v>-723403400</v>
+        <v>-726604300</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -19019,7 +19035,7 @@
       </c>
       <c r="G94" s="39">
         <f t="shared" si="7"/>
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H94" s="39">
         <f t="shared" si="8"/>
@@ -19027,7 +19043,7 @@
       </c>
       <c r="I94" s="11">
         <f t="shared" si="9"/>
-        <v>-720202500</v>
+        <v>-723403400</v>
       </c>
       <c r="J94" s="56">
         <f t="shared" si="10"/>
@@ -19035,7 +19051,7 @@
       </c>
       <c r="K94" s="56">
         <f t="shared" si="11"/>
-        <v>-720202500</v>
+        <v>-723403400</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -19060,7 +19076,7 @@
       </c>
       <c r="G95" s="39">
         <f t="shared" si="7"/>
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H95" s="39">
         <f t="shared" si="8"/>
@@ -19068,7 +19084,7 @@
       </c>
       <c r="I95" s="11">
         <f t="shared" si="9"/>
-        <v>-266840908</v>
+        <v>-268037504</v>
       </c>
       <c r="J95" s="56">
         <f t="shared" si="10"/>
@@ -19076,7 +19092,7 @@
       </c>
       <c r="K95" s="56">
         <f t="shared" si="11"/>
-        <v>-266840908</v>
+        <v>-268037504</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -19101,7 +19117,7 @@
       </c>
       <c r="G96" s="39">
         <f t="shared" si="7"/>
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H96" s="39">
         <f t="shared" si="8"/>
@@ -19109,7 +19125,7 @@
       </c>
       <c r="I96" s="11">
         <f t="shared" si="9"/>
-        <v>-42600000</v>
+        <v>-42800000</v>
       </c>
       <c r="J96" s="56">
         <f t="shared" si="10"/>
@@ -19117,7 +19133,7 @@
       </c>
       <c r="K96" s="56">
         <f t="shared" si="11"/>
-        <v>-42600000</v>
+        <v>-42800000</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -19142,7 +19158,7 @@
       </c>
       <c r="G97" s="39">
         <f t="shared" si="7"/>
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H97" s="39">
         <f t="shared" si="8"/>
@@ -19150,15 +19166,15 @@
       </c>
       <c r="I97" s="11">
         <f t="shared" si="9"/>
-        <v>33666738</v>
+        <v>33826296</v>
       </c>
       <c r="J97" s="56">
         <f t="shared" si="10"/>
-        <v>14543386</v>
+        <v>14612312</v>
       </c>
       <c r="K97" s="56">
         <f t="shared" si="11"/>
-        <v>19123352</v>
+        <v>19213984</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -19183,7 +19199,7 @@
       </c>
       <c r="G98" s="39">
         <f t="shared" si="7"/>
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H98" s="39">
         <f t="shared" si="8"/>
@@ -19191,7 +19207,7 @@
       </c>
       <c r="I98" s="11">
         <f t="shared" si="9"/>
-        <v>23559808</v>
+        <v>23674176</v>
       </c>
       <c r="J98" s="56">
         <f t="shared" si="10"/>
@@ -19199,7 +19215,7 @@
       </c>
       <c r="K98" s="56">
         <f t="shared" si="11"/>
-        <v>23559808</v>
+        <v>23674176</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -19224,7 +19240,7 @@
       </c>
       <c r="G99" s="39">
         <f t="shared" si="7"/>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H99" s="39">
         <f t="shared" si="8"/>
@@ -19232,7 +19248,7 @@
       </c>
       <c r="I99" s="11">
         <f t="shared" si="9"/>
-        <v>-270300000</v>
+        <v>-271625000</v>
       </c>
       <c r="J99" s="56">
         <f t="shared" si="10"/>
@@ -19240,7 +19256,7 @@
       </c>
       <c r="K99" s="56">
         <f t="shared" si="11"/>
-        <v>-270300000</v>
+        <v>-271625000</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -19265,7 +19281,7 @@
       </c>
       <c r="G100" s="39">
         <f t="shared" si="7"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H100" s="39">
         <f t="shared" si="8"/>
@@ -19273,7 +19289,7 @@
       </c>
       <c r="I100" s="11">
         <f t="shared" si="9"/>
-        <v>262350000</v>
+        <v>263675000</v>
       </c>
       <c r="J100" s="56">
         <f t="shared" si="10"/>
@@ -19281,7 +19297,7 @@
       </c>
       <c r="K100" s="56">
         <f t="shared" si="11"/>
-        <v>262350000</v>
+        <v>263675000</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -19306,7 +19322,7 @@
       </c>
       <c r="G101" s="39">
         <f t="shared" si="7"/>
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H101" s="39">
         <f t="shared" si="8"/>
@@ -19314,11 +19330,11 @@
       </c>
       <c r="I101" s="11">
         <f t="shared" si="9"/>
-        <v>12098945</v>
+        <v>12165790</v>
       </c>
       <c r="J101" s="56">
         <f t="shared" si="10"/>
-        <v>12098945</v>
+        <v>12165790</v>
       </c>
       <c r="K101" s="56">
         <f t="shared" si="11"/>
@@ -19347,7 +19363,7 @@
       </c>
       <c r="G102" s="39">
         <f t="shared" si="7"/>
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H102" s="39">
         <f t="shared" si="8"/>
@@ -19355,7 +19371,7 @@
       </c>
       <c r="I102" s="11">
         <f t="shared" si="9"/>
-        <v>534000000</v>
+        <v>537000000</v>
       </c>
       <c r="J102" s="56">
         <f t="shared" si="10"/>
@@ -19363,7 +19379,7 @@
       </c>
       <c r="K102" s="56">
         <f t="shared" si="11"/>
-        <v>534000000</v>
+        <v>537000000</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -19388,7 +19404,7 @@
       </c>
       <c r="G103" s="39">
         <f t="shared" si="7"/>
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H103" s="39">
         <f t="shared" si="8"/>
@@ -19396,11 +19412,11 @@
       </c>
       <c r="I103" s="11">
         <f t="shared" si="9"/>
-        <v>-172000000</v>
+        <v>-173000000</v>
       </c>
       <c r="J103" s="56">
         <f t="shared" si="10"/>
-        <v>-172000000</v>
+        <v>-173000000</v>
       </c>
       <c r="K103" s="56">
         <f t="shared" si="11"/>
@@ -19429,7 +19445,7 @@
       </c>
       <c r="G104" s="39">
         <f t="shared" si="7"/>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H104" s="39">
         <f t="shared" si="8"/>
@@ -19437,11 +19453,11 @@
       </c>
       <c r="I104" s="11">
         <f t="shared" si="9"/>
-        <v>483000000</v>
+        <v>486000000</v>
       </c>
       <c r="J104" s="56">
         <f t="shared" si="10"/>
-        <v>483000000</v>
+        <v>486000000</v>
       </c>
       <c r="K104" s="56">
         <f t="shared" si="11"/>
@@ -19470,7 +19486,7 @@
       </c>
       <c r="G105" s="39">
         <f t="shared" si="7"/>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H105" s="39">
         <f t="shared" si="8"/>
@@ -19478,11 +19494,11 @@
       </c>
       <c r="I105" s="11">
         <f t="shared" si="9"/>
-        <v>179200000</v>
+        <v>180320000</v>
       </c>
       <c r="J105" s="56">
         <f t="shared" si="10"/>
-        <v>179200000</v>
+        <v>180320000</v>
       </c>
       <c r="K105" s="56">
         <f t="shared" si="11"/>
@@ -19511,7 +19527,7 @@
       </c>
       <c r="G106" s="39">
         <f t="shared" si="7"/>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H106" s="39">
         <f t="shared" si="8"/>
@@ -19519,7 +19535,7 @@
       </c>
       <c r="I106" s="11">
         <f t="shared" si="9"/>
-        <v>-483000000</v>
+        <v>-486000000</v>
       </c>
       <c r="J106" s="56">
         <f t="shared" si="10"/>
@@ -19527,7 +19543,7 @@
       </c>
       <c r="K106" s="56">
         <f t="shared" si="11"/>
-        <v>-483000000</v>
+        <v>-486000000</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -19552,7 +19568,7 @@
       </c>
       <c r="G107" s="39">
         <f t="shared" si="7"/>
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H107" s="39">
         <f t="shared" si="8"/>
@@ -19560,15 +19576,15 @@
       </c>
       <c r="I107" s="11">
         <f t="shared" si="9"/>
-        <v>13664594</v>
+        <v>13755088</v>
       </c>
       <c r="J107" s="56">
         <f t="shared" si="10"/>
-        <v>11342365</v>
+        <v>11417480</v>
       </c>
       <c r="K107" s="56">
         <f t="shared" si="11"/>
-        <v>2322229</v>
+        <v>2337608</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -19593,7 +19609,7 @@
       </c>
       <c r="G108" s="39">
         <f t="shared" si="7"/>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H108" s="39">
         <f t="shared" si="8"/>
@@ -19601,7 +19617,7 @@
       </c>
       <c r="I108" s="11">
         <f t="shared" si="9"/>
-        <v>-255105000</v>
+        <v>-256805700</v>
       </c>
       <c r="J108" s="56">
         <f t="shared" si="10"/>
@@ -19609,7 +19625,7 @@
       </c>
       <c r="K108" s="56">
         <f t="shared" si="11"/>
-        <v>-255105000</v>
+        <v>-256805700</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -19634,7 +19650,7 @@
       </c>
       <c r="G109" s="39">
         <f t="shared" si="7"/>
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H109" s="39">
         <f t="shared" si="8"/>
@@ -19642,7 +19658,7 @@
       </c>
       <c r="I109" s="11">
         <f t="shared" si="9"/>
-        <v>-146073000</v>
+        <v>-147073500</v>
       </c>
       <c r="J109" s="56">
         <f t="shared" si="10"/>
@@ -19650,7 +19666,7 @@
       </c>
       <c r="K109" s="56">
         <f t="shared" si="11"/>
-        <v>-146073000</v>
+        <v>-147073500</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -19675,7 +19691,7 @@
       </c>
       <c r="G110" s="39">
         <f t="shared" si="7"/>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H110" s="39">
         <f t="shared" si="8"/>
@@ -19683,7 +19699,7 @@
       </c>
       <c r="I110" s="11">
         <f t="shared" si="9"/>
-        <v>2840000000</v>
+        <v>2860000000</v>
       </c>
       <c r="J110" s="56">
         <f t="shared" si="10"/>
@@ -19691,7 +19707,7 @@
       </c>
       <c r="K110" s="56">
         <f t="shared" si="11"/>
-        <v>2840000000</v>
+        <v>2860000000</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -19716,7 +19732,7 @@
       </c>
       <c r="G111" s="39">
         <f t="shared" si="7"/>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H111" s="39">
         <f t="shared" si="8"/>
@@ -19724,15 +19740,15 @@
       </c>
       <c r="I111" s="11">
         <f t="shared" si="9"/>
-        <v>21310716</v>
+        <v>21485394</v>
       </c>
       <c r="J111" s="56">
         <f t="shared" si="10"/>
-        <v>10658286</v>
+        <v>10745649</v>
       </c>
       <c r="K111" s="56">
         <f t="shared" si="11"/>
-        <v>10652430</v>
+        <v>10739745</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
@@ -19757,7 +19773,7 @@
       </c>
       <c r="G112" s="39">
         <f t="shared" si="7"/>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H112" s="39">
         <f t="shared" si="8"/>
@@ -19765,7 +19781,7 @@
       </c>
       <c r="I112" s="11">
         <f t="shared" si="9"/>
-        <v>-3038800000</v>
+        <v>-3067200000</v>
       </c>
       <c r="J112" s="56">
         <f t="shared" si="10"/>
@@ -19773,7 +19789,7 @@
       </c>
       <c r="K112" s="56">
         <f t="shared" si="11"/>
-        <v>-3038800000</v>
+        <v>-3067200000</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -19798,7 +19814,7 @@
       </c>
       <c r="G113" s="39">
         <f t="shared" si="7"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H113" s="39">
         <f t="shared" si="8"/>
@@ -19806,15 +19822,15 @@
       </c>
       <c r="I113" s="11">
         <f t="shared" si="9"/>
-        <v>14836640</v>
+        <v>14999680</v>
       </c>
       <c r="J113" s="56">
         <f t="shared" si="10"/>
-        <v>11148501</v>
+        <v>11271012</v>
       </c>
       <c r="K113" s="56">
         <f t="shared" si="11"/>
-        <v>3688139</v>
+        <v>3728668</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -19839,7 +19855,7 @@
       </c>
       <c r="G114" s="39">
         <f t="shared" si="7"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H114" s="39">
         <f t="shared" si="8"/>
@@ -19847,15 +19863,15 @@
       </c>
       <c r="I114" s="11">
         <f t="shared" si="9"/>
-        <v>-524400</v>
+        <v>-530100</v>
       </c>
       <c r="J114" s="56">
         <f t="shared" si="10"/>
-        <v>-230000</v>
+        <v>-232500</v>
       </c>
       <c r="K114" s="56">
         <f t="shared" si="11"/>
-        <v>-294400</v>
+        <v>-297600</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -19880,7 +19896,7 @@
       </c>
       <c r="G115" s="39">
         <f t="shared" si="7"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H115" s="39">
         <f t="shared" si="8"/>
@@ -19892,11 +19908,11 @@
       </c>
       <c r="J115" s="56">
         <f t="shared" si="10"/>
-        <v>39500000</v>
+        <v>40000000</v>
       </c>
       <c r="K115" s="56">
         <f t="shared" si="11"/>
-        <v>-39500000</v>
+        <v>-40000000</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -19921,7 +19937,7 @@
       </c>
       <c r="G116" s="39">
         <f t="shared" si="7"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H116" s="39">
         <f t="shared" si="8"/>
@@ -19929,7 +19945,7 @@
       </c>
       <c r="I116" s="11">
         <f t="shared" si="9"/>
-        <v>-11360000</v>
+        <v>-11520000</v>
       </c>
       <c r="J116" s="56">
         <f t="shared" si="10"/>
@@ -19937,7 +19953,7 @@
       </c>
       <c r="K116" s="56">
         <f t="shared" si="11"/>
-        <v>-11360000</v>
+        <v>-11520000</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -19962,7 +19978,7 @@
       </c>
       <c r="G117" s="39">
         <f t="shared" si="7"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H117" s="39">
         <f t="shared" si="8"/>
@@ -19970,15 +19986,15 @@
       </c>
       <c r="I117" s="11">
         <f t="shared" si="9"/>
-        <v>90280</v>
+        <v>91760</v>
       </c>
       <c r="J117" s="56">
         <f t="shared" si="10"/>
-        <v>6523401</v>
+        <v>6630342</v>
       </c>
       <c r="K117" s="56">
         <f t="shared" si="11"/>
-        <v>-6433121</v>
+        <v>-6538582</v>
       </c>
       <c r="N117" s="3"/>
     </row>
@@ -20004,7 +20020,7 @@
       </c>
       <c r="G118" s="39">
         <f t="shared" si="7"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H118" s="39">
         <f t="shared" si="8"/>
@@ -20012,7 +20028,7 @@
       </c>
       <c r="I118" s="11">
         <f t="shared" si="9"/>
-        <v>1536580500</v>
+        <v>1575980000</v>
       </c>
       <c r="J118" s="56">
         <f t="shared" si="10"/>
@@ -20020,7 +20036,7 @@
       </c>
       <c r="K118" s="56">
         <f t="shared" si="11"/>
-        <v>1536580500</v>
+        <v>1575980000</v>
       </c>
       <c r="O118" s="7"/>
     </row>
@@ -20046,7 +20062,7 @@
       </c>
       <c r="G119" s="39">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H119" s="39">
         <f t="shared" si="8"/>
@@ -20054,15 +20070,15 @@
       </c>
       <c r="I119" s="11">
         <f t="shared" si="9"/>
-        <v>2865630</v>
+        <v>2961151</v>
       </c>
       <c r="J119" s="56">
         <f t="shared" si="10"/>
-        <v>3301620</v>
+        <v>3411674</v>
       </c>
       <c r="K119" s="56">
         <f t="shared" si="11"/>
-        <v>-435990</v>
+        <v>-450523</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
@@ -20087,7 +20103,7 @@
       </c>
       <c r="G120" s="39">
         <f t="shared" si="7"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H120" s="11">
         <f t="shared" si="8"/>
@@ -20095,7 +20111,7 @@
       </c>
       <c r="I120" s="11">
         <f t="shared" ref="I120:I126" si="13">B120*(G120-H120)</f>
-        <v>52000000</v>
+        <v>54000000</v>
       </c>
       <c r="J120" s="11">
         <f t="shared" si="10"/>
@@ -20103,7 +20119,7 @@
       </c>
       <c r="K120" s="11">
         <f t="shared" si="11"/>
-        <v>52000000</v>
+        <v>54000000</v>
       </c>
       <c r="N120" s="7"/>
     </row>
@@ -20129,7 +20145,7 @@
       </c>
       <c r="G121" s="39">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H121" s="11">
         <f t="shared" si="8"/>
@@ -20137,7 +20153,7 @@
       </c>
       <c r="I121" s="11">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2600000</v>
       </c>
       <c r="J121" s="11">
         <f t="shared" si="10"/>
@@ -20145,7 +20161,7 @@
       </c>
       <c r="K121" s="11">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -20166,11 +20182,11 @@
         <v>655</v>
       </c>
       <c r="F122" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="39">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H122" s="11">
         <f t="shared" si="8"/>
@@ -20178,29 +20194,37 @@
       </c>
       <c r="I122" s="11">
         <f t="shared" si="13"/>
-        <v>-384551</v>
+        <v>0</v>
       </c>
       <c r="J122" s="11">
         <f t="shared" si="10"/>
-        <v>-110908</v>
+        <v>0</v>
       </c>
       <c r="K122" s="11">
         <f t="shared" si="11"/>
-        <v>-273643</v>
+        <v>0</v>
       </c>
       <c r="N122" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
-      <c r="B123" s="18"/>
-      <c r="C123" s="18"/>
+      <c r="A123" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="B123" s="18">
+        <v>0</v>
+      </c>
+      <c r="C123" s="18">
+        <v>800000</v>
+      </c>
       <c r="D123" s="18">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E123" s="11"/>
+        <v>-800000</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="F123" s="11">
         <v>0</v>
       </c>
@@ -20208,13 +20232,22 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H123" s="11"/>
+      <c r="H123" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="I123" s="11">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="J123" s="11"/>
-      <c r="K123" s="11"/>
+      <c r="J123" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K123" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="11"/>
@@ -20329,27 +20362,27 @@
       </c>
       <c r="C129" s="31">
         <f>SUM(C2:C127)</f>
-        <v>12004426</v>
+        <v>12804426</v>
       </c>
       <c r="D129" s="31">
         <f>SUM(D2:D127)</f>
-        <v>32531972</v>
+        <v>31731972</v>
       </c>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
       <c r="I129" s="31">
-        <f>SUM(I2:I124)</f>
-        <v>6913008039</v>
+        <f>SUM(I2:I126)</f>
+        <v>6957544437</v>
       </c>
       <c r="J129" s="31">
-        <f>SUM(J2:J124)</f>
-        <v>4088562222</v>
+        <f>SUM(J2:J126)</f>
+        <v>4100566648</v>
       </c>
       <c r="K129" s="31">
-        <f>SUM(K2:K124)</f>
-        <v>2824445817</v>
+        <f>SUM(K2:K126)</f>
+        <v>2856977789</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
@@ -20401,15 +20434,15 @@
       <c r="H132" s="11"/>
       <c r="I132" s="3">
         <f>I129/G2</f>
-        <v>14708527.742553191</v>
+        <v>14771856.554140128</v>
       </c>
       <c r="J132" s="31">
         <f>J129/G2</f>
-        <v>8699068.5574468076</v>
+        <v>8706086.3014861997</v>
       </c>
       <c r="K132" s="31">
         <f>K129/G2</f>
-        <v>6009459.1851063827</v>
+        <v>6065770.2526539275</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
@@ -20434,11 +20467,11 @@
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J136">
         <f>J129/I129*1448696</f>
-        <v>856802.66872932995</v>
+        <v>853817.68732941954</v>
       </c>
       <c r="K136">
         <f>K129/I129*1448696</f>
-        <v>591893.33127067005</v>
+        <v>594878.31267058046</v>
       </c>
     </row>
   </sheetData>
@@ -25308,8 +25341,8 @@
   <dimension ref="A1:AA80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25386,7 +25419,7 @@
       </c>
       <c r="E2" s="11">
         <f>D2+E3</f>
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="F2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -25394,7 +25427,7 @@
       </c>
       <c r="G2" s="11">
         <f>B2*(E2-F2)</f>
-        <v>13950000</v>
+        <v>11800000</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -25428,7 +25461,7 @@
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E67" si="0">D3+E4</f>
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F38" si="1">IF(B3&gt;0,1,0)</f>
@@ -25436,7 +25469,7 @@
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G23" si="2">B3*(E3-F3)</f>
-        <v>825000000</v>
+        <v>696000000</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="28"/>
@@ -25470,7 +25503,7 @@
       </c>
       <c r="E4" s="11">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" si="1"/>
@@ -25478,7 +25511,7 @@
       </c>
       <c r="G4" s="11">
         <f t="shared" si="2"/>
-        <v>822000000</v>
+        <v>693000000</v>
       </c>
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
@@ -25505,7 +25538,7 @@
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
@@ -25513,7 +25546,7 @@
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>4110000000</v>
+        <v>3465000000</v>
       </c>
       <c r="L5" t="s">
         <v>129</v>
@@ -25552,7 +25585,7 @@
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
@@ -25560,7 +25593,7 @@
       </c>
       <c r="G6" s="11">
         <f t="shared" si="2"/>
-        <v>819000000</v>
+        <v>690000000</v>
       </c>
       <c r="K6" t="s">
         <v>288</v>
@@ -25599,7 +25632,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
@@ -25607,7 +25640,7 @@
       </c>
       <c r="G7" s="11">
         <f t="shared" si="2"/>
-        <v>-819000000</v>
+        <v>-690000000</v>
       </c>
       <c r="K7" t="s">
         <v>289</v>
@@ -25649,7 +25682,7 @@
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
@@ -25657,7 +25690,7 @@
       </c>
       <c r="G8" s="11">
         <f t="shared" si="2"/>
-        <v>-54600000</v>
+        <v>-46000000</v>
       </c>
       <c r="K8" t="s">
         <v>290</v>
@@ -25699,7 +25732,7 @@
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
@@ -25707,7 +25740,7 @@
       </c>
       <c r="G9" s="11">
         <f>B9*(E9-F9)</f>
-        <v>816000000</v>
+        <v>687000000</v>
       </c>
       <c r="K9" t="s">
         <v>291</v>
@@ -25746,7 +25779,7 @@
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
@@ -25754,7 +25787,7 @@
       </c>
       <c r="G10" s="11">
         <f t="shared" si="2"/>
-        <v>813000000</v>
+        <v>684000000</v>
       </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
@@ -25781,7 +25814,7 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="1"/>
@@ -25789,7 +25822,7 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="2"/>
-        <v>6775000000</v>
+        <v>5700000000</v>
       </c>
       <c r="K11" t="s">
         <v>296</v>
@@ -25822,7 +25855,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="1"/>
@@ -25830,7 +25863,7 @@
       </c>
       <c r="G12" s="11">
         <f t="shared" si="2"/>
-        <v>267552440</v>
+        <v>224624250</v>
       </c>
       <c r="K12" t="s">
         <v>297</v>
@@ -25863,7 +25896,7 @@
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" si="1"/>
@@ -25871,7 +25904,7 @@
       </c>
       <c r="G13" s="11">
         <f t="shared" si="2"/>
-        <v>804000000</v>
+        <v>675000000</v>
       </c>
       <c r="Q13" s="27"/>
       <c r="R13" s="27"/>
@@ -25898,7 +25931,7 @@
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="1"/>
@@ -25906,7 +25939,7 @@
       </c>
       <c r="G14" s="11">
         <f t="shared" si="2"/>
-        <v>319213728</v>
+        <v>267996600</v>
       </c>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
@@ -25933,7 +25966,7 @@
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="1"/>
@@ -25941,7 +25974,7 @@
       </c>
       <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>512000000</v>
+        <v>426000000</v>
       </c>
       <c r="U15" s="27"/>
       <c r="V15" s="28"/>
@@ -25964,7 +25997,7 @@
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
@@ -25972,7 +26005,7 @@
       </c>
       <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>732000000</v>
+        <v>603000000</v>
       </c>
       <c r="U16" s="27"/>
       <c r="V16" s="28"/>
@@ -25995,7 +26028,7 @@
       </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="1"/>
@@ -26003,7 +26036,7 @@
       </c>
       <c r="G17" s="11">
         <f t="shared" si="2"/>
-        <v>729000000</v>
+        <v>600000000</v>
       </c>
       <c r="U17" s="27"/>
       <c r="V17" s="28"/>
@@ -26026,7 +26059,7 @@
       </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" si="1"/>
@@ -26034,7 +26067,7 @@
       </c>
       <c r="G18" s="11">
         <f t="shared" si="2"/>
-        <v>459800000</v>
+        <v>378100000</v>
       </c>
       <c r="U18" s="27"/>
       <c r="V18" s="28"/>
@@ -26059,7 +26092,7 @@
       </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="1"/>
@@ -26067,7 +26100,7 @@
       </c>
       <c r="G19" s="11">
         <f t="shared" si="2"/>
-        <v>182624451</v>
+        <v>148030392</v>
       </c>
       <c r="U19" s="27"/>
       <c r="V19" s="28"/>
@@ -26092,7 +26125,7 @@
       </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="1"/>
@@ -26100,7 +26133,7 @@
       </c>
       <c r="G20" s="11">
         <f t="shared" si="2"/>
-        <v>678000000</v>
+        <v>549000000</v>
       </c>
       <c r="U20" s="27"/>
       <c r="V20" s="28"/>
@@ -26125,7 +26158,7 @@
       </c>
       <c r="E21" s="11">
         <f>D21+E22</f>
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="1"/>
@@ -26133,7 +26166,7 @@
       </c>
       <c r="G21" s="11">
         <f t="shared" si="2"/>
-        <v>110000000</v>
+        <v>88500000</v>
       </c>
       <c r="U21" s="27"/>
       <c r="V21" s="28"/>
@@ -26158,7 +26191,7 @@
       </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" si="1"/>
@@ -26166,7 +26199,7 @@
       </c>
       <c r="G22" s="11">
         <f t="shared" si="2"/>
-        <v>-621000000</v>
+        <v>-492000000</v>
       </c>
       <c r="U22" s="27"/>
       <c r="V22" s="28"/>
@@ -26191,7 +26224,7 @@
       </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="1"/>
@@ -26199,7 +26232,7 @@
       </c>
       <c r="G23" s="11">
         <f t="shared" si="2"/>
-        <v>594000000</v>
+        <v>465000000</v>
       </c>
       <c r="U23" s="27"/>
       <c r="V23" s="28"/>
@@ -26224,7 +26257,7 @@
       </c>
       <c r="E24" s="11">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="1"/>
@@ -26232,7 +26265,7 @@
       </c>
       <c r="G24" s="11">
         <f>B24*(E24-F24)</f>
-        <v>124906914</v>
+        <v>97780665</v>
       </c>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -26257,7 +26290,7 @@
       </c>
       <c r="E25" s="11">
         <f t="shared" si="0"/>
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" si="1"/>
@@ -26265,7 +26298,7 @@
       </c>
       <c r="G25" s="11">
         <f t="shared" ref="G25:G30" si="3">B25*(E25-F25)</f>
-        <v>-630577300</v>
+        <v>-492938600</v>
       </c>
       <c r="U25" s="27"/>
       <c r="V25" s="27"/>
@@ -26290,7 +26323,7 @@
       </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" si="1"/>
@@ -26298,7 +26331,7 @@
       </c>
       <c r="G26" s="11">
         <f t="shared" si="3"/>
-        <v>-585175500</v>
+        <v>-456136800</v>
       </c>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
@@ -26323,7 +26356,7 @@
       </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="1"/>
@@ -26331,7 +26364,7 @@
       </c>
       <c r="G27" s="11">
         <f t="shared" si="3"/>
-        <v>192000000</v>
+        <v>149000000</v>
       </c>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
@@ -26356,7 +26389,7 @@
       </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" si="1"/>
@@ -26364,7 +26397,7 @@
       </c>
       <c r="G28" s="11">
         <f t="shared" si="3"/>
-        <v>1152000000</v>
+        <v>894000000</v>
       </c>
       <c r="U28" s="27"/>
       <c r="V28" s="27"/>
@@ -26389,7 +26422,7 @@
       </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="1"/>
@@ -26397,7 +26430,7 @@
       </c>
       <c r="G29" s="11">
         <f t="shared" si="3"/>
-        <v>1113600000</v>
+        <v>864200000</v>
       </c>
       <c r="U29" s="27"/>
       <c r="V29" s="30"/>
@@ -26422,7 +26455,7 @@
       </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="1"/>
@@ -26430,7 +26463,7 @@
       </c>
       <c r="G30" s="11">
         <f t="shared" si="3"/>
-        <v>-965000</v>
+        <v>-750000</v>
       </c>
       <c r="U30" s="27"/>
       <c r="V30" s="27"/>
@@ -26455,7 +26488,7 @@
       </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="1"/>
@@ -26463,7 +26496,7 @@
       </c>
       <c r="G31" s="11">
         <f>B31*(E31-F31)</f>
-        <v>-4992000000</v>
+        <v>-3874000000</v>
       </c>
       <c r="U31" s="27"/>
       <c r="V31" s="27"/>
@@ -26488,7 +26521,7 @@
       </c>
       <c r="E32" s="11">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" si="1"/>
@@ -26496,7 +26529,7 @@
       </c>
       <c r="G32" s="11">
         <f>B32*(E32-F32)</f>
-        <v>-4978000000</v>
+        <v>-3851400000</v>
       </c>
       <c r="U32" s="27"/>
       <c r="V32" s="27"/>
@@ -26521,7 +26554,7 @@
       </c>
       <c r="E33" s="11">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" si="1"/>
@@ -26529,7 +26562,7 @@
       </c>
       <c r="G33" s="11">
         <f>B33*(E33-F33)</f>
-        <v>55590850</v>
+        <v>41529635</v>
       </c>
       <c r="U33" s="27"/>
       <c r="V33" s="27"/>
@@ -26554,7 +26587,7 @@
       </c>
       <c r="E34" s="11">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" si="1"/>
@@ -26562,7 +26595,7 @@
       </c>
       <c r="G34" s="11">
         <f t="shared" ref="G34:G67" si="4">B34*(E34-F34)</f>
-        <v>4316800000</v>
+        <v>3095600000</v>
       </c>
       <c r="V34" s="27"/>
       <c r="W34" s="28"/>
@@ -26583,7 +26616,7 @@
       </c>
       <c r="E35" s="11">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" si="1"/>
@@ -26591,7 +26624,7 @@
       </c>
       <c r="G35" s="12">
         <f t="shared" si="4"/>
-        <v>1672000000</v>
+        <v>1199000000</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -26609,7 +26642,7 @@
       </c>
       <c r="E36" s="11">
         <f t="shared" si="0"/>
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" si="1"/>
@@ -26617,7 +26650,7 @@
       </c>
       <c r="G36" s="11">
         <f t="shared" si="4"/>
-        <v>57362037</v>
+        <v>39357894</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -26635,7 +26668,7 @@
       </c>
       <c r="E37" s="11">
         <f t="shared" si="0"/>
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="F37" s="11">
         <f t="shared" si="1"/>
@@ -26643,7 +26676,7 @@
       </c>
       <c r="G37" s="11">
         <f t="shared" si="4"/>
-        <v>-124200</v>
+        <v>-85500</v>
       </c>
       <c r="J37" s="64"/>
     </row>
@@ -26662,7 +26695,7 @@
       </c>
       <c r="E38" s="11">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="F38" s="11">
         <f t="shared" si="1"/>
@@ -26670,7 +26703,7 @@
       </c>
       <c r="G38" s="12">
         <f t="shared" si="4"/>
-        <v>272000000</v>
+        <v>186000000</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -26690,7 +26723,7 @@
       </c>
       <c r="E39" s="11">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="F39" s="11">
         <f>IF(B39&gt;0,1,0)</f>
@@ -26698,7 +26731,7 @@
       </c>
       <c r="G39" s="11">
         <f t="shared" si="4"/>
-        <v>272000000</v>
+        <v>186000000</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -26716,7 +26749,7 @@
       </c>
       <c r="E40" s="11">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="F40" s="11">
         <f>IF(B40&gt;0,1,0)</f>
@@ -26724,7 +26757,7 @@
       </c>
       <c r="G40" s="11">
         <f t="shared" si="4"/>
-        <v>-24600000</v>
+        <v>-16000000</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -26742,7 +26775,7 @@
       </c>
       <c r="E41" s="11">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="F41" s="11">
         <f>IF(B41&gt;0,1,0)</f>
@@ -26750,7 +26783,7 @@
       </c>
       <c r="G41" s="11">
         <f t="shared" si="4"/>
-        <v>-76260000</v>
+        <v>-49600000</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -26768,7 +26801,7 @@
       </c>
       <c r="E42" s="11">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" ref="F42:F67" si="5">IF(B42&gt;0,1,0)</f>
@@ -26776,7 +26809,7 @@
       </c>
       <c r="G42" s="11">
         <f t="shared" si="4"/>
-        <v>-14760000</v>
+        <v>-9600000</v>
       </c>
       <c r="J42" s="7"/>
     </row>
@@ -26795,7 +26828,7 @@
       </c>
       <c r="E43" s="11">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="5"/>
@@ -26803,7 +26836,7 @@
       </c>
       <c r="G43" s="11">
         <f t="shared" si="4"/>
-        <v>78000000</v>
+        <v>50050000</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -26821,7 +26854,7 @@
       </c>
       <c r="E44" s="11">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="F44" s="11">
         <f t="shared" si="5"/>
@@ -26829,7 +26862,7 @@
       </c>
       <c r="G44" s="11">
         <f t="shared" si="4"/>
-        <v>-605000</v>
+        <v>-390000</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -26847,7 +26880,7 @@
       </c>
       <c r="E45" s="11">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="F45" s="11">
         <f t="shared" si="5"/>
@@ -26855,7 +26888,7 @@
       </c>
       <c r="G45" s="11">
         <f t="shared" si="4"/>
-        <v>3480000000</v>
+        <v>2233000000</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -26873,7 +26906,7 @@
       </c>
       <c r="E46" s="11">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="F46" s="11">
         <f t="shared" si="5"/>
@@ -26881,7 +26914,7 @@
       </c>
       <c r="G46" s="11">
         <f t="shared" si="4"/>
-        <v>-23400000</v>
+        <v>-14800000</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -26899,7 +26932,7 @@
       </c>
       <c r="E47" s="11">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="F47" s="11">
         <f t="shared" si="5"/>
@@ -26907,7 +26940,7 @@
       </c>
       <c r="G47" s="11">
         <f t="shared" si="4"/>
-        <v>-22800000</v>
+        <v>-14200000</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -26925,7 +26958,7 @@
       </c>
       <c r="E48" s="11">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="5"/>
@@ -26933,7 +26966,7 @@
       </c>
       <c r="G48" s="11">
         <f t="shared" si="4"/>
-        <v>-22600000</v>
+        <v>-14000000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -26951,7 +26984,7 @@
       </c>
       <c r="E49" s="11">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="F49" s="11">
         <f t="shared" si="5"/>
@@ -26959,7 +26992,7 @@
       </c>
       <c r="G49" s="11">
         <f t="shared" si="4"/>
-        <v>321000000</v>
+        <v>192000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -26977,7 +27010,7 @@
       </c>
       <c r="E50" s="11">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" si="5"/>
@@ -26985,7 +27018,7 @@
       </c>
       <c r="G50" s="12">
         <f t="shared" si="4"/>
-        <v>321000000</v>
+        <v>192000000</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -27003,7 +27036,7 @@
       </c>
       <c r="E51" s="11">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" si="5"/>
@@ -27011,7 +27044,7 @@
       </c>
       <c r="G51" s="11">
         <f t="shared" si="4"/>
-        <v>81174482</v>
+        <v>48245211</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -27029,7 +27062,7 @@
       </c>
       <c r="E52" s="11">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" si="5"/>
@@ -27037,7 +27070,7 @@
       </c>
       <c r="G52" s="11">
         <f t="shared" si="4"/>
-        <v>-21400000</v>
+        <v>-12800000</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -27055,7 +27088,7 @@
       </c>
       <c r="E53" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="F53" s="11">
         <f t="shared" si="5"/>
@@ -27063,7 +27096,7 @@
       </c>
       <c r="G53" s="11">
         <f t="shared" si="4"/>
-        <v>-40050000</v>
+        <v>-22828500</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -27081,7 +27114,7 @@
       </c>
       <c r="E54" s="11">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="F54" s="11">
         <f t="shared" si="5"/>
@@ -27089,7 +27122,7 @@
       </c>
       <c r="G54" s="11">
         <f t="shared" si="4"/>
-        <v>-91036036</v>
+        <v>-48019008</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -27107,7 +27140,7 @@
       </c>
       <c r="E55" s="11">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="F55" s="11">
         <f t="shared" si="5"/>
@@ -27115,7 +27148,7 @@
       </c>
       <c r="G55" s="11">
         <f t="shared" si="4"/>
-        <v>-3400000000</v>
+        <v>-1680000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -27133,7 +27166,7 @@
       </c>
       <c r="E56" s="11">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="F56" s="11">
         <f t="shared" si="5"/>
@@ -27141,7 +27174,7 @@
       </c>
       <c r="G56" s="11">
         <f t="shared" si="4"/>
-        <v>64923900</v>
+        <v>27700864</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -27159,7 +27192,7 @@
       </c>
       <c r="E57" s="11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F57" s="11">
         <f t="shared" si="5"/>
@@ -27167,7 +27200,7 @@
       </c>
       <c r="G57" s="11">
         <f t="shared" si="4"/>
-        <v>-2459800000</v>
+        <v>-301200000</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -27185,7 +27218,7 @@
       </c>
       <c r="E58" s="11">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="F58" s="11">
         <f t="shared" si="5"/>
@@ -27193,7 +27226,7 @@
       </c>
       <c r="G58" s="11">
         <f t="shared" si="4"/>
-        <v>-585624000</v>
+        <v>-61002500</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -27207,11 +27240,11 @@
         <v>655</v>
       </c>
       <c r="D59" s="11">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="E59" s="11">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="F59" s="11">
         <f t="shared" si="5"/>
@@ -27219,17 +27252,25 @@
       </c>
       <c r="G59" s="11">
         <f t="shared" si="4"/>
-        <v>23535864</v>
+        <v>534906</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="41"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
+      <c r="A60" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="B60" s="41">
+        <v>-338000</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="D60" s="11">
+        <v>1</v>
+      </c>
       <c r="E60" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="11">
         <f t="shared" si="5"/>
@@ -27237,7 +27278,7 @@
       </c>
       <c r="G60" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-338000</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -27378,7 +27419,7 @@
       <c r="A68" s="11"/>
       <c r="B68" s="31">
         <f>SUM(B2:B66)</f>
-        <v>2682747</v>
+        <v>2344747</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -27386,7 +27427,7 @@
       <c r="F68" s="11"/>
       <c r="G68" s="31">
         <f>SUM(G2:G67)</f>
-        <v>14515657630</v>
+        <v>14399961509</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -27420,7 +27461,7 @@
       <c r="F71" s="11"/>
       <c r="G71" s="3">
         <f>G68/E2</f>
-        <v>51841634.392857142</v>
+        <v>60759331.261603378</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -27454,7 +27495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
     </sheetView>
@@ -31159,8 +31200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31404,11 +31445,11 @@
       </c>
       <c r="F7" s="73">
         <f>K23</f>
-        <v>176780273.02739727</v>
+        <v>175572273.02739727</v>
       </c>
       <c r="G7" s="31">
         <f t="shared" si="0"/>
-        <v>1388805.9135027528</v>
+        <v>2596805.9135027528</v>
       </c>
       <c r="H7" s="11"/>
       <c r="J7" s="62" t="s">
@@ -31568,14 +31609,14 @@
       </c>
       <c r="K11" s="46">
         <f>سارا!D129</f>
-        <v>32531972</v>
+        <v>31731972</v>
       </c>
       <c r="L11" s="3">
         <v>0</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="5"/>
-        <v>32531972</v>
+        <v>31731972</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -31605,14 +31646,14 @@
       </c>
       <c r="K12" s="46">
         <f>'مسکن مریم یاران'!B68</f>
-        <v>2682747</v>
+        <v>2344747</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="5"/>
-        <v>2682747</v>
+        <v>2344747</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -31774,11 +31815,11 @@
         <v>468</v>
       </c>
       <c r="K16" s="46">
-        <v>250000</v>
+        <v>180000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>250000</v>
+        <v>180000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="5"/>
@@ -32127,15 +32168,15 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>176780273.02739727</v>
+        <v>175572273.02739727</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>62794261.684931517</v>
+        <v>62724261.684931517</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
-        <v>113986011.34246576</v>
+        <v>112848011.34246576</v>
       </c>
       <c r="N23" s="27"/>
       <c r="O23" s="11" t="s">
@@ -32179,15 +32220,15 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>103706547</v>
+        <v>102498547</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12+L10</f>
-        <v>22195111</v>
+        <v>22125111</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17+M9</f>
-        <v>81511436</v>
+        <v>80373436</v>
       </c>
       <c r="N24" s="27"/>
       <c r="O24" s="11"/>

</xml_diff>

<commit_message>
updated 13/5/1396 at 17:25
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="698">
   <si>
     <t>18/1/95</t>
   </si>
@@ -2120,10 +2120,16 @@
     <t>8/5/1396</t>
   </si>
   <si>
-    <t>احتمالا مریم</t>
-  </si>
-  <si>
     <t>طلب علی(500 خانه، 500 علیرضا)</t>
+  </si>
+  <si>
+    <t>تاریخ 12 مرداد از کارت مسکن یاران گرفتم</t>
+  </si>
+  <si>
+    <t>12/5/1396</t>
+  </si>
+  <si>
+    <t>مریم گلدون و بشقاب و فانوس خرید</t>
   </si>
 </sst>
 </file>
@@ -2812,8 +2818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3912,9 +3918,11 @@
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D34" s="45">
-        <v>0</v>
-      </c>
-      <c r="E34" s="44"/>
+        <v>200000</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35" s="45">
@@ -3957,7 +3965,7 @@
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <f>SUM(D30:D39)</f>
-        <v>8485102</v>
+        <v>8685102</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -25366,11 +25374,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA80"/>
+  <dimension ref="A1:AA84"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25447,7 +25455,7 @@
       </c>
       <c r="E2" s="11">
         <f>D2+E3</f>
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -25455,7 +25463,7 @@
       </c>
       <c r="G2" s="11">
         <f>B2*(E2-F2)</f>
-        <v>12100000</v>
+        <v>12250000</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -25488,8 +25496,8 @@
         <v>1</v>
       </c>
       <c r="E3" s="11">
-        <f t="shared" ref="E3:E67" si="0">D3+E4</f>
-        <v>239</v>
+        <f t="shared" ref="E3:E71" si="0">D3+E4</f>
+        <v>242</v>
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F38" si="1">IF(B3&gt;0,1,0)</f>
@@ -25497,7 +25505,7 @@
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G23" si="2">B3*(E3-F3)</f>
-        <v>714000000</v>
+        <v>723000000</v>
       </c>
       <c r="J3" s="27"/>
       <c r="K3" s="28"/>
@@ -25531,7 +25539,7 @@
       </c>
       <c r="E4" s="11">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" si="1"/>
@@ -25539,7 +25547,7 @@
       </c>
       <c r="G4" s="11">
         <f t="shared" si="2"/>
-        <v>711000000</v>
+        <v>720000000</v>
       </c>
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
@@ -25566,7 +25574,7 @@
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
@@ -25574,7 +25582,7 @@
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>3555000000</v>
+        <v>3600000000</v>
       </c>
       <c r="L5" t="s">
         <v>129</v>
@@ -25613,7 +25621,7 @@
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
@@ -25621,7 +25629,7 @@
       </c>
       <c r="G6" s="11">
         <f t="shared" si="2"/>
-        <v>708000000</v>
+        <v>717000000</v>
       </c>
       <c r="K6" t="s">
         <v>288</v>
@@ -25660,7 +25668,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
@@ -25668,7 +25676,7 @@
       </c>
       <c r="G7" s="11">
         <f t="shared" si="2"/>
-        <v>-708000000</v>
+        <v>-717000000</v>
       </c>
       <c r="K7" t="s">
         <v>289</v>
@@ -25710,7 +25718,7 @@
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
@@ -25718,7 +25726,7 @@
       </c>
       <c r="G8" s="11">
         <f t="shared" si="2"/>
-        <v>-47200000</v>
+        <v>-47800000</v>
       </c>
       <c r="K8" t="s">
         <v>290</v>
@@ -25760,7 +25768,7 @@
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
@@ -25768,7 +25776,7 @@
       </c>
       <c r="G9" s="11">
         <f>B9*(E9-F9)</f>
-        <v>705000000</v>
+        <v>714000000</v>
       </c>
       <c r="K9" t="s">
         <v>291</v>
@@ -25807,7 +25815,7 @@
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
@@ -25815,7 +25823,7 @@
       </c>
       <c r="G10" s="11">
         <f t="shared" si="2"/>
-        <v>702000000</v>
+        <v>711000000</v>
       </c>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
@@ -25842,7 +25850,7 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="1"/>
@@ -25850,7 +25858,7 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="2"/>
-        <v>5850000000</v>
+        <v>5925000000</v>
       </c>
       <c r="K11" t="s">
         <v>296</v>
@@ -25883,7 +25891,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="1"/>
@@ -25891,7 +25899,7 @@
       </c>
       <c r="G12" s="11">
         <f t="shared" si="2"/>
-        <v>230614230</v>
+        <v>233609220</v>
       </c>
       <c r="K12" t="s">
         <v>297</v>
@@ -25924,7 +25932,7 @@
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" si="1"/>
@@ -25932,7 +25940,7 @@
       </c>
       <c r="G13" s="11">
         <f t="shared" si="2"/>
-        <v>693000000</v>
+        <v>702000000</v>
       </c>
       <c r="Q13" s="27"/>
       <c r="R13" s="27"/>
@@ -25959,7 +25967,7 @@
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="1"/>
@@ -25967,7 +25975,7 @@
       </c>
       <c r="G14" s="11">
         <f t="shared" si="2"/>
-        <v>275143176</v>
+        <v>278716464</v>
       </c>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
@@ -25994,7 +26002,7 @@
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="1"/>
@@ -26002,7 +26010,7 @@
       </c>
       <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>438000000</v>
+        <v>444000000</v>
       </c>
       <c r="U15" s="27"/>
       <c r="V15" s="28"/>
@@ -26025,7 +26033,7 @@
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
@@ -26033,7 +26041,7 @@
       </c>
       <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>621000000</v>
+        <v>630000000</v>
       </c>
       <c r="U16" s="27"/>
       <c r="V16" s="28"/>
@@ -26056,7 +26064,7 @@
       </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="1"/>
@@ -26064,7 +26072,7 @@
       </c>
       <c r="G17" s="11">
         <f t="shared" si="2"/>
-        <v>618000000</v>
+        <v>627000000</v>
       </c>
       <c r="U17" s="27"/>
       <c r="V17" s="28"/>
@@ -26087,7 +26095,7 @@
       </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" si="1"/>
@@ -26095,7 +26103,7 @@
       </c>
       <c r="G18" s="11">
         <f t="shared" si="2"/>
-        <v>389500000</v>
+        <v>395200000</v>
       </c>
       <c r="U18" s="27"/>
       <c r="V18" s="28"/>
@@ -26120,7 +26128,7 @@
       </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="1"/>
@@ -26128,7 +26136,7 @@
       </c>
       <c r="G19" s="11">
         <f t="shared" si="2"/>
-        <v>152857470</v>
+        <v>155271009</v>
       </c>
       <c r="U19" s="27"/>
       <c r="V19" s="28"/>
@@ -26153,7 +26161,7 @@
       </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="1"/>
@@ -26161,7 +26169,7 @@
       </c>
       <c r="G20" s="11">
         <f t="shared" si="2"/>
-        <v>567000000</v>
+        <v>576000000</v>
       </c>
       <c r="U20" s="27"/>
       <c r="V20" s="28"/>
@@ -26186,7 +26194,7 @@
       </c>
       <c r="E21" s="11">
         <f>D21+E22</f>
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="1"/>
@@ -26194,7 +26202,7 @@
       </c>
       <c r="G21" s="11">
         <f t="shared" si="2"/>
-        <v>91500000</v>
+        <v>93000000</v>
       </c>
       <c r="U21" s="27"/>
       <c r="V21" s="28"/>
@@ -26219,7 +26227,7 @@
       </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" si="1"/>
@@ -26227,7 +26235,7 @@
       </c>
       <c r="G22" s="11">
         <f t="shared" si="2"/>
-        <v>-510000000</v>
+        <v>-519000000</v>
       </c>
       <c r="U22" s="27"/>
       <c r="V22" s="28"/>
@@ -26252,7 +26260,7 @@
       </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="1"/>
@@ -26260,7 +26268,7 @@
       </c>
       <c r="G23" s="11">
         <f t="shared" si="2"/>
-        <v>483000000</v>
+        <v>492000000</v>
       </c>
       <c r="U23" s="27"/>
       <c r="V23" s="28"/>
@@ -26285,7 +26293,7 @@
       </c>
       <c r="E24" s="11">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="1"/>
@@ -26293,7 +26301,7 @@
       </c>
       <c r="G24" s="11">
         <f>B24*(E24-F24)</f>
-        <v>101565723</v>
+        <v>103458252</v>
       </c>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -26318,7 +26326,7 @@
       </c>
       <c r="E25" s="11">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" si="1"/>
@@ -26326,7 +26334,7 @@
       </c>
       <c r="G25" s="11">
         <f t="shared" ref="G25:G30" si="3">B25*(E25-F25)</f>
-        <v>-512144000</v>
+        <v>-521746700</v>
       </c>
       <c r="U25" s="27"/>
       <c r="V25" s="27"/>
@@ -26351,7 +26359,7 @@
       </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" si="1"/>
@@ -26359,7 +26367,7 @@
       </c>
       <c r="G26" s="11">
         <f t="shared" si="3"/>
-        <v>-474142200</v>
+        <v>-483144900</v>
       </c>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
@@ -26384,7 +26392,7 @@
       </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="1"/>
@@ -26392,7 +26400,7 @@
       </c>
       <c r="G27" s="11">
         <f t="shared" si="3"/>
-        <v>155000000</v>
+        <v>158000000</v>
       </c>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
@@ -26417,7 +26425,7 @@
       </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" si="1"/>
@@ -26425,7 +26433,7 @@
       </c>
       <c r="G28" s="11">
         <f t="shared" si="3"/>
-        <v>930000000</v>
+        <v>948000000</v>
       </c>
       <c r="U28" s="27"/>
       <c r="V28" s="27"/>
@@ -26450,7 +26458,7 @@
       </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="1"/>
@@ -26458,7 +26466,7 @@
       </c>
       <c r="G29" s="11">
         <f t="shared" si="3"/>
-        <v>899000000</v>
+        <v>916400000</v>
       </c>
       <c r="U29" s="27"/>
       <c r="V29" s="30"/>
@@ -26483,7 +26491,7 @@
       </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="1"/>
@@ -26491,7 +26499,7 @@
       </c>
       <c r="G30" s="11">
         <f t="shared" si="3"/>
-        <v>-780000</v>
+        <v>-795000</v>
       </c>
       <c r="U30" s="27"/>
       <c r="V30" s="27"/>
@@ -26516,7 +26524,7 @@
       </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="1"/>
@@ -26524,7 +26532,7 @@
       </c>
       <c r="G31" s="11">
         <f>B31*(E31-F31)</f>
-        <v>-4030000000</v>
+        <v>-4108000000</v>
       </c>
       <c r="U31" s="27"/>
       <c r="V31" s="27"/>
@@ -26549,7 +26557,7 @@
       </c>
       <c r="E32" s="11">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" si="1"/>
@@ -26557,7 +26565,7 @@
       </c>
       <c r="G32" s="11">
         <f>B32*(E32-F32)</f>
-        <v>-4008600000</v>
+        <v>-4087200000</v>
       </c>
       <c r="U32" s="27"/>
       <c r="V32" s="27"/>
@@ -26582,7 +26590,7 @@
       </c>
       <c r="E33" s="11">
         <f t="shared" si="0"/>
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" si="1"/>
@@ -26590,7 +26598,7 @@
       </c>
       <c r="G33" s="11">
         <f>B33*(E33-F33)</f>
-        <v>43491665</v>
+        <v>44472680</v>
       </c>
       <c r="U33" s="27"/>
       <c r="V33" s="27"/>
@@ -26615,15 +26623,15 @@
       </c>
       <c r="E34" s="11">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G34" s="11">
-        <f t="shared" ref="G34:G67" si="4">B34*(E34-F34)</f>
-        <v>3266000000</v>
+        <f t="shared" ref="G34:G71" si="4">B34*(E34-F34)</f>
+        <v>3351200000</v>
       </c>
       <c r="V34" s="27"/>
       <c r="W34" s="28"/>
@@ -26644,7 +26652,7 @@
       </c>
       <c r="E35" s="11">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" si="1"/>
@@ -26652,7 +26660,7 @@
       </c>
       <c r="G35" s="12">
         <f t="shared" si="4"/>
-        <v>1265000000</v>
+        <v>1298000000</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -26670,7 +26678,7 @@
       </c>
       <c r="E36" s="11">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" si="1"/>
@@ -26678,7 +26686,7 @@
       </c>
       <c r="G36" s="11">
         <f t="shared" si="4"/>
-        <v>41870100</v>
+        <v>43126203</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -26696,7 +26704,7 @@
       </c>
       <c r="E37" s="11">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F37" s="11">
         <f t="shared" si="1"/>
@@ -26704,7 +26712,7 @@
       </c>
       <c r="G37" s="11">
         <f t="shared" si="4"/>
-        <v>-90900</v>
+        <v>-93600</v>
       </c>
       <c r="J37" s="64"/>
     </row>
@@ -26723,7 +26731,7 @@
       </c>
       <c r="E38" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F38" s="11">
         <f t="shared" si="1"/>
@@ -26731,7 +26739,7 @@
       </c>
       <c r="G38" s="12">
         <f t="shared" si="4"/>
-        <v>198000000</v>
+        <v>204000000</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -26751,7 +26759,7 @@
       </c>
       <c r="E39" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F39" s="11">
         <f>IF(B39&gt;0,1,0)</f>
@@ -26759,7 +26767,7 @@
       </c>
       <c r="G39" s="11">
         <f t="shared" si="4"/>
-        <v>198000000</v>
+        <v>204000000</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -26777,7 +26785,7 @@
       </c>
       <c r="E40" s="11">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F40" s="11">
         <f>IF(B40&gt;0,1,0)</f>
@@ -26785,7 +26793,7 @@
       </c>
       <c r="G40" s="11">
         <f t="shared" si="4"/>
-        <v>-17200000</v>
+        <v>-17800000</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -26803,7 +26811,7 @@
       </c>
       <c r="E41" s="11">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F41" s="11">
         <f>IF(B41&gt;0,1,0)</f>
@@ -26811,7 +26819,7 @@
       </c>
       <c r="G41" s="11">
         <f t="shared" si="4"/>
-        <v>-53320000</v>
+        <v>-55180000</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -26829,15 +26837,15 @@
       </c>
       <c r="E42" s="11">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F42" s="11">
-        <f t="shared" ref="F42:F67" si="5">IF(B42&gt;0,1,0)</f>
+        <f t="shared" ref="F42:F71" si="5">IF(B42&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="G42" s="11">
         <f t="shared" si="4"/>
-        <v>-10320000</v>
+        <v>-10680000</v>
       </c>
       <c r="J42" s="7"/>
     </row>
@@ -26856,7 +26864,7 @@
       </c>
       <c r="E43" s="11">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="5"/>
@@ -26864,7 +26872,7 @@
       </c>
       <c r="G43" s="11">
         <f t="shared" si="4"/>
-        <v>53950000</v>
+        <v>55900000</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -26882,7 +26890,7 @@
       </c>
       <c r="E44" s="11">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F44" s="11">
         <f t="shared" si="5"/>
@@ -26890,7 +26898,7 @@
       </c>
       <c r="G44" s="11">
         <f t="shared" si="4"/>
-        <v>-420000</v>
+        <v>-435000</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -26908,7 +26916,7 @@
       </c>
       <c r="E45" s="11">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F45" s="11">
         <f t="shared" si="5"/>
@@ -26916,7 +26924,7 @@
       </c>
       <c r="G45" s="11">
         <f t="shared" si="4"/>
-        <v>2407000000</v>
+        <v>2494000000</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -26934,7 +26942,7 @@
       </c>
       <c r="E46" s="11">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F46" s="11">
         <f t="shared" si="5"/>
@@ -26942,7 +26950,7 @@
       </c>
       <c r="G46" s="11">
         <f t="shared" si="4"/>
-        <v>-16000000</v>
+        <v>-16600000</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -26960,7 +26968,7 @@
       </c>
       <c r="E47" s="11">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F47" s="11">
         <f t="shared" si="5"/>
@@ -26968,7 +26976,7 @@
       </c>
       <c r="G47" s="11">
         <f t="shared" si="4"/>
-        <v>-15400000</v>
+        <v>-16000000</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -26986,7 +26994,7 @@
       </c>
       <c r="E48" s="11">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="5"/>
@@ -26994,7 +27002,7 @@
       </c>
       <c r="G48" s="11">
         <f t="shared" si="4"/>
-        <v>-15200000</v>
+        <v>-15800000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -27012,7 +27020,7 @@
       </c>
       <c r="E49" s="11">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F49" s="11">
         <f t="shared" si="5"/>
@@ -27020,7 +27028,7 @@
       </c>
       <c r="G49" s="11">
         <f t="shared" si="4"/>
-        <v>210000000</v>
+        <v>219000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -27038,7 +27046,7 @@
       </c>
       <c r="E50" s="11">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" si="5"/>
@@ -27046,7 +27054,7 @@
       </c>
       <c r="G50" s="12">
         <f t="shared" si="4"/>
-        <v>210000000</v>
+        <v>219000000</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -27064,7 +27072,7 @@
       </c>
       <c r="E51" s="11">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" si="5"/>
@@ -27072,7 +27080,7 @@
       </c>
       <c r="G51" s="11">
         <f t="shared" si="4"/>
-        <v>52839993</v>
+        <v>55137384</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -27090,7 +27098,7 @@
       </c>
       <c r="E52" s="11">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" si="5"/>
@@ -27098,7 +27106,7 @@
       </c>
       <c r="G52" s="11">
         <f t="shared" si="4"/>
-        <v>-14000000</v>
+        <v>-14600000</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -27116,7 +27124,7 @@
       </c>
       <c r="E53" s="11">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F53" s="11">
         <f t="shared" si="5"/>
@@ -27124,7 +27132,7 @@
       </c>
       <c r="G53" s="11">
         <f t="shared" si="4"/>
-        <v>-25231500</v>
+        <v>-26433000</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -27142,7 +27150,7 @@
       </c>
       <c r="E54" s="11">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F54" s="11">
         <f t="shared" si="5"/>
@@ -27150,7 +27158,7 @@
       </c>
       <c r="G54" s="11">
         <f t="shared" si="4"/>
-        <v>-54021384</v>
+        <v>-57022572</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -27168,7 +27176,7 @@
       </c>
       <c r="E55" s="11">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F55" s="11">
         <f t="shared" si="5"/>
@@ -27176,7 +27184,7 @@
       </c>
       <c r="G55" s="11">
         <f t="shared" si="4"/>
-        <v>-1920000000</v>
+        <v>-2040000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -27194,7 +27202,7 @@
       </c>
       <c r="E56" s="11">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F56" s="11">
         <f t="shared" si="5"/>
@@ -27202,7 +27210,7 @@
       </c>
       <c r="G56" s="11">
         <f t="shared" si="4"/>
-        <v>32894776</v>
+        <v>35491732</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -27220,7 +27228,7 @@
       </c>
       <c r="E57" s="11">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F57" s="11">
         <f t="shared" si="5"/>
@@ -27228,7 +27236,7 @@
       </c>
       <c r="G57" s="11">
         <f t="shared" si="4"/>
-        <v>-602400000</v>
+        <v>-753000000</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -27246,7 +27254,7 @@
       </c>
       <c r="E58" s="11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F58" s="11">
         <f t="shared" si="5"/>
@@ -27254,7 +27262,7 @@
       </c>
       <c r="G58" s="11">
         <f t="shared" si="4"/>
-        <v>-134205500</v>
+        <v>-170807000</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -27272,7 +27280,7 @@
       </c>
       <c r="E59" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F59" s="11">
         <f t="shared" si="5"/>
@@ -27280,7 +27288,7 @@
       </c>
       <c r="G59" s="11">
         <f t="shared" si="4"/>
-        <v>3744342</v>
+        <v>5349060</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -27298,7 +27306,7 @@
       </c>
       <c r="E60" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F60" s="11">
         <f t="shared" si="5"/>
@@ -27306,7 +27314,7 @@
       </c>
       <c r="G60" s="11">
         <f t="shared" si="4"/>
-        <v>-2366000</v>
+        <v>-3380000</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -27320,11 +27328,11 @@
         <v>688</v>
       </c>
       <c r="D61" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E61" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F61" s="11">
         <f t="shared" si="5"/>
@@ -27332,25 +27340,25 @@
       </c>
       <c r="G61" s="11">
         <f t="shared" si="4"/>
-        <v>-750000</v>
+        <v>-1200000</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="B62" s="41">
-        <v>-5000</v>
+        <v>-100000</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>694</v>
+        <v>26</v>
       </c>
       <c r="D62" s="11">
         <v>4</v>
       </c>
       <c r="E62" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" s="11">
         <f t="shared" si="5"/>
@@ -27358,25 +27366,25 @@
       </c>
       <c r="G62" s="11">
         <f t="shared" si="4"/>
-        <v>-25000</v>
+        <v>-400000</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B63" s="41">
-        <v>-100000</v>
+        <v>-200000</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>158</v>
       </c>
       <c r="D63" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>D63+E68</f>
+        <v>0</v>
       </c>
       <c r="F63" s="11">
         <f t="shared" si="5"/>
@@ -27384,19 +27392,25 @@
       </c>
       <c r="G63" s="11">
         <f t="shared" si="4"/>
-        <v>-100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="41"/>
-      <c r="C64" s="11"/>
+      <c r="A64" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="41">
+        <v>-87000</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>697</v>
+      </c>
       <c r="D64" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E64:E71" si="6">D64+E69</f>
+        <v>1</v>
       </c>
       <c r="F64" s="11">
         <f t="shared" si="5"/>
@@ -27404,18 +27418,16 @@
       </c>
       <c r="G64" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-87000</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
+      <c r="B65" s="41"/>
       <c r="C65" s="11"/>
-      <c r="D65" s="11">
-        <v>0</v>
-      </c>
+      <c r="D65" s="11"/>
       <c r="E65" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F65" s="11">
@@ -27429,13 +27441,11 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="11">
-        <v>0</v>
-      </c>
+      <c r="D66" s="11"/>
       <c r="E66" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F66" s="11">
@@ -27449,13 +27459,11 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
+      <c r="B67" s="41"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="11">
-        <v>0</v>
-      </c>
+      <c r="D67" s="11"/>
       <c r="E67" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F67" s="11">
@@ -27469,71 +27477,151 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
-      <c r="B68" s="31">
-        <f>SUM(B2:B66)</f>
-        <v>2089747</v>
-      </c>
+      <c r="B68" s="41"/>
       <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="31">
-        <f>SUM(G2:G67)</f>
-        <v>14413154991</v>
+      <c r="D68" s="11">
+        <v>0</v>
+      </c>
+      <c r="E68" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F68" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
-      <c r="B69" s="11" t="s">
-        <v>283</v>
-      </c>
+      <c r="B69" s="11"/>
       <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11" t="s">
-        <v>284</v>
+      <c r="D69" s="11">
+        <v>0</v>
+      </c>
+      <c r="E69" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
+      <c r="D70" s="11">
+        <v>0</v>
+      </c>
+      <c r="E70" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F70" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="3">
-        <f>G68/E2</f>
-        <v>59313395.024691358</v>
+      <c r="D71" s="11">
+        <v>0</v>
+      </c>
+      <c r="E71" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
+      <c r="B72" s="31">
+        <f>SUM(B2:B70)</f>
+        <v>1807747</v>
+      </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
-      <c r="G72" s="11" t="s">
+      <c r="G72" s="31">
+        <f>SUM(G2:G71)</f>
+        <v>14419377232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="3">
+        <f>G72/E2</f>
+        <v>58615354.601626016</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G79" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G80" s="41">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="41">
         <v>13400000000</v>
       </c>
     </row>
@@ -31252,8 +31340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31497,11 +31585,11 @@
       </c>
       <c r="F7" s="73">
         <f>K23</f>
-        <v>175302273.02739727</v>
+        <v>174830273.02739727</v>
       </c>
       <c r="G7" s="31">
         <f t="shared" si="0"/>
-        <v>2866805.9135027528</v>
+        <v>3338805.9135027528</v>
       </c>
       <c r="H7" s="11"/>
       <c r="J7" s="62" t="s">
@@ -31697,15 +31785,15 @@
         <v>462</v>
       </c>
       <c r="K12" s="46">
-        <f>'مسکن مریم یاران'!B68</f>
-        <v>2089747</v>
+        <f>'مسکن مریم یاران'!B72</f>
+        <v>1807747</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="5"/>
-        <v>2089747</v>
+        <v>1807747</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -31768,7 +31856,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="J14" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K14" s="46">
         <v>1000000</v>
@@ -31819,11 +31907,11 @@
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>-8500000</v>
+        <v>-8700000</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="5"/>
-        <v>8500000</v>
+        <v>8700000</v>
       </c>
       <c r="N15" s="27"/>
       <c r="O15" s="11"/>
@@ -31867,11 +31955,11 @@
         <v>468</v>
       </c>
       <c r="K16" s="46">
-        <v>315000</v>
+        <v>225000</v>
       </c>
       <c r="L16" s="3">
         <f>K16</f>
-        <v>315000</v>
+        <v>225000</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="5"/>
@@ -31923,14 +32011,14 @@
         <v>469</v>
       </c>
       <c r="K17" s="46">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="5"/>
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="N17" s="27"/>
       <c r="O17" s="11" t="s">
@@ -32220,15 +32308,15 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>175302273.02739727</v>
+        <v>174830273.02739727</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>62709261.684931517</v>
+        <v>62419261.684931517</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
-        <v>112593011.34246576</v>
+        <v>112411011.34246576</v>
       </c>
       <c r="N23" s="27"/>
       <c r="O23" s="11" t="s">
@@ -32272,15 +32360,15 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>102378547</v>
+        <v>101906547</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12+L10</f>
-        <v>22260111</v>
+        <v>22170111</v>
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17+M9</f>
-        <v>80118436</v>
+        <v>79736436</v>
       </c>
       <c r="N24" s="27"/>
       <c r="O24" s="11"/>

</xml_diff>

<commit_message>
updated 4/6/1396 at 18:48
</commit_message>
<xml_diff>
--- a/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
+++ b/AudioDemo/finance/New Microsoft Excel Worksheet.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="732">
   <si>
     <t>18/1/95</t>
   </si>
@@ -2227,6 +2227,12 @@
   </si>
   <si>
     <t>حواله اچ سی مریم 3 اسفند 18 درصد تا آخر شهریور</t>
+  </si>
+  <si>
+    <t>روز 4 شهریور از کارت یاران گرفتم</t>
+  </si>
+  <si>
+    <t>4/6/1396</t>
   </si>
 </sst>
 </file>
@@ -2921,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3991,9 +3997,11 @@
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="D32" s="43">
-        <v>0</v>
-      </c>
-      <c r="E32" s="42"/>
+        <v>200000</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>730</v>
+      </c>
       <c r="O32">
         <v>31</v>
       </c>
@@ -4063,7 +4071,7 @@
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <f>SUM(D30:D39)</f>
-        <v>6646572</v>
+        <v>6846572</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -27131,8 +27139,8 @@
   <dimension ref="A1:AA102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H87" sqref="H87"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27209,7 +27217,7 @@
       </c>
       <c r="E2" s="11">
         <f>D2+E3</f>
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F2" s="11">
         <f>IF(B2&gt;0,1,0)</f>
@@ -27217,7 +27225,7 @@
       </c>
       <c r="G2" s="11">
         <f>B2*(E2-F2)</f>
-        <v>13300000</v>
+        <v>13450000</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
@@ -27251,7 +27259,7 @@
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E66" si="0">D3+E4</f>
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F3" s="11">
         <f t="shared" ref="F3:F38" si="1">IF(B3&gt;0,1,0)</f>
@@ -27259,7 +27267,7 @@
       </c>
       <c r="G3" s="11">
         <f t="shared" ref="G3:G23" si="2">B3*(E3-F3)</f>
-        <v>786000000</v>
+        <v>795000000</v>
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="26"/>
@@ -27293,7 +27301,7 @@
       </c>
       <c r="E4" s="11">
         <f t="shared" si="0"/>
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F4" s="11">
         <f t="shared" si="1"/>
@@ -27301,7 +27309,7 @@
       </c>
       <c r="G4" s="11">
         <f t="shared" si="2"/>
-        <v>783000000</v>
+        <v>792000000</v>
       </c>
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
@@ -27328,7 +27336,7 @@
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="1"/>
@@ -27336,7 +27344,7 @@
       </c>
       <c r="G5" s="11">
         <f t="shared" si="2"/>
-        <v>3915000000</v>
+        <v>3960000000</v>
       </c>
       <c r="L5" t="s">
         <v>129</v>
@@ -27375,7 +27383,7 @@
       </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="1"/>
@@ -27383,7 +27391,7 @@
       </c>
       <c r="G6" s="11">
         <f t="shared" si="2"/>
-        <v>780000000</v>
+        <v>789000000</v>
       </c>
       <c r="K6" t="s">
         <v>288</v>
@@ -27422,7 +27430,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="1"/>
@@ -27430,7 +27438,7 @@
       </c>
       <c r="G7" s="11">
         <f t="shared" si="2"/>
-        <v>-780000000</v>
+        <v>-789000000</v>
       </c>
       <c r="K7" t="s">
         <v>289</v>
@@ -27472,7 +27480,7 @@
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="1"/>
@@ -27480,7 +27488,7 @@
       </c>
       <c r="G8" s="11">
         <f t="shared" si="2"/>
-        <v>-52000000</v>
+        <v>-52600000</v>
       </c>
       <c r="K8" t="s">
         <v>290</v>
@@ -27522,7 +27530,7 @@
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="1"/>
@@ -27530,7 +27538,7 @@
       </c>
       <c r="G9" s="11">
         <f>B9*(E9-F9)</f>
-        <v>777000000</v>
+        <v>786000000</v>
       </c>
       <c r="K9" t="s">
         <v>291</v>
@@ -27569,7 +27577,7 @@
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
@@ -27577,7 +27585,7 @@
       </c>
       <c r="G10" s="11">
         <f t="shared" si="2"/>
-        <v>774000000</v>
+        <v>783000000</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
@@ -27604,7 +27612,7 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="1"/>
@@ -27612,7 +27620,7 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="2"/>
-        <v>6450000000</v>
+        <v>6525000000</v>
       </c>
       <c r="K11" t="s">
         <v>296</v>
@@ -27645,7 +27653,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="1"/>
@@ -27653,7 +27661,7 @@
       </c>
       <c r="G12" s="11">
         <f t="shared" si="2"/>
-        <v>254574150</v>
+        <v>257569140</v>
       </c>
       <c r="K12" t="s">
         <v>297</v>
@@ -27686,7 +27694,7 @@
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" si="1"/>
@@ -27694,7 +27702,7 @@
       </c>
       <c r="G13" s="11">
         <f t="shared" si="2"/>
-        <v>765000000</v>
+        <v>774000000</v>
       </c>
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
@@ -27721,7 +27729,7 @@
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="1"/>
@@ -27729,7 +27737,7 @@
       </c>
       <c r="G14" s="11">
         <f t="shared" si="2"/>
-        <v>303729480</v>
+        <v>307302768</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
@@ -27756,7 +27764,7 @@
       </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="1"/>
@@ -27764,7 +27772,7 @@
       </c>
       <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>486000000</v>
+        <v>492000000</v>
       </c>
       <c r="U15" s="25"/>
       <c r="V15" s="26"/>
@@ -27787,7 +27795,7 @@
       </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
@@ -27795,7 +27803,7 @@
       </c>
       <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>693000000</v>
+        <v>702000000</v>
       </c>
       <c r="U16" s="25"/>
       <c r="V16" s="26"/>
@@ -27818,7 +27826,7 @@
       </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" si="1"/>
@@ -27826,7 +27834,7 @@
       </c>
       <c r="G17" s="11">
         <f t="shared" si="2"/>
-        <v>690000000</v>
+        <v>699000000</v>
       </c>
       <c r="U17" s="25"/>
       <c r="V17" s="26"/>
@@ -27849,7 +27857,7 @@
       </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" si="1"/>
@@ -27857,7 +27865,7 @@
       </c>
       <c r="G18" s="11">
         <f t="shared" si="2"/>
-        <v>435100000</v>
+        <v>440800000</v>
       </c>
       <c r="U18" s="25"/>
       <c r="V18" s="26"/>
@@ -27882,7 +27890,7 @@
       </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="1"/>
@@ -27890,7 +27898,7 @@
       </c>
       <c r="G19" s="11">
         <f t="shared" si="2"/>
-        <v>172165782</v>
+        <v>174579321</v>
       </c>
       <c r="U19" s="25"/>
       <c r="V19" s="26"/>
@@ -27915,7 +27923,7 @@
       </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="1"/>
@@ -27923,7 +27931,7 @@
       </c>
       <c r="G20" s="11">
         <f t="shared" si="2"/>
-        <v>639000000</v>
+        <v>648000000</v>
       </c>
       <c r="U20" s="25"/>
       <c r="V20" s="26"/>
@@ -27948,7 +27956,7 @@
       </c>
       <c r="E21" s="11">
         <f>D21+E22</f>
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="1"/>
@@ -27956,7 +27964,7 @@
       </c>
       <c r="G21" s="11">
         <f t="shared" si="2"/>
-        <v>103500000</v>
+        <v>105000000</v>
       </c>
       <c r="U21" s="25"/>
       <c r="V21" s="26"/>
@@ -27981,7 +27989,7 @@
       </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" si="1"/>
@@ -27989,7 +27997,7 @@
       </c>
       <c r="G22" s="11">
         <f t="shared" si="2"/>
-        <v>-582000000</v>
+        <v>-591000000</v>
       </c>
       <c r="U22" s="25"/>
       <c r="V22" s="26"/>
@@ -28014,7 +28022,7 @@
       </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="1"/>
@@ -28022,7 +28030,7 @@
       </c>
       <c r="G23" s="11">
         <f t="shared" si="2"/>
-        <v>555000000</v>
+        <v>564000000</v>
       </c>
       <c r="U23" s="25"/>
       <c r="V23" s="26"/>
@@ -28047,7 +28055,7 @@
       </c>
       <c r="E24" s="11">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="1"/>
@@ -28055,7 +28063,7 @@
       </c>
       <c r="G24" s="11">
         <f>B24*(E24-F24)</f>
-        <v>116705955</v>
+        <v>118598484</v>
       </c>
       <c r="U24" s="25"/>
       <c r="V24" s="25"/>
@@ -28080,7 +28088,7 @@
       </c>
       <c r="E25" s="11">
         <f t="shared" si="0"/>
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" si="1"/>
@@ -28088,7 +28096,7 @@
       </c>
       <c r="G25" s="11">
         <f t="shared" ref="G25:G30" si="3">B25*(E25-F25)</f>
-        <v>-588965600</v>
+        <v>-598568300</v>
       </c>
       <c r="U25" s="25"/>
       <c r="V25" s="25"/>
@@ -28113,7 +28121,7 @@
       </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" si="1"/>
@@ -28121,7 +28129,7 @@
       </c>
       <c r="G26" s="11">
         <f t="shared" si="3"/>
-        <v>-546163800</v>
+        <v>-555166500</v>
       </c>
       <c r="U26" s="25"/>
       <c r="V26" s="25"/>
@@ -28146,7 +28154,7 @@
       </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="1"/>
@@ -28154,7 +28162,7 @@
       </c>
       <c r="G27" s="11">
         <f t="shared" si="3"/>
-        <v>179000000</v>
+        <v>182000000</v>
       </c>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
@@ -28179,7 +28187,7 @@
       </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" si="1"/>
@@ -28187,7 +28195,7 @@
       </c>
       <c r="G28" s="11">
         <f t="shared" si="3"/>
-        <v>1074000000</v>
+        <v>1092000000</v>
       </c>
       <c r="U28" s="25"/>
       <c r="V28" s="25"/>
@@ -28212,7 +28220,7 @@
       </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="1"/>
@@ -28220,7 +28228,7 @@
       </c>
       <c r="G29" s="11">
         <f t="shared" si="3"/>
-        <v>1038200000</v>
+        <v>1055600000</v>
       </c>
       <c r="U29" s="25"/>
       <c r="V29" s="28"/>
@@ -28245,7 +28253,7 @@
       </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="1"/>
@@ -28253,7 +28261,7 @@
       </c>
       <c r="G30" s="11">
         <f t="shared" si="3"/>
-        <v>-900000</v>
+        <v>-915000</v>
       </c>
       <c r="U30" s="25"/>
       <c r="V30" s="25"/>
@@ -28278,7 +28286,7 @@
       </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="1"/>
@@ -28286,7 +28294,7 @@
       </c>
       <c r="G31" s="11">
         <f>B31*(E31-F31)</f>
-        <v>-4654000000</v>
+        <v>-4732000000</v>
       </c>
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
@@ -28311,7 +28319,7 @@
       </c>
       <c r="E32" s="11">
         <f t="shared" si="0"/>
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" si="1"/>
@@ -28319,7 +28327,7 @@
       </c>
       <c r="G32" s="11">
         <f>B32*(E32-F32)</f>
-        <v>-4637400000</v>
+        <v>-4716000000</v>
       </c>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
@@ -28344,7 +28352,7 @@
       </c>
       <c r="E33" s="11">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" si="1"/>
@@ -28352,7 +28360,7 @@
       </c>
       <c r="G33" s="11">
         <f>B33*(E33-F33)</f>
-        <v>51339785</v>
+        <v>52320800</v>
       </c>
       <c r="U33" s="25"/>
       <c r="V33" s="25"/>
@@ -28377,7 +28385,7 @@
       </c>
       <c r="E34" s="11">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" si="1"/>
@@ -28385,7 +28393,7 @@
       </c>
       <c r="G34" s="11">
         <f t="shared" ref="G34:G89" si="4">B34*(E34-F34)</f>
-        <v>3947600000</v>
+        <v>4032800000</v>
       </c>
       <c r="V34" s="25"/>
       <c r="W34" s="26"/>
@@ -28406,7 +28414,7 @@
       </c>
       <c r="E35" s="11">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" si="1"/>
@@ -28414,7 +28422,7 @@
       </c>
       <c r="G35" s="12">
         <f t="shared" si="4"/>
-        <v>1529000000</v>
+        <v>1562000000</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -28432,7 +28440,7 @@
       </c>
       <c r="E36" s="11">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" si="1"/>
@@ -28440,7 +28448,7 @@
       </c>
       <c r="G36" s="11">
         <f t="shared" si="4"/>
-        <v>51918924</v>
+        <v>53175027</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -28458,7 +28466,7 @@
       </c>
       <c r="E37" s="11">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F37" s="11">
         <f t="shared" si="1"/>
@@ -28466,7 +28474,7 @@
       </c>
       <c r="G37" s="11">
         <f t="shared" si="4"/>
-        <v>-112500</v>
+        <v>-115200</v>
       </c>
       <c r="J37" s="62"/>
     </row>
@@ -28485,7 +28493,7 @@
       </c>
       <c r="E38" s="11">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F38" s="11">
         <f t="shared" si="1"/>
@@ -28493,7 +28501,7 @@
       </c>
       <c r="G38" s="12">
         <f t="shared" si="4"/>
-        <v>246000000</v>
+        <v>252000000</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -28513,7 +28521,7 @@
       </c>
       <c r="E39" s="11">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F39" s="11">
         <f>IF(B39&gt;0,1,0)</f>
@@ -28521,7 +28529,7 @@
       </c>
       <c r="G39" s="11">
         <f t="shared" si="4"/>
-        <v>246000000</v>
+        <v>252000000</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -28539,7 +28547,7 @@
       </c>
       <c r="E40" s="11">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F40" s="11">
         <f>IF(B40&gt;0,1,0)</f>
@@ -28547,7 +28555,7 @@
       </c>
       <c r="G40" s="11">
         <f t="shared" si="4"/>
-        <v>-22000000</v>
+        <v>-22600000</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -28565,7 +28573,7 @@
       </c>
       <c r="E41" s="11">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F41" s="11">
         <f>IF(B41&gt;0,1,0)</f>
@@ -28573,7 +28581,7 @@
       </c>
       <c r="G41" s="11">
         <f t="shared" si="4"/>
-        <v>-68200000</v>
+        <v>-70060000</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -28591,7 +28599,7 @@
       </c>
       <c r="E42" s="11">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" ref="F42:F89" si="5">IF(B42&gt;0,1,0)</f>
@@ -28599,7 +28607,7 @@
       </c>
       <c r="G42" s="11">
         <f t="shared" si="4"/>
-        <v>-13200000</v>
+        <v>-13560000</v>
       </c>
       <c r="J42" s="7"/>
     </row>
@@ -28618,7 +28626,7 @@
       </c>
       <c r="E43" s="11">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="5"/>
@@ -28626,7 +28634,7 @@
       </c>
       <c r="G43" s="11">
         <f t="shared" si="4"/>
-        <v>69550000</v>
+        <v>71500000</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -28644,7 +28652,7 @@
       </c>
       <c r="E44" s="11">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F44" s="11">
         <f t="shared" si="5"/>
@@ -28652,7 +28660,7 @@
       </c>
       <c r="G44" s="11">
         <f t="shared" si="4"/>
-        <v>-540000</v>
+        <v>-555000</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -28670,7 +28678,7 @@
       </c>
       <c r="E45" s="11">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F45" s="11">
         <f t="shared" si="5"/>
@@ -28678,7 +28686,7 @@
       </c>
       <c r="G45" s="11">
         <f t="shared" si="4"/>
-        <v>3103000000</v>
+        <v>3190000000</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -28696,7 +28704,7 @@
       </c>
       <c r="E46" s="11">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F46" s="11">
         <f t="shared" si="5"/>
@@ -28704,7 +28712,7 @@
       </c>
       <c r="G46" s="11">
         <f t="shared" si="4"/>
-        <v>-20800000</v>
+        <v>-21400000</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -28722,7 +28730,7 @@
       </c>
       <c r="E47" s="11">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F47" s="11">
         <f t="shared" si="5"/>
@@ -28730,7 +28738,7 @@
       </c>
       <c r="G47" s="11">
         <f t="shared" si="4"/>
-        <v>-20200000</v>
+        <v>-20800000</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -28748,7 +28756,7 @@
       </c>
       <c r="E48" s="11">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="5"/>
@@ -28756,7 +28764,7 @@
       </c>
       <c r="G48" s="11">
         <f t="shared" si="4"/>
-        <v>-20000000</v>
+        <v>-20600000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -28774,7 +28782,7 @@
       </c>
       <c r="E49" s="11">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F49" s="11">
         <f t="shared" si="5"/>
@@ -28782,7 +28790,7 @@
       </c>
       <c r="G49" s="11">
         <f t="shared" si="4"/>
-        <v>282000000</v>
+        <v>291000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -28800,7 +28808,7 @@
       </c>
       <c r="E50" s="11">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" si="5"/>
@@ -28808,7 +28816,7 @@
       </c>
       <c r="G50" s="12">
         <f t="shared" si="4"/>
-        <v>282000000</v>
+        <v>291000000</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -28826,7 +28834,7 @@
       </c>
       <c r="E51" s="11">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" si="5"/>
@@ -28834,7 +28842,7 @@
       </c>
       <c r="G51" s="11">
         <f t="shared" si="4"/>
-        <v>71219121</v>
+        <v>73516512</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -28852,7 +28860,7 @@
       </c>
       <c r="E52" s="11">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" si="5"/>
@@ -28860,7 +28868,7 @@
       </c>
       <c r="G52" s="11">
         <f t="shared" si="4"/>
-        <v>-18800000</v>
+        <v>-19400000</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -28878,7 +28886,7 @@
       </c>
       <c r="E53" s="11">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F53" s="11">
         <f t="shared" si="5"/>
@@ -28886,7 +28894,7 @@
       </c>
       <c r="G53" s="11">
         <f t="shared" si="4"/>
-        <v>-34843500</v>
+        <v>-36045000</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -28904,7 +28912,7 @@
       </c>
       <c r="E54" s="11">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F54" s="11">
         <f t="shared" si="5"/>
@@ -28912,7 +28920,7 @@
       </c>
       <c r="G54" s="11">
         <f t="shared" si="4"/>
-        <v>-78030888</v>
+        <v>-81032076</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -28930,7 +28938,7 @@
       </c>
       <c r="E55" s="11">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F55" s="11">
         <f t="shared" si="5"/>
@@ -28938,7 +28946,7 @@
       </c>
       <c r="G55" s="11">
         <f t="shared" si="4"/>
-        <v>-2880000000</v>
+        <v>-3000000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -28956,7 +28964,7 @@
       </c>
       <c r="E56" s="11">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F56" s="11">
         <f t="shared" si="5"/>
@@ -28964,7 +28972,7 @@
       </c>
       <c r="G56" s="11">
         <f t="shared" si="4"/>
-        <v>53670424</v>
+        <v>56267380</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -28982,7 +28990,7 @@
       </c>
       <c r="E57" s="11">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F57" s="11">
         <f t="shared" si="5"/>
@@ -28990,7 +28998,7 @@
       </c>
       <c r="G57" s="11">
         <f t="shared" si="4"/>
-        <v>-1807200000</v>
+        <v>-1957800000</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -29008,7 +29016,7 @@
       </c>
       <c r="E58" s="11">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F58" s="11">
         <f t="shared" si="5"/>
@@ -29016,7 +29024,7 @@
       </c>
       <c r="G58" s="11">
         <f t="shared" si="4"/>
-        <v>-427017500</v>
+        <v>-463619000</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -29034,7 +29042,7 @@
       </c>
       <c r="E59" s="11">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F59" s="11">
         <f t="shared" si="5"/>
@@ -29042,7 +29050,7 @@
       </c>
       <c r="G59" s="11">
         <f t="shared" si="4"/>
-        <v>16582086</v>
+        <v>18186804</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -29060,7 +29068,7 @@
       </c>
       <c r="E60" s="11">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F60" s="11">
         <f t="shared" si="5"/>
@@ -29068,7 +29076,7 @@
       </c>
       <c r="G60" s="11">
         <f t="shared" si="4"/>
-        <v>-10478000</v>
+        <v>-11492000</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -29086,7 +29094,7 @@
       </c>
       <c r="E61" s="11">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F61" s="11">
         <f t="shared" si="5"/>
@@ -29094,7 +29102,7 @@
       </c>
       <c r="G61" s="11">
         <f t="shared" si="4"/>
-        <v>-4350000</v>
+        <v>-4800000</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -29112,7 +29120,7 @@
       </c>
       <c r="E62" s="11">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F62" s="11">
         <f t="shared" si="5"/>
@@ -29120,7 +29128,7 @@
       </c>
       <c r="G62" s="11">
         <f t="shared" si="4"/>
-        <v>-2500000</v>
+        <v>-2800000</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -29138,7 +29146,7 @@
       </c>
       <c r="E63" s="11">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F63" s="11">
         <f t="shared" si="5"/>
@@ -29146,7 +29154,7 @@
       </c>
       <c r="G63" s="11">
         <f t="shared" si="4"/>
-        <v>-4200000</v>
+        <v>-4800000</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -29164,7 +29172,7 @@
       </c>
       <c r="E64" s="11">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F64" s="11">
         <f t="shared" si="5"/>
@@ -29172,7 +29180,7 @@
       </c>
       <c r="G64" s="11">
         <f t="shared" si="4"/>
-        <v>-1827000</v>
+        <v>-2088000</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -29190,7 +29198,7 @@
       </c>
       <c r="E65" s="11">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F65" s="11">
         <f t="shared" si="5"/>
@@ -29198,7 +29206,7 @@
       </c>
       <c r="G65" s="11">
         <f t="shared" si="4"/>
-        <v>-466990</v>
+        <v>-549400</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -29216,7 +29224,7 @@
       </c>
       <c r="E66" s="11">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F66" s="11">
         <f t="shared" si="5"/>
@@ -29224,7 +29232,7 @@
       </c>
       <c r="G66" s="11">
         <f t="shared" si="4"/>
-        <v>-5344000</v>
+        <v>-6346000</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -29242,7 +29250,7 @@
       </c>
       <c r="E67" s="11">
         <f t="shared" ref="E67:E89" si="6">D67+E68</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F67" s="11">
         <f t="shared" si="5"/>
@@ -29250,7 +29258,7 @@
       </c>
       <c r="G67" s="11">
         <f t="shared" si="4"/>
-        <v>-220000</v>
+        <v>-280000</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -29268,7 +29276,7 @@
       </c>
       <c r="E68" s="11">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F68" s="11">
         <f t="shared" si="5"/>
@@ -29276,7 +29284,7 @@
       </c>
       <c r="G68" s="11">
         <f t="shared" si="4"/>
-        <v>-3005000</v>
+        <v>-3906500</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -29294,7 +29302,7 @@
       </c>
       <c r="E69" s="11">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F69" s="11">
         <f t="shared" si="5"/>
@@ -29302,7 +29310,7 @@
       </c>
       <c r="G69" s="11">
         <f t="shared" si="4"/>
-        <v>-1000000</v>
+        <v>-1300000</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -29320,7 +29328,7 @@
       </c>
       <c r="E70" s="11">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F70" s="11">
         <f t="shared" si="5"/>
@@ -29328,7 +29336,7 @@
       </c>
       <c r="G70" s="11">
         <f t="shared" si="4"/>
-        <v>-1000000</v>
+        <v>-1600000</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -29346,7 +29354,7 @@
       </c>
       <c r="E71" s="11">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F71" s="11">
         <f t="shared" si="5"/>
@@ -29354,7 +29362,7 @@
       </c>
       <c r="G71" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>46167</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -29372,7 +29380,7 @@
       </c>
       <c r="E72" s="11">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F72" s="11">
         <f t="shared" si="5"/>
@@ -29380,7 +29388,7 @@
       </c>
       <c r="G72" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -29398,7 +29406,7 @@
       </c>
       <c r="E73" s="11">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F73" s="11">
         <f t="shared" si="5"/>
@@ -29406,7 +29414,7 @@
       </c>
       <c r="G73" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7800000</v>
       </c>
       <c r="J73" t="s">
         <v>25</v>
@@ -29423,11 +29431,11 @@
         <v>726</v>
       </c>
       <c r="D74" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E74" s="11">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F74" s="11">
         <f t="shared" si="5"/>
@@ -29435,17 +29443,25 @@
       </c>
       <c r="G74" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
+      <c r="A75" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="B75" s="39">
+        <v>-200000</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="11">
+        <v>1</v>
+      </c>
       <c r="E75" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="11">
         <f t="shared" si="5"/>
@@ -29453,7 +29469,7 @@
       </c>
       <c r="G75" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-200000</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -29723,7 +29739,7 @@
       <c r="A90" s="11"/>
       <c r="B90" s="29">
         <f>SUM(B2:B89)</f>
-        <v>10441166</v>
+        <v>10241166</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -29731,7 +29747,7 @@
       <c r="F90" s="11"/>
       <c r="G90" s="29">
         <f>SUM(G2:G89)</f>
-        <v>14446390929</v>
+        <v>14477514427</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -29765,7 +29781,7 @@
       <c r="F93" s="11"/>
       <c r="G93" s="3">
         <f>G90/E2</f>
-        <v>54106333.067415729</v>
+        <v>53620423.803703703</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -33780,8 +33796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34070,11 +34086,11 @@
       </c>
       <c r="F8" s="71">
         <f>K23</f>
-        <v>172619738.32876712</v>
+        <v>172419738.32876712</v>
       </c>
       <c r="G8" s="29">
         <f t="shared" si="0"/>
-        <v>11162191.788645893</v>
+        <v>11362191.788645893</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>25</v>
@@ -34233,14 +34249,14 @@
       </c>
       <c r="K12" s="44">
         <f>'مسکن مریم یاران'!B90</f>
-        <v>10441166</v>
+        <v>10241166</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="5"/>
-        <v>10441166</v>
+        <v>10241166</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -34354,11 +34370,11 @@
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>-6650000</v>
+        <v>-6850000</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="5"/>
-        <v>6650000</v>
+        <v>6850000</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="11"/>
@@ -34755,11 +34771,11 @@
       </c>
       <c r="K23" s="3">
         <f>SUM(K7:K22)</f>
-        <v>172619738.32876712</v>
+        <v>172419738.32876712</v>
       </c>
       <c r="L23" s="3">
         <f>SUM(L7:L22)</f>
-        <v>59777144.219178081</v>
+        <v>59577144.219178081</v>
       </c>
       <c r="M23" s="3">
         <f>SUM(M7:M22)</f>
@@ -34807,7 +34823,7 @@
       </c>
       <c r="K24" s="3">
         <f>K9+K11+K12+K13+K10+K16+K17</f>
-        <v>98687026</v>
+        <v>98487026</v>
       </c>
       <c r="L24" s="3">
         <f>L9+L16+L12+L10</f>
@@ -34815,7 +34831,7 @@
       </c>
       <c r="M24" s="3">
         <f>M11+M12+M13+M17+M9</f>
-        <v>81881690</v>
+        <v>81681690</v>
       </c>
       <c r="N24" s="25"/>
       <c r="O24" s="11"/>

</xml_diff>